<commit_message>
Add flaschards for chapter 11
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
+++ b/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>Question</t>
   </si>
@@ -19,16 +19,244 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;Welches weitere Gesetz definiert Unternehmensformen die für die Auslegung des KSchG relevant sind?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;UGB 2007&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Schutznormen des KSchG?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/3" rel="noopener noreferrer" target="_blank"&gt;§ 3-6 KSchG&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/fagg/paragraf/11" rel="noopener noreferrer" target="_blank"&gt;§§ 11ff FAGG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Verbraucher kann von einem sog. Haustürgeschäft zurücktreten (grundlos innerhalb bestimmter Fristen) &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; (§ 3 KSchG)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;besonderes Rücktrittsrecht  &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(§ 3 KSchG, §§ 11ff FAGG)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Kostenvoranschlag gegenüber Verbraucher gilt als Garantie &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; (§ 5 KSchG)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Bestimmte Klauseln im AGB sind Unwirksam (§ 6 KSchG)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Verbrauchergeschäfte? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/1" rel="noopener noreferrer" target="_blank"&gt;§ 1 &lt;/a&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/1" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;KSchG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;: &lt;/span&gt;Wenn an einem zweiseitigen RG einerseits ein Unternehmer, für den das RG zum Betrieb seines Unternehmens gehört, und andererseits ein Verbraucher, auf den das nicht zutrifft, beteiligt -&amp;gt; Anwendung des KSchG &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Prinzip der kausalen Tradition (Lehre von Titel und Modus)? Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/380" rel="noopener noreferrer" target="_blank"&gt;§ 380 ABGB&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/424" rel="noopener noreferrer" target="_blank" style="color: rgb(115, 133, 197); background-color: rgb(40, 45, 88);"&gt;§§ 424ff ABGB&lt;/a&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;, &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/1053" rel="noopener noreferrer" target="_blank" style="color: rgb(115, 133, 197); background-color: rgb(40, 45, 88);"&gt;§ 1053 ABGB&lt;/a&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;, &lt;/span&gt;&lt;/p&gt;&lt;p&gt;Zum Erwerb des Eigentrumsrechts muss zum gültigen Verpflichtungsgeschäft (&lt;strong&gt;Titel&lt;/strong&gt;) auch ein Verfügungsgeschäft (&lt;strong&gt;Modus&lt;/strong&gt;) hinzutreten.&lt;/p&gt;&lt;p&gt;-&amp;gt; &lt;strong&gt;Man wird nicht bereits mit Abschluss des Kaufvertrages Eigentümer.&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Abstrakte/Kausale Rechtsgeschäfte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;abstrakt&lt;/strong&gt;: Wenn sich der Zweck (Rechtsgrund, causa) einer Verpflichtungserklärung nicht entnehmen lässt, sind idR ungültig.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;kausal&lt;/strong&gt;: wenn sich aus ihnen der Rechtsgrund entnehmen lässt&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Verpflichtungs- und Verfügungsgeschäfte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Verpflichtung&lt;/strong&gt;: geben dem Gläubiger einen schuldrechtlichen Anspruch (Forderung) auf Lieferung der Sache, aber noch kein dingliches (Eigentums-)Recht an der Sache. z.B: Käufer wird erst Eigentümer, wenn die Sache durch &lt;strong&gt;Verfügungsgeschäft &lt;/strong&gt;vom Verkäufer übergeben wird.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verfügung&lt;/strong&gt;: Führt die Verschiebung des (sachenrechtlichen) Eigentumsrecht von Verkäufer an Käufer herbei. &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Ziel- und Dauerschuldverhältnisse?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ziel&lt;/strong&gt;: Ansprüche erlöschen durch die intendierte einmalige Leistungserbringung (Kaufvertrag: Lieferung + Bezahlung)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Dauer&lt;/strong&gt;: Wiederkehrende Leistungserbringung ohne Erlöschen&lt;strong&gt; &lt;/strong&gt;der Ansprüche ist vorgesehen (Strom, Zeitungsabo, unbefristeter Mietvertrag)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Konsensualverträge/Realverträge?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Konsensual&lt;/strong&gt;: Kommen durch bloße Einigung zustande  (Kaufvertrag, Mietvertrag, ...)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Real&lt;/strong&gt;: Erfordert zum Abschluss auch Sachübergabe (Darlehensvertrag, Leihvertrag und Verwahrungsvertrag)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Entgeltliche/Unentgeltliche/Entgeltfremde Rechtesgeschäfte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;entgeltlich&lt;/strong&gt;: immer Zweiseitig, jede Partei bringt die eigene Leistung um die Gegenleistung zu erhalten (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/917" rel="noopener noreferrer" target="_blank"&gt;§ 917 ABGB&lt;/a&gt;). Leistung muss nicht Geld sein.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;unentgeltlich&lt;/strong&gt;: Ein Partner erhält keine Gegenleistung (Schenkungsvertrag)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;entgeltsfremd&lt;/strong&gt;: liegen vor, wenn ein Bürge nachträglich einem existierenden Darlehensvertrag beitritt, ohne dass sich die Konditionen für den Hauptschuldner ändern.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie nennt man entgeltliche Rechtsgeschäfte noch? Was ist die Bedeutung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Synallagmatische Verträge&lt;/li&gt;&lt;li&gt;Erbringt ein Teil seine Leistung nicht, muss auch der andere seine nicht erbringen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Rechtsgeschäfte unter Lebenden, und von Todes wegen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Lebenden&lt;/strong&gt;: Wirkung tritt zu Lebzeiten der Partner ein (Kaufvertrag, Mietvertrag, .. )&lt;/li&gt;&lt;li&gt;&lt;strong&gt;von Todes wegen&lt;/strong&gt;: Tritt nach dem Tod mindest einer Partei ein (Erbvertrag, Testament, ... )&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind empfangsbedürftige und nicht empfangsbedürftige Rechtesgeschäfte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Testament nicht empfangsbedürftig&lt;/li&gt;&lt;li&gt;Kündigung, Angebotserklärung/Annahme, etc sind Empfangsbedürftig -&amp;gt; Empfangstheorie&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Einseitig/Zweiseitig verpflichtende Rechtsgeschäfte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Einseitig&lt;/strong&gt;: Nur ein Partner zur Leistung verpflichtet (Schenkung)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Zweiseitig &lt;/strong&gt;(ABGB nennt diese&lt;strong&gt; Gegenseitige Verträge&lt;/strong&gt;): Beide Seiten verpflichtet (Kaufvertrag, ... )&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Ein-, Zwei- und mehrseitige Rechtsgeschäfte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Differenzierung anhand der Anzahl der erforderlichen Willenserkärungen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ein&lt;/strong&gt;: Testament, Auslobung, Kündigung, ...&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Zwei&lt;/strong&gt;: Kaufvertrag, ...&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Mehr&lt;/strong&gt;: Gesellschaftsvertrag&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Rechtsgeschäft im juristischen Sinn?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ein Tatbestand, der aus einer oder mehreren Willensäußerungen von Rechtssubjekten besteht, an welche die Privatrechtsordnung den Eintritt von Rechtsfolgen knüpft.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann begrenzen Drittwirkungen der Grundrechte die Privatautonomie?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Keine unmittelbare Drittwirkung der Grundrechte, aber:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Interpretation von Generalklauseln (z.B. Sittenwidrigkeit) können in die Interpretation privatrechtlicher Normen einfließen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Fiskalgeltung der Grundrechte: Gebietskörperschaften sind an die Grundrechte gebunden, auch wenn sie privatrechtlich Handeln. &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Kontrahierungszwang? Wodurch kann er entstehen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Zwang zum Vertragsabschluss&lt;/li&gt;&lt;li&gt;Entsteht durch:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gesetzliche Anordnung (z.B.: bei Monopol, Gefährdung der Nahversorgung)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Auch ohne ausdrückliche Gesetzliche Vorschrift bei faktischer Monopolstellung eines Vertragspartners (Nichtabschluss würde sonst rechtswidriges/sittenwidriges Verhalten darstellen)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche drei Arten der Grenzen der Privatautonomie gibt es?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gesetzliche Vorschriften / zwingendes Recht&lt;/li&gt;&lt;li&gt;Begrenzung der Abschlussfreiheit durch Kontrahierungszwang&lt;/li&gt;&lt;li&gt;Drittwirkung der Grundrechte&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die 7 Inhalte der Privatautonomie?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Abschlussfreiheit (ob, wann und mit wem Vertrag geschlossen wird)&lt;/li&gt;&lt;li&gt;Inhaltsfreiheit&lt;/li&gt;&lt;li&gt;Typenfreiheit (neue Vertragstypen zu schaffen)&lt;/li&gt;&lt;li&gt;Beendigungsfreiheit&lt;/li&gt;&lt;li&gt;Änderungsfreiheit&lt;/li&gt;&lt;li&gt;Formfreiheit&lt;/li&gt;&lt;li&gt;Testierfreiheit (ob und wie der Verstorbene letztwillig testiert)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtsfähigkeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;gibt jedem Rechtssubjekt die Macht, seine Belange (seine eigene Rechtssphäre) nach freiem Belieben zu regeln, Rechte zu erwerben, zu ändern oder aufzugeben&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Rechtsgeschäft?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Rechtsgeschäfte sind (private) Willenserklärungen von Rechtssubjekten, die rechtlich durchsetzbar und von einem Rechtsfolgewillen getragen sind.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Privatautonomie?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;ermöglicht jedem Rechtssubjekt durch freie eigene willentliche Entscheidung seine Rechtsverhältnisse (Berechtigung und Verpflichtung) eigenverantwortlich nach Belieben innerhalb der gesetzlichen Schranken zu gestalten&lt;/li&gt;&lt;li&gt;Genießt Verfassungsrang&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Willenserklärung?&lt;/p&gt;&lt;p&gt;Woraus besteht eine Willenserklärung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Grundbestandteil jedes Rechtsgeschäfts&lt;/li&gt;&lt;li&gt;Willensäußerung und Handlung, Rechtsfolgewille, Kundgabezweck&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(226, 148, 20);"&gt;Strenge Rechtsfolgentheorie zu Rechtsfolgewille&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Es ist nicht erforderlich, dass der Erklärende einen genauen Überblick über alle konkreten Rechtsfolgen hat.&amp;nbsp;&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(226, 148, 20);"&gt;Geschäftswille als Rechtsfolgewille&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Es reicht aus, wenn der Handelnde den Willen hat, ein rechtlich verbindliches Geschäft zu schließen.&amp;nbsp;&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was bedeutet "Kein Widerruf durch den Erklärenden" bzw. das Bindungsproblem? Was sind die Voraussetzungen und deren Rechtliche Grundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Vor dem Zugang ist die Erklärung noch nicht wirksam und kann daher vom Erklärenden noch widerrufen werden, es liegt hier noch keine Bindungswirkung vor.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Voraussetzung für einen gültigen Widerruf ist nur, dass der Widerruf vor oder spätestens gleichzeitig mit der zu widerrufenden Erklärung zugeht (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/862a" rel="noopener noreferrer" target="_blank"&gt;§ 862a ABGB&lt;/a&gt;).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Willenserklärung: &lt;/span&gt;Rechtsfolgewille - Geltungswille&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Der Handelnde ist an seiner Erklärung gebunden, wenn er in dem Bewusstsein handelt, rechtliche verbindliche Handlungen zu setzen, die erforderlichenfalls mit staatlichen Zwang durchsetzbar sind (gemäßigte Rechtsfolgentheorie).&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Bindungswille des Erklärenden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der Willenserklärung muss ein &lt;strong&gt;Bindungswille des Antragstellers&lt;/strong&gt; entnehmbar sein. Bindungswille liegt vor, wenn aus der Erklärung hervorgeht, dass der Erklärende dem Adressaten das Recht einräumen will, durch einfaches „Ja“ bzw. einseitige Annahme den Vertrag zustande zu bringen (Gestaltungsrecht).&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Kein Bindungswille: z. B. Kataloge, Muster,…&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Erklärungsboten?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Alle die nicht Empfangsboten sind. Sie können die Erkärung nur weitergeben, nicht empfangen. Die Erklärung ist dem Empfänger nur dann zugegangen, wenn sie wirklich in dessen Machtbereich gelangt.&lt;/p&gt;&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;z.B.: Post, Kinder; &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Willenserklärung: Kundgabezweck&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Das Rechtssubjekt muss die Handlung nach „außen kundtun“, dem Erklärungsempfänger zur Kenntnis bringen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Willenserklärung: Willensäußerung und Handlung&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der Handlungswille des Rechtssubjektes ist unabdingbarer Bestandteil für das Vorliegen einer Willenserklärung. Das Verhalten soll willentlich, also vom eigenen Willen gesteuert, sein.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Bestimmtheit der Willenserklärung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/869" rel="noopener noreferrer" target="_blank"&gt;§ 869 ABGB&lt;/a&gt;&lt;/p&gt;&lt;p&gt;Das Angebot muss i&lt;strong&gt;nhaltlich ausreichend bestimmt&lt;/strong&gt; sein, d.h. die wesentlichen Punkte (&lt;strong&gt;Ware und Preis müssen bestimmt oder bestimmbar sein&lt;/strong&gt;) des abzuschließenden Vertrages müssen, jedenfalls der Mindestinhalt (&lt;strong&gt;essentialia negotii&lt;/strong&gt;) muss bestimmt sein.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Empfangstheorie?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Es kommt nicht auf den Zeitpunkt der internen Erklärungsbindung (A denkt sich, er schreibt B) an, auch nicht auf den Zeitpunkt der Äußerung der Erklärung (A schreibt den Brief), und auch nicht auf die Absendung der Erklärung, sondern den Eintritt der Erklärung in die Machtsphäre des Empfängers!&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Empfangsboten?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;werden nach der Verkehrsauffassung vom Empfänger als zur Entgegennahme, von Schriftstücken bestellt anzusehen.&lt;/p&gt;&lt;p&gt;z. B.: Ehegatte, Sekretärin im Büro;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Zugang der Willenserklärung beim Erklärungsempfänger? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Erst mit dem Zugang an den Oblaten (= Erklärungsempfänger) wird das Angebot wirksam. Davor existiert das Angebot zwar, ist aber nicht wirksam, ohne rechtliche Relevanz. &lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Hier ist die Empfangstheorie zu beachten. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die 5 Voraussetzungen für ein Angebot?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;Willenserklärung (Willensäußerung oder –handlung, Rechtsfolgewille, Kundgabezweck)&lt;/li&gt;&lt;li&gt;Bestimmtheit der Willenserklärung&lt;/li&gt;&lt;li&gt;Bindungswille des Erklärenden&lt;/li&gt;&lt;li&gt;Zugang der Willenserklärung beim Erklärungsempfänger&lt;/li&gt;&lt;li&gt;Kein Widerruf durch den Erklärenden = Bindungsproblem&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Anspruch?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ein&amp;nbsp;Anspruch&amp;nbsp;berechtigt&amp;nbsp;eine&amp;nbsp;Person&amp;nbsp;(Berechtigter&amp;nbsp;oder&amp;nbsp;Gläubiger)&amp;nbsp;dazu,&amp;nbsp;von&amp;nbsp;einer&amp;nbsp;anderen&amp;nbsp;Person&amp;nbsp;(Verpflichteten&amp;nbsp;oder&amp;nbsp;Schuldner)&amp;nbsp;ein&amp;nbsp;aktives&amp;nbsp;Tun&amp;nbsp;oder&amp;nbsp;passives&amp;nbsp;Unterlassen&amp;nbsp;fordern&amp;nbsp;zu&amp;nbsp;können.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die drei Abgrenzungstheorien?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;strong&gt;Interessentheorie &lt;/strong&gt;(Jurist Ulpian): öffentliches Recht dient den Interessen der Allgemeinheit, Privatrecht den Interessen des Einzelnen.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Subjektionstheorie&lt;/strong&gt;: Während beim Privatrecht einander gleichberechtigte Rechtssubjekte gegenüberstehen (&lt;a href="https://www.jusline.at/gesetz/jn/paragraf/1" rel="noopener noreferrer" target="_blank"&gt;§ 1 JN)&lt;/a&gt;, stehen einander im öffentlichen Recht der Rechtsunterworfene und der Hoheitsträger gegenüber.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Subjektstheorie&lt;/strong&gt;: Es handelt sich um öffentliches Recht, wenn zumindest ein Hoheitsträger am Rechtsverhältnis beteiligt ist, der in Ausübung der Hoheitsgewalt auftritt. Tritt kein Beteiligter mit Hoheitsgewalt auf, so liegt privatrechtliches Handeln vor.&amp;nbsp;&lt;/li&gt;&lt;/ol&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Bedeutung der Abgrenzung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/jn/paragraf/1" rel="noopener noreferrer" target="_blank"&gt;§ 1 JN&lt;/a&gt; und § &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/1" rel="noopener noreferrer" target="_blank"&gt;1 ABGB &lt;/a&gt;&lt;/p&gt;&lt;p&gt;Während das Privatrecht die Rechtsbeziehungen von gleichberechtigten Rechtssubjekten untereinander trägt (z. B. Mietrecht, Vertragsrecht, etc.), steht im öffentlichen Recht der Staat den rechtsunterworfenen Bürgern übergeordnet gegenüber und wird hoheitlich tätig (z. B. Baurecht, Steuerrecht, etc.).&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Was ist die Rechtsordnung? &lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;ist eine staatliche Zwangsordnung und besteht auf der Summe all jener Normen, deren Einhaltung mit staatlicher Zwangsgewalt durchgesetzt werden kann. Dem einzelnen Rechtssubjekt können (durchsetzbare) Rechte eingeräumt werden oder (durchsetzbare) Verhaltenspflichten auferlegt werden.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das Recht im objektiven Sinn?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Die Rechtsordnung soll das geordnete menschliche Zusammenleben gewährleisten. Rechtlich verbindliche Normen (Recht im objektiven Sinn) werden also charakterisiert durch die Möglichkeit der unmittelbaren und zwangsweisen Durchsetzung, wobei diese Entscheidung der Republik Österreich obliegt.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist Moral?&lt;/p&gt;&lt;p&gt;Was sind die Sanktionen bei Verletzung?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
@@ -436,7 +664,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B44"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -490,6 +718,310 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Add flashcards for chapter 12, 13 and 15
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
+++ b/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="230">
   <si>
     <t>Question</t>
   </si>
@@ -19,16 +19,478 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;Wie kann ein auslegungsbedürftiger Vertrag mit der &lt;strong&gt;einfachen Vertragsinpterpretation &lt;/strong&gt;ausgelegt werden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Unter Rückgriff auf:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;den &lt;strong&gt;subjektiven Willen der Parteien&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;den &lt;strong&gt;Objektiven Wortlaut der Erklärung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;sowie die &lt;strong&gt;Übung des redlichen Verkehrs&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Folge von &lt;strong&gt;verstecktem &lt;/strong&gt;Dissens über die Nebenpunkte?&lt;/p&gt;&lt;p&gt;Wie wird gegebenenfalls eine derart entstandene Lücke gefüllt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Es kommt drauf an, ob angenommen werden kann, dass der &lt;strong&gt;Vertrag auch ohne Einigung&lt;/strong&gt; über die &lt;strong&gt;offenen Nebepunkte geschlossen &lt;/strong&gt;worden wäre.&lt;/li&gt;&lt;li&gt;Dies ist idR der Fall, wenn die Nebenpunkte durch &lt;strong&gt;Gesetz oder Verkehrssitte&lt;/strong&gt; ergänzbar sind, und von den Parteien kein Vorbehalt diesbezüglich gemacht wurde.&lt;/li&gt;&lt;li&gt;Diese Lücke wird mittels &lt;strong&gt;dispositivem Recht&lt;/strong&gt; oder &lt;strong&gt;ergänzender Vertragsauslegung &lt;/strong&gt;gefüllt.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Zweifelsregel?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/915" rel="noopener noreferrer" target="_blank" style="background-color: yellow; color: black;"&gt;§ 915 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Bei entgeltlichen Rechtsgeschäften ist eine undeutliche Äußerung im Zweifel zum Nachteil desjenigen zu verstehen, der sich ihrer bedient hat.&lt;/li&gt;&lt;li&gt;Lässt sich kein eindeutiger Sinn ermitteln, so ist die Aussage wegen unbestimmtheit nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/869" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(115, 133, 197);"&gt;§ 869 ABGB&lt;/a&gt; ungütlig.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was wird höher gewertet, der &lt;strong&gt;erkennbare subjektive Wille&lt;/strong&gt; oder der &lt;strong&gt;objektive Wortlaut&lt;/strong&gt;, und &lt;strong&gt;warum&lt;/strong&gt;? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;Was sind die Folgen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/914" rel="noopener noreferrer" target="_blank" style="background-color: yellow; color: black;"&gt;§§ 914f ABGB&lt;/a&gt; iVm &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank"&gt;§ 863 ABGB&lt;/a&gt; &lt;/p&gt;&lt;ul&gt;&lt;li&gt;Der erkennbare Subjektive Wille: Es ist die erkennbare Absicht der Parteien zu erforschen, Der Erklärungsempfänger hat den im objektiven Erklärungswert zum Ausdruck kommenden &lt;strong&gt;wahren subjektiven Willen&lt;/strong&gt; zu ermitteln.&lt;/li&gt;&lt;li&gt;Folge: Bei Verträgen gilt primär der übereinstimmende wahre Wille der Parteien, selbst wenn der Wortlaut davon abweicht. &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der hypothetische Parteiwillen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Das, was die &lt;strong&gt;konkreten &lt;/strong&gt;Parteien &lt;strong&gt;vernünftigerweise&lt;/strong&gt; &lt;strong&gt;gewollt&lt;/strong&gt; &lt;strong&gt;hätten&lt;/strong&gt;, wenn ihnen die &lt;strong&gt;Unvollständigkeit &lt;/strong&gt;des &lt;strong&gt;Vertrages bewusst &lt;/strong&gt;gewesen wäre.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wie funktioniert die Lückenschließung durch &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;ergänzende Vertragsauslegung&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Verwendet:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;hypothetischen Parteiwillen&lt;/li&gt;&lt;li&gt;Übung des redlichen Verkehrs&lt;/li&gt;&lt;li&gt;Treu und Glauben&lt;/li&gt;&lt;li&gt;Verkehrsauffassung&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche 3 Quellen für Vertragsvereinbarungen gibt es?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;essentiala negotii&lt;/strong&gt; durch Parteeeinigung&lt;/li&gt;&lt;li&gt;&lt;strong&gt;naturalia negotii&lt;/strong&gt; fügt das Gesetz hinzu&lt;/li&gt;&lt;li&gt;&lt;strong&gt;accidentalia negotii&lt;/strong&gt; können die Parteien weiters vereinbaren&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie funktioniert die Lückenschließung durch &lt;strong&gt;dispositives Recht&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Lücken sind durch &lt;strong&gt;gesetzliche Vorschriften&lt;/strong&gt; zu ergänzen&lt;/p&gt;&lt;ul&gt;&lt;li class="ql-indent-1"&gt;Außer es steht fest, dass die Parteien die Geltung des dispositiven Rechts &lt;strong&gt;nicht herbeiführen&lt;/strong&gt; wollten und &lt;strong&gt;dennoch keine Regelung&lt;/strong&gt; getroffen haben&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Einfluss der &lt;strong&gt;Übung des redlichen Verkehrs&lt;/strong&gt; auf den objektiven Wortlaut?&lt;/p&gt;&lt;p&gt;Welche Elemente sind zu beachten?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ist die Erklärung nicht eindeutig, so ist sie vom Empfänger entsprechend der &lt;strong&gt;Verkehrssitte&lt;/strong&gt;, also der Übung des redlichen Verkehrs zu verstehen.&lt;/li&gt;&lt;li&gt;Beachten:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Sprachgebrauch&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Art&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ort (z.B.: ortstypischer Dialekt)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Umstände (Verkehrskreis, Verbraucher, Unternehmer, ... )&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Rechtsgrundlage für die Auslegungsregeln für Verträge?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="ql-align-justify"&gt;&lt;span style="color: black; background-color: yellow;"&gt;§§ &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank" style="color: black; background-color: yellow;"&gt;863 Abs 2&lt;/a&gt;&lt;span style="color: black; background-color: yellow;"&gt;, &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/914" rel="noopener noreferrer" target="_blank" style="color: black; background-color: yellow;"&gt;914&lt;/a&gt;&lt;span style="color: black; background-color: yellow;"&gt;, &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/915" rel="noopener noreferrer" target="_blank" style="color: black; background-color: yellow;"&gt;915&lt;/a&gt;&lt;span style="color: black; background-color: yellow;"&gt; ABGB&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/ugb/paragraf/346" rel="noopener noreferrer" target="_blank" style="color: black; background-color: yellow;"&gt;§ 346 UGB&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann darf eine zurechenbare Willenserklärung nicht angenommen werden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wenn für den Empfänger zwar ein Vertrauenstatbestand vorlag, aber der Empfänger auf diese Handlung &lt;strong&gt;nicht vertraut&lt;/strong&gt; hat.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist &lt;strong&gt;fehlende Erklärungsbewusstsein&lt;/strong&gt; des Erklärenden?&lt;/p&gt;&lt;p&gt;Wann sind Erklärungen dennoch Zurechenbar?&lt;/p&gt;&lt;p&gt;Was hätte der Erklärende in dem Fall verhindern müssen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Unbewusst abgegebene Erklärungen&lt;/li&gt;&lt;li&gt;Nur dann zurechenbar, wenn sich der Erklärende fahrlässig verhalten hat &lt;/li&gt;&lt;li&gt;Verhindern, dass diese Erklärungen/Handlungen vom &lt;strong&gt;gutgläubigen Dritten&lt;/strong&gt; als &lt;strong&gt;Willenserklärungen angesehen &lt;/strong&gt;werden &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(&lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(226, 148, 20);"&gt;Erklärungsfahrlässigkeit&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein objektiv-redlicher Erklärungsempfänger?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wer sich bemüht, richtig zu verstehen, was der Erklärende ausdrücken möchte&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Bedeutungen der &lt;strong&gt;Willenstheorie&lt;/strong&gt;, &lt;strong&gt;Erklärungstheorie &lt;/strong&gt;und &lt;strong&gt;Vertrauenstheorie&lt;/strong&gt;, was ist bei der Erklärung Maßgebend?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Willenstheorie&lt;/strong&gt;: Wille des Erklärenden&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erklärungstheorie&lt;/strong&gt;: objektiver Wortlaut der Erklärung&lt;/li&gt;&lt;li&gt;Maßgebend: &lt;strong&gt;Vertrauenstheorie &lt;/strong&gt;(Abgeleitet von &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank"&gt;§ 863 ABGB)&lt;/a&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Die Erklärung aus der Sicht eines &lt;strong&gt;objektiv-redlichen Erklärungsempfängers&lt;/strong&gt;, alle Kenntnisse des wirklichen Empfängers, auch ungewöhnliche, inklusive. &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Worum geht es bei der Interpretation von Erklärungen und Verträgen?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Um die Ermittlung des Inhalts einer einzelnen Vertragsabschlusserklärung&lt;/li&gt;&lt;li&gt;Um die Ermittlung des Vertragsinhalts&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Folge von Dissens über Hauptpunkte?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;Ist es relevant ob offener oder versteckter Dissens?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/869" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 869 S2 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Kein Vertrag kommt zustande.&lt;/li&gt;&lt;li&gt;Unabhängig ob offener oder versteckter Dissens&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche 3 Arten des Dissens gibt es?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/869" rel="noopener noreferrer" target="_blank"&gt;§ 869 S2 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Dissens wegen Unvollständigkeit der Vereinbarung:&lt;/strong&gt; z.B.: Haupt oder Nebenpunkte sind offen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Dissens wegen Diskrepanz der Erklärungen&lt;/strong&gt;: Angebot- und Annahmeerklärung stimmen im Wortlaut nicht überein, und können auch durch Auslegung nicht zur Deckung gebracht werden&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Dissens wegen Mehrdeutigkeit oder Unverständlichkeit der Erklärungen&lt;/strong&gt;: Angebot und Annahme stimmen zwar im Wortlaut überein, sind aber objektiv mehrdeutig und werden von den Parteien unterschiedlich verstanden.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist &lt;strong&gt;versteckter &lt;/strong&gt;Dissens?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Zumindest eine Partei glaubt, dass in allen Punkten einigung erzielt wurde&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist &lt;strong&gt;offener &lt;/strong&gt;Dissens?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Beide Parteien wissen, dass sie sich noch nicht einig sind&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was kann (offener und versteckter) Dissens betreffen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Haupt- oder Nebenpunkte im Vertrag&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Kann es Erklärungsirrtum bei natürlichem Konsens geben?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nein, der Vertragsinhalt besteht nur aus dem subjektiven Willen beider Parteien (es gibt keinen objektiven Erklärungswert der abweichen könnte)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was wird höher bewertet, übereinstimmender subjektiver Wille, oder übereinstimmender objektiver Erklärungswert?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der übereinstimmende Subjektive Wille, der objektive Erklärungswert kann nämliich irrtümlich vom subjektiven Willen des Anbieters abweichen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Abgrenzung zwischen Konsens, Dissens und Erklärungsirrtum?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Konsens&lt;/strong&gt;: subjektiver Wille (der Parteien) oder objektiver Erklärungswert (der Erkärungen) stimmt überein.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Dissens&lt;/strong&gt;: Weder subjektiver Wille noch objektiver Erklärungswert stimmen überein&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erklärungsirrtum&lt;/strong&gt;: Der subjektive Wille einer Partei weicht vom objektiven Erklärungswert ab.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der objektive Erklärungswert? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der in den Vertrag eingesetzte Wert (z.B.: Preis), kann &lt;strong&gt;irrtümlich&lt;/strong&gt; vom subjektiven Willen des Anbieters abweichen&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der normative Konsens?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der Erklärungsempfänger vertraut auf den &lt;strong&gt;objektiven Erklärungswert&lt;/strong&gt;, aber der Vertragsinhalt entspricht nicht dem subjektiven Willen der anderen Partei (-&amp;gt; &lt;strong&gt;Fehler bei Angebotslegung&lt;/strong&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der natürliche Konsens?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der innere Wille beider Parteien stimmt überein&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Inhaltskontrolle der AGB?&lt;/p&gt;&lt;p&gt;Was sind die drei Ebenen und deren Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Soll den Kunden vor überschießenden AGB Schützen -&amp;gt; die Unterlegenheit des Kunden ausgleichen. Diese zivilrechtliche Kontrolle wird durch eine vorhergehende aufsichtsbehördliche Genehmigung oder Kontrolle &lt;strong&gt;nicht &lt;/strong&gt;ausgeschlossen.&lt;/li&gt;&lt;li&gt;3 Ebenen:&lt;/li&gt;&lt;/ul&gt;&lt;ol&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Einbeziehungskontrolle&lt;/strong&gt;: Prüfung ob die AGB in ihrer Gesamtheit von den Parteien erhoben wurde (Parteieneinigung, z.B.: Unterschriften)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Geltungskontrolle&lt;/strong&gt;: Alle Einzelbestimmungen der AGB, die tatsächlich Vertragsinhalt geworden sind, werden der Geltungskontrolle unterzogen (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/864a" rel="noopener noreferrer" target="_blank"&gt;§ 864a ABGB&lt;/a&gt;). &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Inhaltskontrolle&lt;/strong&gt;: Verbleibende Klauseln (Kein Verstoß gegen &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/879" rel="noopener noreferrer" target="_blank"&gt;§ 879 Abs 3 &lt;/a&gt;und &lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/6" rel="noopener noreferrer" target="_blank"&gt;§ 6 KSchG&lt;/a&gt;)&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Einbeziehungskontrolle: Was ist für die Geltung von AGB erforderlich/für den Abschluss?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Soweit nicht durch Gesetz oder Verordnung anders angeordnet, gelten AGB nur kraft &lt;strong&gt;ausdrücklicher oder konkludenter Vereinbarung &lt;/strong&gt;der Parteien (Willenseinigung &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/861" rel="noopener noreferrer" target="_blank"&gt;§ 861 ABGB&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Geltungskontrolle: Was sind die Rechtsfolgen eines Verstoßes einer Klausel gegen § 864a ABGB?&lt;/p&gt;&lt;p&gt;Wann wird die Unwirksamkeit von Amts wegen geprüft, wann nur auf Einwand (des Unterworfenen)?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Klausel ist nicht Vertragsbestandteil&lt;/li&gt;&lt;li&gt;Der Restvertrag gilt &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(&lt;/span&gt;&lt;strong style="color: rgb(226, 148, 20); background-color: rgb(40, 45, 88);"&gt;Restgültigkeit des Vertrags&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;)&lt;/span&gt;, nur die Klausel selbst ist nichtig.&lt;/li&gt;&lt;li&gt;Erscheint die Klausel nach dem Verfahrensstadiums des Zivilprozesses &lt;strong&gt;nicht offenkundig&lt;/strong&gt; bedenklich, so wird die Unwirksamkeit nicht amtswegig sondern nur bei darauf gerichteter Einwendung geprüft.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie funktioniert die Geltungskontrolle der AGBs?&lt;/p&gt;&lt;p&gt;Welche 4 Tatbestandselemente sind notwendig?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;Jede konkrete Einzelklausel der AGB wird betrachtet&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;4 &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;kumulative &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;Tatbestandselemente für &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/864a" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 864a ABGB&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;:&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bestimmung ungewöhnlichen Inhalts&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nachteiligkeit für den Partner des Aufstellers&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Überraschungseffekt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Kein besonderer Hinweis des Aufstelleres auf die ungewöhnliche Klausel&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Inhaltskontrolle: Nichtigkeit gemäß &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/879" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 879 Abs 3&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;:&lt;/span&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Was sind die zwei Voraussetzungen?&lt;/li&gt;&lt;li&gt;Was ist die Rechtsfolge?&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Voraussetzungen: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Keine Hauptleistung (= Nebenbestimmungen)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gröbliche &lt;/strong&gt;Benachteiligung des Unterworfenen:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Bloße Benachteiligung reicht nicht aus.&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Gröblich z.B.: Verdünnte Willensfreiheit, oder AGB weichen von Wertung des objektiven dispositiven Rechts stark ab.&lt;/li&gt;&lt;li&gt;Klausel nicht Vertragsbestandteil, also nichtig.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Restvertrag gilt (&lt;strong&gt;Restgültigkeit des Vertrags&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Relative Nichtigkeit einer Klausel ist nur auf Einwendung wahrzunehmen.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Entgeltliche/Unentgeltliche/Entgeltfremde Rechtsgeschäfte?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage für Entgeltliche Rechtsgeschäfte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;entgeltlich&lt;/strong&gt;: immer Zweiseitig, jede Partei bringt die eigene Leistung um die Gegenleistung zu erhalten (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/917" rel="noopener noreferrer" target="_blank"&gt;§ 917 ABGB&lt;/a&gt;). Leistung muss nicht Geld sein.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;unentgeltlich&lt;/strong&gt;: Ein Partner erhält keine Gegenleistung (Schenkungsvertrag)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;entgeltsfremd&lt;/strong&gt;: liegen vor, wenn ein Bürge nachträglich einem existierenden Darlehensvertrag beitritt, ohne dass sich die Konditionen für den Hauptschuldner ändern.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie verhalten sich Individualvereinbarungen zu den AGB?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Spezielle Individualvereinbarungen, selbst mündliche, verdrängen die AGB.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie funktionieren die 3 Ebenen der Inhaltskontrolle in der Übersicht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;Scheitern AGB an Einbeziehungskontrolle -&amp;gt; &lt;strong&gt;Bedingungswerk &lt;/strong&gt;(gesamte AGB) wird nicht Teil des Vertrags &lt;/li&gt;&lt;li&gt;Scheitern einzelne Bestimmungen an der Geltungskontrolle, so sind nur diese Bestimmungen nichtig&lt;/li&gt;&lt;li&gt;Scheitern einzelne Bestimmungen an der Inhaltskontrolle, so sind nur diese nichtig&lt;/li&gt;&lt;li&gt;Alle übrigen Bestimmungen bleiben Vertragsinhalt.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Inhaltskontrolle: Wie kann die Nichtigkeit von AGB für Verbraucher durchgesetzt werden? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;strong&gt;Einzelprozess &lt;/strong&gt;(Auch ohne Vorbringen des Verbrauchers)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verbandsklage &lt;/strong&gt;von den Interessenverbänden &lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/28" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§§ 28-29 KSchG&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Abmahnung &lt;/strong&gt;-&amp;gt; Konventionalstrafe (&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/28" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 28 Abs 2 KSchG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Überschießende Klauseln &lt;/strong&gt;in AGB: Bei Verstoß gegen &lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/6" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 6 Abs 1 und 2 KSchG&lt;/a&gt; wird von der Fortgeltung der Klauseln ausgegangen, wenn sie (für den Konsumenten) vorteilhafte Bestimmungen enthalten.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Inhaltskontrolle: Wie wird das Transparenzgebot &lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/6" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 6 Abs 3 KSchG&lt;/a&gt; verstanden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Vertragsbestimmungen müssen den Verbraucher zuverlässig über seine Rechte und Pflichten informieren. Er soll möglichst &lt;strong&gt;durchschaubar, klar verständlich&lt;/strong&gt; und &lt;strong&gt;angepasst &lt;/strong&gt;an die Vertragsart so aufgeklärt werden, dass er &lt;strong&gt;nicht &lt;/strong&gt;von der &lt;strong&gt;Durchsetzung seiner Rechte abgehalten &lt;/strong&gt;wird, und ihm auch &lt;strong&gt;keine unberechtigten Pflichten auferlegt&lt;/strong&gt; werden.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Inhaltskontrolle: Abweichungen vom objektiven Recht&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Es wird nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/879" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 879 Abs 3&lt;/a&gt; &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;und &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/6" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 6 KSchG&lt;/a&gt; geprüft, ob Klauseln sachlich&lt;strong&gt; nicht gerechtfertigte unangemessene Abweichungen vom objektiven Recht&lt;/strong&gt; zulasten des unterworfenen enthalten.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Geltungskontrolle: Was ist der Überraschungseffekt (Überrumpelungs- bzw. Übertölpelungseffekt)&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Versteckte Klauseln die für den Unterworfenen überraschend sind.&lt;/li&gt;&lt;li&gt;Entfällt wenn diese Klauseln &lt;strong&gt;hervorgehoben &lt;/strong&gt;sind (fett, farbig, unterstrichen, ... ) oder &lt;strong&gt;mündlich &lt;/strong&gt;erklärt werden.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Entscheiden ist, ob dem Leser die ungewöhnliche Bestimmung aus dem Gesamteindruck der Urkunde auffällt.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Geltungskontrolle: Wann ist eine Bestimmung Nachteilig für den Partner des Aufstellers?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Weicht zulasten des Unterworfenen vom dispositiven objektiven Recht ab&lt;/li&gt;&lt;li&gt;Oder Stellt den Unterworfenen im Vergleich zum Aufsteller der AGB schlechter (aus der Sicht eines redlichen Vertragspartners)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Geltungskontrolle: Wie wird ungewöhnlicher Inhalt bestimmt?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Objektiv ungewöhnlich&lt;/strong&gt;: Wenn eine derartige Bestimmung in einem derartigen Vertrag üblicherweise (im redlichen Verkehr) nicht enthalten ist&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Subjektiv ungewöhnlich&lt;/strong&gt;:  Eine objektiv nicht ungewöhnliche Klausel kann subjektiv ungewöhnlich sein, wenn sie für den konkreten Vertragspartner im konkreten Zusammenhang, aus Sicht eines redlichen Aufstellers, überraschend sein musste und der Aufsteller nicht mit der Unterwerfung des Partners rechnen durfte.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Einbeziehungskontrolle: &lt;/span&gt;&lt;/p&gt;&lt;p&gt;Was sind kollidierende oder kreuzende AGB?&lt;/p&gt;&lt;p&gt;Was sind die Folgen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die AGB zweier Geschäftspartner sind punktuell nicht vereinbar&lt;/li&gt;&lt;li&gt;Folgen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Teildissens über die widersprüchlichen Punkte&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Die Beurteilung der Gültigkeit des Restvertrags folgt den Regeln über &lt;strong&gt;versteckten &lt;/strong&gt;und &lt;strong&gt;offenen &lt;/strong&gt;Dissens über Haupt- und Nebenpunkte.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nicht geregelte Punkte sind mit &lt;strong&gt;dispositivem Recht&lt;/strong&gt; und &lt;strong&gt;ergänzender Vertragsauslegung&lt;/strong&gt; zu ermitteln.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Einbeziehungskontrolle: &lt;/span&gt;&lt;/p&gt;&lt;p&gt;Wie kann ein Kunde den AGB zustimmen?&lt;/p&gt;&lt;p&gt;Können AGBs "Nachgeschoben" werden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ausdrücklich oder Konkludent&lt;/li&gt;&lt;li&gt;Einseitiges "Nachschieben" durch den Aufsteller der AGB &lt;strong&gt;reicht nicht&lt;/strong&gt; aus, eine &lt;strong&gt;Parteieneinigung &lt;/strong&gt;zur nachträglichen Einbeziehung von AGB ist &lt;strong&gt;aber nicht ausgeschlossen&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Einbeziehungskontrolle: &lt;/span&gt;Wie müssen AGB einbezogen werden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;ausdrücklicher &lt;strong&gt;Hinweis reicht&lt;/strong&gt;: "ich verweise auf meine AGB" (AGB müssen nicht real vorliegen) &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die „Verdünnung der Willensfreiheit“ des Kunden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Kunde kann "in der Schnelle" des Vertragsabschlusses den Inhalt umfangreicher AGB häufig nicht zur Kenntnis nehmen, oder ist sich der Reichweite nicht bewusst.&lt;/li&gt;&lt;li&gt;Kunde hat nur die Wahl die AGB Gesamt zu akzeptieren oder auf die Ware zu verzichten.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind AGB?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Allgemeine Geschäftsbedingungen sind vorformulierte standardisierte Vertragsbedingungen, die ein Vertragspartner für alle oder eine bestimmte Gruppe von Verträgen erstellt.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie funktioniert das Widerrufsrecht im Konsumentenschutz?&lt;/p&gt;&lt;p&gt;Was ist die Voraussetzung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nach § 3 KSchG: Verbraucher hat das Recht Angebot &lt;strong&gt;bis Vertragsabschluss&lt;/strong&gt; durch einseitigen Widerruf zu zerstören.&lt;/p&gt;&lt;p&gt;Voraussetzung: Vertragserklärung außerhalb des Geschäftsraumes des Unternehmens.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wo finden sich gesetzliche Rücktrittsrechte außerhalb von KschG und FAGG?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;H&lt;span style="background-color: rgb(255, 255, 255); color: rgb(77, 81, 86);"&gt;ypothekar- und Immobilienkreditgesetz (&lt;/span&gt;&lt;a href="https://www.ris.bka.gv.at/GeltendeFassung.wxe?Abfrage=Bundesnormen&amp;amp;Gesetzesnummer=20009367" rel="noopener noreferrer" target="_blank" style="background-color: rgb(255, 255, 255); color: rgb(77, 81, 86);"&gt;§ 13 HIKrG&lt;/a&gt;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(77, 81, 86);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Verbraucherkreditgesetz (&lt;a href="https://www.jusline.at/gesetz/vkrg/paragraf/13" rel="noopener noreferrer" target="_blank"&gt;§ 13 VKrG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Teilnutzungsgesetz (&lt;a href="https://www.jusline.at/gesetz/tng/paragraf/8" rel="noopener noreferrer" target="_blank"&gt;§ 8 TNG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Bauträgervertragsgesetz (&lt;a href="https://www.jusline.at/gesetz/btvg/paragraf/5" rel="noopener noreferrer" target="_blank"&gt;§ 5 BTVG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;...&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Voraussetzungen für einen Rücktritt von Fernabsatzverträgen?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/fagg/paragraf/11" rel="noopener noreferrer" target="_blank"&gt;§§ 11-18 FAGG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;§ 11 - Voraussetzungen&lt;/li&gt;&lt;li&gt;§ 18 - Kein Rücktrittsrecht&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Voraussetzungen für einen Rücktritt wegen Nichteintritts maßgeblicher Umstände? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/3a" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 3a KschG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Maßgebliche Umstände treten nicht oder nur in erheblich geringerem Maß als vom Unternehmer dargestellt ein&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Voraussetzungen für den Rücktritt vom Haustürgeschäft?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/3" rel="noopener noreferrer" target="_blank"&gt;§ 3 KschG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Weder in den vom &lt;strong&gt;Unternehmer für seine geschäftlichen Zwecke dauernd benützten Räumen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Noch bei&lt;strong&gt; einem von diesem dafür auf einer Messe oder einem Markt benützten Stand&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die 3 (wichtigsten) gesetzlichen Rücktrittsrechte des Käufers (insb. Verbrauchers)?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;Rücktritt vom Haustürgeschäft&lt;/li&gt;&lt;li&gt;Rücktritt wegen Nichteintritts maßgeblicher Umstände&lt;/li&gt;&lt;li&gt;Rücktritt von Fernabsatzverträgen&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Option/Optionsvertrag?&lt;/p&gt;&lt;p&gt;Was die rechtlichen Folgen?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Eine Partei räumt der anderen, oder einem Dritten, das Recht ein (unabhängig von einer weiteren rechtsgeschäftlichen Erklärung des Verpflichteten), ein inhaltlich &lt;strong&gt;im Vorhinein bestimmtes Schuldverhältnis&lt;/strong&gt; in Geltung zu setzen&lt;/li&gt;&lt;li&gt;Rechtsfolge: Der Optionsberechtigte kann &lt;strong&gt;nach Ausübung der Option&lt;/strong&gt; unmittelbar die vertragliche Hauptleistung einklagen.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Punktation? Rechtliche Grundlagen?&lt;/p&gt;&lt;p&gt;Was sind die Voraussetzungen?&lt;/p&gt;&lt;p&gt;Was die rechtlichen Folgen? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/885" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 885 ABGB&lt;/a&gt;: Vorläufige (nicht formelle) verbindliche Fixierung der Hauptpunkte eines Vertrages -&amp;gt; Vertrag kommt zustande.&lt;/li&gt;&lt;li&gt;Voraussetzungen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Unterliegt der Schriftform (Schriftlich + Unterschrift), erfordert also Bindungswillen beider Parteien&lt;/li&gt;&lt;li&gt;Rechtsfolgen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Klage auf vertraglich geschuldete Leistungen möglich&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zeitlich nicht begrenzt (anders als Vorvertrag) -&amp;gt; normale Verjährungsjahre&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Vorvertrag, was die gesetzliche Grundlage?&lt;/p&gt;&lt;p&gt;Wann und wie Lange ist er gültig?&lt;/p&gt;&lt;p&gt;Worauf kann geklagt werden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/936" rel="noopener noreferrer" target="_blank"&gt;§ 936 ABGB&lt;/a&gt;: Vertrag über den künftigen Abschluss des von den Parteien in Aussicht genommenen Hauptvertrages.&lt;/li&gt;&lt;li&gt;Gilt nur:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Parteien haben sich über den wesentlichen Inhalt (z.B.: Ware und Preis) des Hauptvertrages geeinigt.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zeitpunkt für Hauptvertrag-Abschluss ist fixiert.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gilt max 1 Jahr&lt;/li&gt;&lt;li&gt;Klage nur auf Abschluss des Hauptvertrags, nicht auf Leistungen aus dem Hauptvertrag.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;ECG&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;E-Commerce-Gesetz&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche gesetzlichen Grundlagen regeln Vertragsabschluss im E-Commerce?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Elektronische Willenserklärung -&amp;gt; es gelten grundsätzlich die allgemeinen Regelungen &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/861" rel="noopener noreferrer" target="_blank"&gt;§§ 861ff ABGB&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/ecg/paragraf/10" rel="noopener noreferrer" target="_blank"&gt;§§ 10 -12 ECG&lt;/a&gt;: Sondervorschriften über &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Abgabe einer Vertragserklärung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vertragsbestimmungen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Geschäftsbedingungen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zugang elektronischer Erklärungen.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was regelt das FAGG?&lt;/p&gt;&lt;p&gt;Was ist in Bezug auf Vertragsschluss besonders zu beachten?&lt;/p&gt;&lt;p&gt;Welche gesetzlichen Grundlagen gibt es?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/fagg/paragraf/1" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§§ 1 - 11 FAGG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/fagg/paragraf/1" rel="noopener noreferrer" target="_blank"&gt;§ 1 Abs 1 FAGG&lt;/a&gt; -&amp;gt; Fern- und Auswärtsgeschäfte zwischen Unternehmern und Verbrauchern.&lt;/li&gt;&lt;li&gt;Beachten: Informationspflichten vor Vertragsschluss&lt;/li&gt;&lt;li&gt;Art und Umfang der Informationserteilung abhängig von Vertragstypen und Vertragsschlusssituation (§§ 4 - 9 FAGG)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;FAGG&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Fern- und Auswertsgeschäfte-Gesetz&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Einfluss eines Kaufmännischen Bestätigungsschreiben auf einen Vertrag?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Grundsätzlich keine vertragsändernde Wirkung&lt;/li&gt;&lt;li&gt;Schweigen des Empfängers gilt nicht als Zustimmung zu Vertragsabschluss- oder Änderung, außer:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bestätigungsschreiben ergänzt bloß &lt;strong&gt;geringfügige Punkte&lt;/strong&gt;, die beim Vertragsabschluss &lt;strong&gt;bewusst von beiden Parteien&lt;/strong&gt; offen gelassen wurden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Empfänger wird &lt;strong&gt;nur begünstigt.&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Kreuzofferte? &lt;/p&gt;&lt;p&gt;Was ist die Auswirkung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;"Überkreuzung" am Postweg: Zwei künftige Vertragspartner übermitteln einander Angebote auf An- und Verkauf derselben Sache die inhaltlich identisch sind.&lt;/li&gt;&lt;li&gt;Vertrag wird mit Zugang der letzten Offerte perfekt; wenn Parteirollen zusammenpassen (Verkäufer+Käufer)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Angebot "ohne Obligo" (unverbindliches, freibleibendes Offert)?&lt;/p&gt;&lt;p&gt;Ist es gültig? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Beschränkung der Bindung an den Vertragsabschluss durch einseitige Annahme durch Klausel&lt;/li&gt;&lt;li&gt;Anbieter behält sich vor &lt;strong&gt;bis zur Annahme&lt;/strong&gt; durch Widerruf das Angebot zu zerstören&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Üblicherweise Widerruf nur bis Zugang bei Annehmenden, Klausel versucht also Widerrufzeitraum zu verlängern&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Frage: Darf der Anbieter das?&lt;/li&gt;&lt;li&gt;Im Zweifel nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/915" rel="noopener noreferrer" target="_blank"&gt;§ 915 ABGB&lt;/a&gt; vorgehen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Anbieter kann nach Zugang nicht mehr widerrufen, d.h. Angebot ist gar kein wirkliches Angebot da kein Bindungswille.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Annahmeerklärung des Annehmenden ist also eigentlich ein Angebot.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ursprünglicher Anbieter hat Redepflicht um abzulehnen, sonst kommt Vertrag nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/842a" rel="noopener noreferrer" target="_blank"&gt;§ 842a&lt;/a&gt; ABGB zustande&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was bedeutet "Protestatio facto contraria valet"?&lt;/p&gt;&lt;p&gt;Welche rechtlichen Fragen stellen sich daraus?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Protest entgegen den Fakten schadet nicht&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Fragen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Kann faktische Inanspruchnahme einer Leistung einen Vertrag zustandekommen lassen? &lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Auch wenn er klar äußert, dass er keinen Vertrag abschließen will? &lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Beispiel: Einsteigen in Öffentliches Verkehrsmittel, Benutzen von Parkplatz&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;Kann faktische Inanspruchnahme einer Leistung einen Vertrag zustandekommen lassen? &lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;Auch wenn er klar äußert, dass er keinen Vertrag abschließen will? &lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;Was bedeutet dies für "Protest entgegen den Fakten schadet nicht" in Ö? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank"&gt;§ 863 ABGB&lt;/a&gt;: Konkludente Handlung nur, wenn kein vernünftiger Grund daran zu zweifeln&lt;/li&gt;&lt;li&gt;Rechtslehre sagt: Nur ausdrückliche oder konkludente WE führt zu Vertrag&lt;/li&gt;&lt;li&gt;Daher bei Klarstellung das kein Wille zum Vertrag -&amp;gt; kein Vertrag&lt;/li&gt;&lt;li&gt;Zahlungen für Inanspruchnahme daher nicht aus Vertrag, aber z.B.: Bereicherungsrecht, Schadenersatzrecht.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;-&amp;gt; Protest gegen die Fakten schadet in Österreich!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der unterschied zwischen "Angebot an unbekannte Person" und "invitatio ad offerendum"?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Angebot an unbekannt:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bindungswille: Verkäufer gibt zu erkennen das präsentierte, reale Waren zum Verkauf an jeden stehen, solange Vorrat reicht (z.B.: Getränkeautomat)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Kann idR durch Willensbetätigung angenommen werden (Annahmehandlung nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/864" rel="noopener noreferrer" target="_blank"&gt;§ 864 ABGB&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Konkreter Unterschied: &lt;strong&gt;Beschränkung des Angebotes auf den real vorhandenen Vorrat&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Invitatio ad offerendum: Erklärender will sich erkennbar nicht gegenüber jedermann binden (z.B.: Flugblatt, Katalog)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Prinzip der kausalen Tradition (Lehre von Titel und Modus)? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/380" rel="noopener noreferrer" target="_blank"&gt;§ 380 ABGB&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/424" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(115, 133, 197);"&gt;§§ 424ff ABGB&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;, &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/1053" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(115, 133, 197);"&gt;§ 1053 ABGB&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;, &lt;/span&gt;&lt;/p&gt;&lt;p&gt;Zum Erwerb des Eigentumsrechts muss zum gültigen Verpflichtungsgeschäft (&lt;strong&gt;Titel&lt;/strong&gt;) auch ein Verfügungsgeschäft (&lt;strong&gt;Modus&lt;/strong&gt;) hinzutreten.&lt;/p&gt;&lt;p&gt;-&amp;gt; &lt;strong&gt;Man wird nicht bereits mit Abschluss des Kaufvertrages Eigentümer.&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie nennt man entgeltliche Rechtsgeschäfte noch? &lt;/p&gt;&lt;p&gt;Was ist die Bedeutung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Synallagmatische Verträge&lt;/li&gt;&lt;li&gt;Erbringt ein Teil seine Leistung nicht, muss auch der andere seine nicht erbringen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Schutznormen des KSchG? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/3" rel="noopener noreferrer" target="_blank"&gt;§ 3-6 KSchG&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/fagg/paragraf/11" rel="noopener noreferrer" target="_blank"&gt;§§ 11ff FAGG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Verbraucher kann von einem sog. Haustürgeschäft zurücktreten (grundlos innerhalb bestimmter Fristen) &lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; (§ 3 KSchG)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;besonderes Rücktrittsrecht &lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;(§ 3 KSchG, §§ 11ff FAGG)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Kostenvoranschlag gegenüber Verbraucher gilt als Garantie &lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; (§ 5 KSchG)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Bestimmte Klauseln in AGBs sind Unwirksam (§ 6 KSchG)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Realofferte? Was die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/864" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(136, 125, 220);"&gt;§ 864 Abs. 2 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Behalten, Verwenden, Verbrauchen einer Sache gilt nicht als Annahme eines Angebots, wenn sie dem Empfänger ohne dessen Veranlassung übersandt wurde.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Angebotsannahme: Rechtzeitigkeit der Annahme&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/862" rel="noopener noreferrer" target="_blank"&gt;§ 862 ABGB&lt;/a&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Angebot erlischt nach Geltungsdauer, diese muss eruiert werden:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Vom Erklärenden gesetzt (im Rahmen von &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/902" rel="noopener noreferrer" target="_blank"&gt;§§ 902f ABGB&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Sonst gesetzliche Frist nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/862" rel="noopener noreferrer" target="_blank"&gt;§ 862 S2 ABGB&lt;/a&gt; (inkl Postlauf des Angebots, Überlegungsfrist und Postlauf der Annahme)&lt;/li&gt;&lt;li&gt;Ausnahme &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/862a" rel="noopener noreferrer" target="_blank"&gt;§ 862a ABGB&lt;/a&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Verzögerung der nachweislich rechtzeitig abgesendeten Annahmeerklärung am Postweg (=Übermittlung)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Der Antragsteller kann aber &lt;strong&gt;unverzüglich &lt;/strong&gt;(ohne schuldhaftes Zögern) zurücktreten&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Was sind die 5 Voraussetzungen für Angebotsannahme durch &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Willensbetätigung&lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/864" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 864 ABGB&lt;/a&gt; &lt;/p&gt;&lt;ol&gt;&lt;li&gt;Willenserklärung nicht zu erwarten (Natur des Geschäfts, Verkehrssitte, Verzicht durch Anbieter)&lt;/li&gt;&lt;li&gt;Annahmehandlung: Annehmender Verfügt über die Sache in einer Weise, zu der er nur berechtigt ist, wenn er das Angebot annehmen will (z.B: Versand der bestellten Ware).&lt;/li&gt;&lt;li&gt;Annahmewille (Vertragsabschlusswille)&lt;/li&gt;&lt;li&gt;Rechtzeitigkeit der Annahme: Während der Geltungsdauer des Angebots; Willensbetätigung ist aber &lt;strong&gt;nicht zugangsbedürftig &lt;/strong&gt;-&amp;gt; es zählt Zeitpunkt der Annahmehandlung. &lt;/li&gt;&lt;li&gt;Kein Widerruf der Willensbetätigung: Widerruf der Annahme bis zur Kenntnisnahme des Anbietenden möglich.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Realakte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Handlungen ohne Kundgabezweck die auch ohne Geschäftsfähigkeit und Rechtsfolgewillen Rechtsfolgen auslösen (z.B.: Urheberrechte durch Schaffen von Kunstwerk, Rechte und Pflichte durch Fund)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Willensmitteilung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Willenshandlungen ohne Rechtsfolgewillen (z.B. Mahnung zeigt dass Zahlung erwünscht ist)&lt;/li&gt;&lt;li&gt;Rechtsfolgen treten unabhängig von Rechtsfolgewillen des Handelnden ein (z.B.: Mahnung bewirkt Fälligkeit)&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Willensmitteilung kann kein Angebot/Annahme sein.&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Wissenserklärung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Nur auf Kundgabe von Fakten oder Kenntnissen gerichtet (Quittung, Mitteilung des Kontostantds, ... )&lt;/li&gt;&lt;li&gt;Vorschriften für Rechtsgeschäfte weitgehend auf &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wissenserklärung  angewandt, aber &lt;/span&gt;Angebot/Annahme durch &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wissenserklärung &lt;/span&gt;nicht möglich&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was kann eine stillschweigende/konkludente Willenserklärung sein?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Eindeutige Handlung nach Verkehrssitte ohne vernünftigen Grund daran zu zweifeln (z.B.: verzehren des aus dem Korb entnommenen Brots)&lt;/li&gt;&lt;li&gt;passives Unterlassen (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 863 ABGB&lt;/a&gt; ): Schweigen gilt nicht als Zustimmung, außer es besteht eine Redepflicht aus:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gesetz&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Verträgen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Übung des redlichen Verkehrs (z.B.: ständige Geschäftsverbindungen)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;vorvertragliche Aufklärungspflichten&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die 4 Voraussetzungen für die Annahme eines Angebots durch &lt;strong&gt;Willenserklärung&lt;/strong&gt;? Was ist die Rechtliche Grundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank"&gt;§ 863 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ol&gt;&lt;li&gt;Ausdrückliche oder konkludente Willenserklärung&lt;/li&gt;&lt;li&gt;Zugang der Willenserkärung&lt;/li&gt;&lt;li&gt;Rechtzeitigkeit der Annahme&lt;/li&gt;&lt;li&gt;Kein Widerruf der Annahme&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die 2 Grundvorraussetzungen für das Zustandekommen eines Vertrags? Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/861" rel="noopener noreferrer" target="_blank"&gt;§§ 861 ff ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Angebot + Annahme&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtsfähigkeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;gibt jedem Rechtssubjekt die Macht, seine Belange (seine eigene Rechtssphäre) nach freiem Belieben zu regeln.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Willenserklärung: &lt;/span&gt;Rechtsfolgewille (Geltungswille)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Der Handelnde ist an seiner Erklärung gebunden, wenn er in dem Bewusstsein handelt, rechtliche verbindliche Handlungen zu setzen, die erforderlichenfalls mit staatlichen Zwang durchsetzbar sind (gemäßigte Rechtsfolgentheorie).&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Welches weitere Gesetz definiert Unternehmensformen die für die Auslegung des KSchG relevant sind?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;UGB 2007&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die Schutznormen des KSchG?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/3" rel="noopener noreferrer" target="_blank"&gt;§ 3-6 KSchG&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/fagg/paragraf/11" rel="noopener noreferrer" target="_blank"&gt;§§ 11ff FAGG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Verbraucher kann von einem sog. Haustürgeschäft zurücktreten (grundlos innerhalb bestimmter Fristen) &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; (§ 3 KSchG)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;besonderes Rücktrittsrecht  &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(§ 3 KSchG, §§ 11ff FAGG)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Kostenvoranschlag gegenüber Verbraucher gilt als Garantie &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; (§ 5 KSchG)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Bestimmte Klauseln im AGB sind Unwirksam (§ 6 KSchG)&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;p&gt;UGB 2007 (Unternehmensgesetzbuch)&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was sind Verbrauchergeschäfte? &lt;/p&gt;</t>
@@ -37,12 +499,6 @@
     <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/1" rel="noopener noreferrer" target="_blank"&gt;§ 1 &lt;/a&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/1" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;KSchG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;: &lt;/span&gt;Wenn an einem zweiseitigen RG einerseits ein Unternehmer, für den das RG zum Betrieb seines Unternehmens gehört, und andererseits ein Verbraucher, auf den das nicht zutrifft, beteiligt -&amp;gt; Anwendung des KSchG &lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist das Prinzip der kausalen Tradition (Lehre von Titel und Modus)? Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/380" rel="noopener noreferrer" target="_blank"&gt;§ 380 ABGB&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/424" rel="noopener noreferrer" target="_blank" style="color: rgb(115, 133, 197); background-color: rgb(40, 45, 88);"&gt;§§ 424ff ABGB&lt;/a&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;, &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/1053" rel="noopener noreferrer" target="_blank" style="color: rgb(115, 133, 197); background-color: rgb(40, 45, 88);"&gt;§ 1053 ABGB&lt;/a&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;, &lt;/span&gt;&lt;/p&gt;&lt;p&gt;Zum Erwerb des Eigentrumsrechts muss zum gültigen Verpflichtungsgeschäft (&lt;strong&gt;Titel&lt;/strong&gt;) auch ein Verfügungsgeschäft (&lt;strong&gt;Modus&lt;/strong&gt;) hinzutreten.&lt;/p&gt;&lt;p&gt;-&amp;gt; &lt;strong&gt;Man wird nicht bereits mit Abschluss des Kaufvertrages Eigentümer.&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was sind Abstrakte/Kausale Rechtsgeschäfte?&lt;/p&gt;</t>
   </si>
   <si>
@@ -67,18 +523,6 @@
     <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Konsensual&lt;/strong&gt;: Kommen durch bloße Einigung zustande  (Kaufvertrag, Mietvertrag, ...)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Real&lt;/strong&gt;: Erfordert zum Abschluss auch Sachübergabe (Darlehensvertrag, Leihvertrag und Verwahrungsvertrag)&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was sind Entgeltliche/Unentgeltliche/Entgeltfremde Rechtesgeschäfte?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;entgeltlich&lt;/strong&gt;: immer Zweiseitig, jede Partei bringt die eigene Leistung um die Gegenleistung zu erhalten (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/917" rel="noopener noreferrer" target="_blank"&gt;§ 917 ABGB&lt;/a&gt;). Leistung muss nicht Geld sein.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;unentgeltlich&lt;/strong&gt;: Ein Partner erhält keine Gegenleistung (Schenkungsvertrag)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;entgeltsfremd&lt;/strong&gt;: liegen vor, wenn ein Bürge nachträglich einem existierenden Darlehensvertrag beitritt, ohne dass sich die Konditionen für den Hauptschuldner ändern.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie nennt man entgeltliche Rechtsgeschäfte noch? Was ist die Bedeutung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Synallagmatische Verträge&lt;/li&gt;&lt;li&gt;Erbringt ein Teil seine Leistung nicht, muss auch der andere seine nicht erbringen&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was sind Rechtsgeschäfte unter Lebenden, und von Todes wegen?&lt;/p&gt;</t>
   </si>
   <si>
@@ -133,12 +577,6 @@
     <t>&lt;ul&gt;&lt;li&gt;Abschlussfreiheit (ob, wann und mit wem Vertrag geschlossen wird)&lt;/li&gt;&lt;li&gt;Inhaltsfreiheit&lt;/li&gt;&lt;li&gt;Typenfreiheit (neue Vertragstypen zu schaffen)&lt;/li&gt;&lt;li&gt;Beendigungsfreiheit&lt;/li&gt;&lt;li&gt;Änderungsfreiheit&lt;/li&gt;&lt;li&gt;Formfreiheit&lt;/li&gt;&lt;li&gt;Testierfreiheit (ob und wie der Verstorbene letztwillig testiert)&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist die Rechtsfähigkeit?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;gibt jedem Rechtssubjekt die Macht, seine Belange (seine eigene Rechtssphäre) nach freiem Belieben zu regeln, Rechte zu erwerben, zu ändern oder aufzugeben&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist ein Rechtsgeschäft?&lt;/p&gt;</t>
   </si>
   <si>
@@ -148,13 +586,13 @@
     <t>&lt;p&gt;Was ist die Privatautonomie?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;ermöglicht jedem Rechtssubjekt durch freie eigene willentliche Entscheidung seine Rechtsverhältnisse (Berechtigung und Verpflichtung) eigenverantwortlich nach Belieben innerhalb der gesetzlichen Schranken zu gestalten&lt;/li&gt;&lt;li&gt;Genießt Verfassungsrang&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine Willenserklärung?&lt;/p&gt;&lt;p&gt;Woraus besteht eine Willenserklärung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Grundbestandteil jedes Rechtsgeschäfts&lt;/li&gt;&lt;li&gt;Willensäußerung und Handlung, Rechtsfolgewille, Kundgabezweck&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;ul&gt;&lt;li&gt;ermöglicht jedem Rechtssubjekt durch eigene willentliche Entscheidung seine Rechtsverhältnisse nach Belieben im Rahmen der Gesetze zu gestalten&lt;/li&gt;&lt;li&gt;Genießt Verfassungsrang&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Willenserklärung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Eine Willenserklärung ist eine Willensäußerung oder –handlung, die auf die Herbeiführung von Rechtsfolgen gerichtet ist  und mit der ein Kundgabezweck verfolgt wird.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(226, 148, 20);"&gt;Strenge Rechtsfolgentheorie zu Rechtsfolgewille&lt;/span&gt;&lt;/p&gt;</t>
@@ -175,12 +613,6 @@
     <t>&lt;p&gt;Vor dem Zugang ist die Erklärung noch nicht wirksam und kann daher vom Erklärenden noch widerrufen werden, es liegt hier noch keine Bindungswirkung vor.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Voraussetzung für einen gültigen Widerruf ist nur, dass der Widerruf vor oder spätestens gleichzeitig mit der zu widerrufenden Erklärung zugeht (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/862a" rel="noopener noreferrer" target="_blank"&gt;§ 862a ABGB&lt;/a&gt;).&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Willenserklärung: &lt;/span&gt;Rechtsfolgewille - Geltungswille&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Der Handelnde ist an seiner Erklärung gebunden, wenn er in dem Bewusstsein handelt, rechtliche verbindliche Handlungen zu setzen, die erforderlichenfalls mit staatlichen Zwang durchsetzbar sind (gemäßigte Rechtsfolgentheorie).&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist der Bindungswille des Erklärenden?&lt;/p&gt;</t>
   </si>
   <si>
@@ -202,13 +634,13 @@
     <t>&lt;p&gt;Willenserklärung: Willensäußerung und Handlung&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Der Handlungswille des Rechtssubjektes ist unabdingbarer Bestandteil für das Vorliegen einer Willenserklärung. Das Verhalten soll willentlich, also vom eigenen Willen gesteuert, sein.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Bestimmtheit der Willenserklärung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/869" rel="noopener noreferrer" target="_blank"&gt;§ 869 ABGB&lt;/a&gt;&lt;/p&gt;&lt;p&gt;Das Angebot muss i&lt;strong&gt;nhaltlich ausreichend bestimmt&lt;/strong&gt; sein, d.h. die wesentlichen Punkte (&lt;strong&gt;Ware und Preis müssen bestimmt oder bestimmbar sein&lt;/strong&gt;) des abzuschließenden Vertrages müssen, jedenfalls der Mindestinhalt (&lt;strong&gt;essentialia negotii&lt;/strong&gt;) muss bestimmt sein.&lt;/p&gt;</t>
+    <t>&lt;p&gt;Der Handlungswille des Rechtssubjektes ist unabdingbarer Bestandteil für das Vorliegen einer Willenserklärung. Das Verhalten soll willentlich sein (Reflexe, Gewalt, ... gilt nicht)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Bestimmtheit der Willenserklärung?&lt;/p&gt;&lt;p&gt;Was ist die rechtliche Grundlage? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/869" rel="noopener noreferrer" target="_blank"&gt;§ 869 ABGB&lt;/a&gt;&lt;/p&gt;&lt;p&gt;Das Angebot muss &lt;strong&gt;inhaltlich ausreichend bestimmt&lt;/strong&gt; sein, d.h. die wesentlichen Punkte (&lt;strong&gt;Ware und Preis müssen bestimmt oder bestimmbar sein&lt;/strong&gt;) des abzuschließenden Vertrages müssen, jedenfalls der Mindestinhalt (&lt;strong&gt;essentialia negotii&lt;/strong&gt;) muss bestimmt sein.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist die Empfangstheorie?&lt;/p&gt;</t>
@@ -245,12 +677,6 @@
   </si>
   <si>
     <t>&lt;ol&gt;&lt;li&gt;&lt;strong&gt;Interessentheorie &lt;/strong&gt;(Jurist Ulpian): öffentliches Recht dient den Interessen der Allgemeinheit, Privatrecht den Interessen des Einzelnen.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Subjektionstheorie&lt;/strong&gt;: Während beim Privatrecht einander gleichberechtigte Rechtssubjekte gegenüberstehen (&lt;a href="https://www.jusline.at/gesetz/jn/paragraf/1" rel="noopener noreferrer" target="_blank"&gt;§ 1 JN)&lt;/a&gt;, stehen einander im öffentlichen Recht der Rechtsunterworfene und der Hoheitsträger gegenüber.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Subjektstheorie&lt;/strong&gt;: Es handelt sich um öffentliches Recht, wenn zumindest ein Hoheitsträger am Rechtsverhältnis beteiligt ist, der in Ausübung der Hoheitsgewalt auftritt. Tritt kein Beteiligter mit Hoheitsgewalt auf, so liegt privatrechtliches Handeln vor.&amp;nbsp;&lt;/li&gt;&lt;/ol&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Bedeutung der Abgrenzung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/jn/paragraf/1" rel="noopener noreferrer" target="_blank"&gt;§ 1 JN&lt;/a&gt; und § &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/1" rel="noopener noreferrer" target="_blank"&gt;1 ABGB &lt;/a&gt;&lt;/p&gt;&lt;p&gt;Während das Privatrecht die Rechtsbeziehungen von gleichberechtigten Rechtssubjekten untereinander trägt (z. B. Mietrecht, Vertragsrecht, etc.), steht im öffentlichen Recht der Staat den rechtsunterworfenen Bürgern übergeordnet gegenüber und wird hoheitlich tätig (z. B. Baurecht, Steuerrecht, etc.).&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist die Rechtsordnung? &lt;/p&gt;</t>
@@ -664,7 +1090,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B115"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -1022,6 +1448,574 @@
         <v>87</v>
       </c>
     </row>
+    <row r="45" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Add cards for chapter 14
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
+++ b/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="288">
   <si>
     <t>Question</t>
   </si>
@@ -19,24 +19,210 @@
     <t>Answer</t>
   </si>
   <si>
-    <t>&lt;p&gt;Wie kann ein auslegungsbedürftiger Vertrag mit der &lt;strong&gt;einfachen Vertragsinpterpretation &lt;/strong&gt;ausgelegt werden?&lt;/p&gt;</t>
+    <t>&lt;p&gt;Welcher Zeitpunkt zählt als Empfangszeitpunkt laut Empfangstheorie wenn z.B.: eine Erklärung in einem Postfach hinterlegt wird?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der objektiv erste mögliche Zeitpunkt der Kenntnisnahme durch den Empfänger, z.B.: Ankunft des Briefs im Postfach (der Empfänger &lt;strong&gt;könnte&lt;/strong&gt; den Brief abholen), NICHT wenn der Empfänger &lt;strong&gt;tatsächlich&lt;/strong&gt; Abholt.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was sind die 5 Voraussetzungen für Angebotsannahme durch &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Willensbetätigung&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;?&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Rechtsgrundlage?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/864" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 864 ABGB&lt;/a&gt; &lt;/p&gt;&lt;ol&gt;&lt;li&gt;Willenserklärung nicht zu erwarten (Natur des Geschäfts, Verkehrssitte, Verzicht durch Anbieter)&lt;/li&gt;&lt;li&gt;Annahmehandlung: Annehmender Verfügt über die Sache in einer Weise, zu der er nur berechtigt ist, wenn er das Angebot annehmen will (z.B: Versand der bestellten Ware).&lt;/li&gt;&lt;li&gt;Annahmewille (Vertragsabschlusswille)&lt;/li&gt;&lt;li&gt;Rechtzeitigkeit der Annahme: Während der Geltungsdauer des Angebots; Willensbetätigung ist aber &lt;strong&gt;nicht zugangsbedürftig &lt;/strong&gt;-&amp;gt; es zählt Zeitpunkt der Annahmehandlung. &lt;/li&gt;&lt;li&gt;Kein Widerruf der Willensbetätigung: Widerruf der Annahme bis zur Kenntnisnahme des Anbietenden möglich.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Rechtsfolgen der Nichterfüllung einer Bedingung?&lt;/p&gt;&lt;p&gt;Wie muss eine Bedingung erfüllt werden?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Rechtserwerb wird verhindert bzw. Rechtsverlust herbeigeführt.&lt;/li&gt;&lt;li&gt;Muss nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/699" rel="noopener noreferrer" target="_blank"&gt;§ 699 ABGB&lt;/a&gt; &lt;strong&gt;stets genau erfüllt &lt;/strong&gt;werden.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Rechtsfolgen der Nichteinhaltung einer Auflage? &lt;/p&gt;&lt;p&gt;Wie muss eine Auflage erfüllt werden?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Einhaltung kann durch Klage oder Exekution erzwungen werden.&lt;/li&gt;&lt;li&gt;Nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/709" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 709 ABGB&lt;/a&gt; genügt die &lt;strong&gt;annähernde &lt;/strong&gt;Erfüllung, wenn die &lt;strong&gt;genaue&lt;/strong&gt; Erfüllung &lt;strong&gt;nicht möglich &lt;/strong&gt;ist.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Auflage?&lt;/p&gt;&lt;p&gt;Wie ist sie im Zweifel zu behandeln, Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/709" rel="noopener noreferrer" target="_blank"&gt;§ 709 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Die einem Empfänger einer Zuwendung im Zusammenhang mit einer &lt;strong&gt;letztwillligen Verfügung&lt;/strong&gt; oder einem &lt;strong&gt;unentgeltlichen Rechtsgeschäft unter Lebenden&lt;/strong&gt; auferlegte &lt;strong&gt;Verpflichtung &lt;/strong&gt;zur &lt;strong&gt;Vornahme eines bestimmten Verhaltens&lt;/strong&gt; bei &lt;strong&gt;sonstigem Verlust der Zuwendung&lt;/strong&gt;, wobei es unerheblich ist, in wessen Interesse das geforderte Verhalten ist.&lt;/li&gt;&lt;li&gt;Im zweifel als auflösende Bedingung nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/10" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 710 ABGB&lt;/a&gt; &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie werden Samstage, Sonntage und gesetzliche Feiertage bei Fristen gehandhabt?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Zählen in die Berechnung der Frist&lt;/li&gt;&lt;li&gt;Ist der letzte Tag der Frist ein Sa, So oder gesetzl. Feiertag, so läuft die Frist mit&lt;strong&gt; Ende des nächstfolgenden Werktages ab&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/903" rel="noopener noreferrer" target="_blank"&gt;§ 903 S3 ABGB&lt;/a&gt;, &lt;a href="https://www.ris.bka.gv.at/GeltendeFassung.wxe?Abfrage=Bundesnormen&amp;amp;Gesetzesnummer=10000765" rel="noopener noreferrer" target="_blank"&gt;Art. 5 EuFrÜb&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Rechtsgrundlagen für Fristen sind heranzuziehen, wenn weder Sondergesetze noch Parteien anders vereinbaren?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/902" rel="noopener noreferrer" target="_blank"&gt;§§ 902-904 ABGB&lt;/a&gt; und EuFrÜb (Europäisches Übereinkommen über die Berechnung von Frist)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Befristung?&lt;/p&gt;&lt;p&gt;Was ist der Unterschied zur Bedingung? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Eine von den &lt;strong&gt;Parteien gesetzte Beschränkung&lt;/strong&gt; des Rechtsgeschäftes, bei der &lt;strong&gt;Inkrafttreten&lt;/strong&gt; oder &lt;strong&gt;Außerkrafttreten &lt;/strong&gt;der Rechtswirkung entweder &lt;strong&gt;kalendrisch bestimmt&lt;/strong&gt;, oder von einem &lt;strong&gt;sicher eintretenden Ereignis&lt;/strong&gt; abhängig gemacht wird.&lt;/li&gt;&lt;li&gt;Unterschied: Bedingung hat ein ungewisses Ereignis.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Beispiel 1: "Wenn A stirbt ..." ist eine Befristung, aufgrund der Gewissheit des Eintretens.&lt;/p&gt;&lt;p&gt;Beispiel 2: "Sollte A das 90. Lebensjahr erreichen ... " ist eine Bedingung, weil Ungewiss.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Termin?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ein rechtlich erheblicher Zeitpunkt&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Frist?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Eine rechtlich erhebliche Zeitspanne&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Beeinflussing wider Treu und Glauben? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gelingt es jemandem, dem die Bedingung zum &lt;strong&gt;Nachteil &lt;/strong&gt;gereicht, sie zu &lt;strong&gt;vereiteln&lt;/strong&gt;, gilt die Bedingung als &lt;strong&gt;eingetreten&lt;/strong&gt;. &lt;/li&gt;&lt;li&gt;Gelingt es jemandem, dem die Bedingung zum &lt;strong&gt;Vorteil &lt;/strong&gt;gereicht, die Bedingung wider Treu und Glauben &lt;strong&gt;herbeizuführen&lt;/strong&gt;, gilt die Bedingung als &lt;strong&gt;ausgefallen&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Beispiel: X verspricht Y ihm sein Auto zu schenken, wenn die nächste Reperatur ansteht. Y sapotiert das Auto von X. Die Bedingung wurde wider Treu und Glauben herbeigeführt und gilt daher als ausgefallen und die Schenkung tritt nicht in kraft.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtsgrundlage für unmögliche aufschiebende und unmögliche auflösende Bedingungen? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/698" rel="noopener noreferrer" target="_blank" style="color: black; background-color: rgb(40, 45, 88);"&gt;§ 698 ABGB&lt;/a&gt;, für letzten Willen auch &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/898" rel="noopener noreferrer" target="_blank"&gt;§ 898 ABGB&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann ist eine Bedingung unmöglich?&lt;/p&gt;&lt;p&gt;Was ist unmöglich allgemein definiert?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Eine Bedingung ist &lt;strong&gt;unmöglich&lt;/strong&gt;, wenn sie aus &lt;strong&gt;tatsächlichen&lt;/strong&gt; oder &lt;strong&gt;rechtlichen Gründen &lt;/strong&gt;nicht eintreten kann.&lt;/li&gt;&lt;li&gt;Unmöglich ist, was &lt;strong&gt;objektiv gesehen&lt;/strong&gt; und &lt;strong&gt;nicht &lt;/strong&gt;nur &lt;strong&gt;vorrübergehend &lt;/strong&gt;sondern &lt;strong&gt;dauerhaft&lt;/strong&gt; &lt;strong&gt;unmöglich&lt;/strong&gt; ist und niemand erfüllen kann.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Bedingungen gelten nicht?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/697" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: black;"&gt;§ 697 ABGB&lt;/a&gt;&lt;/p&gt;&lt;p&gt;Unverständliche, unbestimmte, sowie gesetz- oder sittenwidrige Bestimmungen&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind bejahende (positive) Bedingungen?&lt;/p&gt;&lt;p&gt;Was sind verneinende (negative) Bedingungen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Positive&lt;/strong&gt;: wenn du deine Freundin heiratest, bekommst du ein Auto &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Negative&lt;/strong&gt;: Wenn du nicht rauchst, bekommst du ein Auto&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sind Rechtsbedingungen Bedingungen im Sinne von &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/696" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: black;"&gt;§ 696 ABGB&lt;/a&gt;? Warum schon/warum nicht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nein, sie sind gesetzliche Vorraussetzungen und daher &lt;strong&gt;unabhängig von der Aufnahme in den Vertrag&lt;/strong&gt; zu beachten.&lt;/p&gt;&lt;p&gt;(z.B.: Zustimmung des Gesetzlichen Vertreters zu einem Geschäft eines unmündigen Minderjährigen) &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Bedingung?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="ql-align-justify"&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/696" rel="noopener noreferrer" target="_blank" style="color: black;"&gt;§ 696 ABGB&lt;/a&gt;&lt;/p&gt;&lt;p class="ql-align-justify"&gt;&lt;span style="color: black; background-color: lightgrey;"&gt;Eine &lt;/span&gt;&lt;strong style="color: black; background-color: lightgrey;"&gt;Bedingung&lt;/strong&gt;&lt;span style="color: black; background-color: lightgrey;"&gt; ist ein ungewisses Ereignis, von dem ein Recht abhängig gemacht wird.&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine &lt;strong&gt;uneigentliche &lt;/strong&gt;Bedingung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Parteien wissen nicht, ob das Ereignis schon eingetreten ist.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine &lt;strong&gt;eigentliche &lt;/strong&gt;Bedingung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der Eintritt der rechtswirkungen ist von einem &lt;strong&gt;künftigen ungewissen&lt;/strong&gt; Ereignis abhängig.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtsgrundlage für die Wiederholung einer Bedingung? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/899" rel="noopener noreferrer" target="_blank"&gt;§ 899 ABGB&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Potestativbedingung?&lt;/p&gt;&lt;p&gt;Wie wird sie noch genannt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Das vereinbarte Ereignis ist steuerbar oder beinflussbar (z.B.: Vater schenkt Sohn ein Auto, wenn dieser seine Freundin heiratet)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Wollensbedingung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Zufallsbedingung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Das vereinbarte Ereignis ist von den Parteien nicht beeinflussbar oder steuerbar (z.B.: Vater schenkt Sohn ein Auto wenn er im Lotto gewinnt)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was sind die Rechtsfolgen einer auflösenden Bedingung?&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Ähnlichkeit zur Anfechtung?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Eine Auflösende Bedingung vernichtet das Geschäft ex-nunc (&lt;strong&gt;ab &lt;/strong&gt;dem &lt;strong&gt;Eintritt &lt;/strong&gt;der &lt;strong&gt;vereinbarten Bedingung&lt;/strong&gt;) &lt;/li&gt;&lt;li&gt;Ähnlichkeit zur Anfechtung: Vertrag kommt zunächst gültig zustande und Rechtsswirkungen entfalten sich, erst später wird er vernichtet.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Rechtsfolgen einer aufschiebenden Bedingung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Zum Zeitpunkt der Vereinbarung entsteht eine Anwartschaft (&lt;strong&gt;Vorrecht&lt;/strong&gt;) auf die beabsichtigten Leistungen. &lt;/li&gt;&lt;li&gt;Bleibt die Bedingung aus, so wird dieses Vorrecht &lt;strong&gt;ex-tunc &lt;/strong&gt;(Rückwirkend) nichtig. &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie wird ermittelt ob die Parteien aufschiebende oder Auflösende Bedigungen vereinbart haben?&lt;/p&gt;&lt;p&gt;Kann die Art der Bedingungen für die einzelnen Parteien unterschiedlich sein?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Im Einzelfall durch Auslegung der Willenserklärungen zu ermitteln.&lt;/li&gt;&lt;li&gt;Art kann für die Parteien unterschiedlich sein, z.B.: bei Eigentumsvorbehalt (Auto gehört mir erst bei völliger Bezahlung. D.h.: Für Käufer ist es aufschiebende Bedingung, für Verkäufer auflösend [er "verliert" das Auto bei völliger Bezahlung durch den Käufer])&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine auflösende Bedingung?&lt;/p&gt;&lt;p&gt;Wie wird sie noch genannt?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/696" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: black;"&gt;§ 696 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Tritt sofort in Kraft, tritt jedoch in dem Moment &lt;strong&gt;außer Kraft&lt;/strong&gt;, in dem das ungewisse &lt;strong&gt;Ereignis eintritt.&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Resolutivbedingung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine aufschiebende Bedingung?&lt;/p&gt;&lt;p&gt;Wie wird sie noch genannt?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/696" rel="noopener noreferrer" target="_blank" style="color: black; background-color: rgb(40, 45, 88);"&gt;§ 696 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Tritt erst in jenem Augenblick &lt;strong&gt;in Kraft&lt;/strong&gt;, in welchem das ungewisse &lt;strong&gt;Ereignis eintritt.&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Suspensivbedigungung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Geschäftsirrtum?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ein &lt;strong&gt;Motiv &lt;/strong&gt;wurde zum &lt;strong&gt;Vertragsinhalt &lt;/strong&gt;oder sogar zur &lt;strong&gt;Bedigung&lt;/strong&gt; (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/901" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 901 ABGB&lt;/a&gt;), daher kann der Vertrag wegen Geschäftsirrtum &lt;strong&gt;angefochten &lt;/strong&gt;oder &lt;strong&gt;angepasst &lt;/strong&gt;werden.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Rechtsfolgen von einseitigen Irrtümern über Motive?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Da von der Unbeachtlichkeit von Motiven auszugehen ist, gibt es keine Rechtsfolgen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sind Motive beim Vertragsabschluss grundsätzlich zu beachten?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage für die Ausnahme?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Grundsätzlich ist von der Unbeachtlichkeit auszugehen.&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/901" rel="noopener noreferrer" target="_blank"&gt;§ 901 ABGB&lt;/a&gt; ist die Ausnahme (Motiv wird ausdrücklich zur Bedingung gemacht)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Zweifelsregel?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/915" rel="noopener noreferrer" target="_blank" style="background-color: yellow; color: black;"&gt;§ 915 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Bei entgeltlichen Rechtsgeschäften ist eine undeutliche Äußerung im Zweifel zum Nachteil desjenigen zu verstehen, der sich ihrer bedient hat.&lt;/li&gt;&lt;li&gt;Lässt sich kein eindeutiger Sinn ermitteln, so ist die Aussage wegen unbestimmtheit nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/869" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(115, 133, 197);"&gt;§ 869 ABGB&lt;/a&gt; ungütlig.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie kann ein auslegungsbedürftiger Vertrag mit der &lt;strong&gt;einfachen Vertragsinterpretation &lt;/strong&gt;ausgelegt werden?&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Unter Rückgriff auf:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;den &lt;strong&gt;subjektiven Willen der Parteien&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;den &lt;strong&gt;Objektiven Wortlaut der Erklärung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;sowie die &lt;strong&gt;Übung des redlichen Verkehrs&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
+    <t>&lt;p&gt;Welche 3 Quellen für Vertragsvereinbarungen gibt es?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;essentiala negotii&lt;/strong&gt; durch Parteieinigung&lt;/li&gt;&lt;li&gt;&lt;strong&gt;naturalia negotii&lt;/strong&gt; fügt das Gesetz hinzu&lt;/li&gt;&lt;li&gt;&lt;strong&gt;accidentalia negotii&lt;/strong&gt; können die Parteien weiters vereinbaren&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Was ist die Folge von &lt;strong&gt;verstecktem &lt;/strong&gt;Dissens über die Nebenpunkte?&lt;/p&gt;&lt;p&gt;Wie wird gegebenenfalls eine derart entstandene Lücke gefüllt?&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;Es kommt drauf an, ob angenommen werden kann, dass der &lt;strong&gt;Vertrag auch ohne Einigung&lt;/strong&gt; über die &lt;strong&gt;offenen Nebepunkte geschlossen &lt;/strong&gt;worden wäre.&lt;/li&gt;&lt;li&gt;Dies ist idR der Fall, wenn die Nebenpunkte durch &lt;strong&gt;Gesetz oder Verkehrssitte&lt;/strong&gt; ergänzbar sind, und von den Parteien kein Vorbehalt diesbezüglich gemacht wurde.&lt;/li&gt;&lt;li&gt;Diese Lücke wird mittels &lt;strong&gt;dispositivem Recht&lt;/strong&gt; oder &lt;strong&gt;ergänzender Vertragsauslegung &lt;/strong&gt;gefüllt.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist die Zweifelsregel?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/915" rel="noopener noreferrer" target="_blank" style="background-color: yellow; color: black;"&gt;§ 915 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Bei entgeltlichen Rechtsgeschäften ist eine undeutliche Äußerung im Zweifel zum Nachteil desjenigen zu verstehen, der sich ihrer bedient hat.&lt;/li&gt;&lt;li&gt;Lässt sich kein eindeutiger Sinn ermitteln, so ist die Aussage wegen unbestimmtheit nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/869" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(115, 133, 197);"&gt;§ 869 ABGB&lt;/a&gt; ungütlig.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was wird höher gewertet, der &lt;strong&gt;erkennbare subjektive Wille&lt;/strong&gt; oder der &lt;strong&gt;objektive Wortlaut&lt;/strong&gt;, und &lt;strong&gt;warum&lt;/strong&gt;? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;Was sind die Folgen?&lt;/p&gt;</t>
   </si>
   <si>
@@ -55,12 +241,6 @@
     <t>&lt;p&gt;Verwendet:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;hypothetischen Parteiwillen&lt;/li&gt;&lt;li&gt;Übung des redlichen Verkehrs&lt;/li&gt;&lt;li&gt;Treu und Glauben&lt;/li&gt;&lt;li&gt;Verkehrsauffassung&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Welche 3 Quellen für Vertragsvereinbarungen gibt es?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;essentiala negotii&lt;/strong&gt; durch Parteeeinigung&lt;/li&gt;&lt;li&gt;&lt;strong&gt;naturalia negotii&lt;/strong&gt; fügt das Gesetz hinzu&lt;/li&gt;&lt;li&gt;&lt;strong&gt;accidentalia negotii&lt;/strong&gt; können die Parteien weiters vereinbaren&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Wie funktioniert die Lückenschließung durch &lt;strong&gt;dispositives Recht&lt;/strong&gt;?&lt;/p&gt;</t>
   </si>
   <si>
@@ -433,12 +613,6 @@
     <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/862" rel="noopener noreferrer" target="_blank"&gt;§ 862 ABGB&lt;/a&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Angebot erlischt nach Geltungsdauer, diese muss eruiert werden:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Vom Erklärenden gesetzt (im Rahmen von &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/902" rel="noopener noreferrer" target="_blank"&gt;§§ 902f ABGB&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Sonst gesetzliche Frist nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/862" rel="noopener noreferrer" target="_blank"&gt;§ 862 S2 ABGB&lt;/a&gt; (inkl Postlauf des Angebots, Überlegungsfrist und Postlauf der Annahme)&lt;/li&gt;&lt;li&gt;Ausnahme &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/862a" rel="noopener noreferrer" target="_blank"&gt;§ 862a ABGB&lt;/a&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Verzögerung der nachweislich rechtzeitig abgesendeten Annahmeerklärung am Postweg (=Übermittlung)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Der Antragsteller kann aber &lt;strong&gt;unverzüglich &lt;/strong&gt;(ohne schuldhaftes Zögern) zurücktreten&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Was sind die 5 Voraussetzungen für Angebotsannahme durch &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Willensbetätigung&lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/864" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 864 ABGB&lt;/a&gt; &lt;/p&gt;&lt;ol&gt;&lt;li&gt;Willenserklärung nicht zu erwarten (Natur des Geschäfts, Verkehrssitte, Verzicht durch Anbieter)&lt;/li&gt;&lt;li&gt;Annahmehandlung: Annehmender Verfügt über die Sache in einer Weise, zu der er nur berechtigt ist, wenn er das Angebot annehmen will (z.B: Versand der bestellten Ware).&lt;/li&gt;&lt;li&gt;Annahmewille (Vertragsabschlusswille)&lt;/li&gt;&lt;li&gt;Rechtzeitigkeit der Annahme: Während der Geltungsdauer des Angebots; Willensbetätigung ist aber &lt;strong&gt;nicht zugangsbedürftig &lt;/strong&gt;-&amp;gt; es zählt Zeitpunkt der Annahmehandlung. &lt;/li&gt;&lt;li&gt;Kein Widerruf der Willensbetätigung: Widerruf der Annahme bis zur Kenntnisnahme des Anbietenden möglich.&lt;/li&gt;&lt;/ol&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was sind Realakte?&lt;/p&gt;</t>
   </si>
   <si>
@@ -646,7 +820,7 @@
     <t>&lt;p&gt;Was ist die Empfangstheorie?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Es kommt nicht auf den Zeitpunkt der internen Erklärungsbindung (A denkt sich, er schreibt B) an, auch nicht auf den Zeitpunkt der Äußerung der Erklärung (A schreibt den Brief), und auch nicht auf die Absendung der Erklärung, sondern den Eintritt der Erklärung in die Machtsphäre des Empfängers!&lt;/span&gt;&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Es kommt nicht auf den Zeitpunkt der internen Erklärungsbindung (A denkt sich, er schreibt B) an, auch nicht auf den Zeitpunkt der Äußerung der Erklärung (A schreibt den Brief), und auch nicht auf die Absendung der Erklärung, sondern den Eintritt der Erklärung in die Machtsphäre des Empfängers!&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was sind Empfangsboten?&lt;/p&gt;</t>
@@ -1090,7 +1264,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B115"/>
+  <dimension ref="A1:B144"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -2016,6 +2190,238 @@
         <v>229</v>
       </c>
     </row>
+    <row r="116" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Add Cards for Chapter 1,2 and 4
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
+++ b/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="324">
   <si>
     <t>Question</t>
   </si>
@@ -19,6 +19,30 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;Was ist das Pandektensystem? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Aufteilung des ABGB/Zivilrechts in:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Allgemeinen Teil&lt;/li&gt;&lt;li&gt;Schuldrecht&lt;/li&gt;&lt;li&gt;Sachenrecht&lt;/li&gt;&lt;li&gt;Familienrecht&lt;/li&gt;&lt;li&gt;Erbrecht&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das &lt;strong&gt;Institutionensystem&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Aufteilung des ABGB in die drei Teile (Siehe Inhaltsverzeichnis)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Oblat?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der Erklärungsempfänger&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann erlischt ein Angebot?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/862" rel="noopener noreferrer" target="_blank"&gt;§ 862 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;nach Ablauf der gesetzten oder gesetzlichen Pflicht&lt;/li&gt;&lt;li&gt;bei Ablehnung&lt;/li&gt;&lt;li&gt;Insolvenz des Antragstellers&lt;/li&gt;&lt;li&gt;Tod oder nachträgliche Geschäftsunfähigkeit des Antragstellers oder Erklärungsempfängers, wenn der Wille aus den Umständen hervorgeht&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Welcher Zeitpunkt zählt als Empfangszeitpunkt laut Empfangstheorie wenn z.B.: eine Erklärung in einem Postfach hinterlegt wird?&lt;/p&gt;</t>
   </si>
   <si>
@@ -631,7 +655,7 @@
     <t>&lt;ul&gt;&lt;li&gt;Nur auf Kundgabe von Fakten oder Kenntnissen gerichtet (Quittung, Mitteilung des Kontostantds, ... )&lt;/li&gt;&lt;li&gt;Vorschriften für Rechtsgeschäfte weitgehend auf &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wissenserklärung  angewandt, aber &lt;/span&gt;Angebot/Annahme durch &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wissenserklärung &lt;/span&gt;nicht möglich&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was kann eine stillschweigende/konkludente Willenserklärung sein?&lt;/p&gt;</t>
+    <t>&lt;p&gt;Was kann eine stillschweigende/konkludente Willenserklärung sein?&lt;/p&gt;&lt;p&gt;Kann ein Unterlassen eine Willenserklärung sein? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;Eindeutige Handlung nach Verkehrssitte ohne vernünftigen Grund daran zu zweifeln (z.B.: verzehren des aus dem Korb entnommenen Brots)&lt;/li&gt;&lt;li&gt;passives Unterlassen (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 863 ABGB&lt;/a&gt; ): Schweigen gilt nicht als Zustimmung, außer es besteht eine Redepflicht aus:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gesetz&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Verträgen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Übung des redlichen Verkehrs (z.B.: ständige Geschäftsverbindungen)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;vorvertragliche Aufklärungspflichten&lt;/li&gt;&lt;/ul&gt;</t>
@@ -749,6 +773,90 @@
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;Abschlussfreiheit (ob, wann und mit wem Vertrag geschlossen wird)&lt;/li&gt;&lt;li&gt;Inhaltsfreiheit&lt;/li&gt;&lt;li&gt;Typenfreiheit (neue Vertragstypen zu schaffen)&lt;/li&gt;&lt;li&gt;Beendigungsfreiheit&lt;/li&gt;&lt;li&gt;Änderungsfreiheit&lt;/li&gt;&lt;li&gt;Formfreiheit&lt;/li&gt;&lt;li&gt;Testierfreiheit (ob und wie der Verstorbene letztwillig testiert)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Allgemeine Teil des Zivilrechts?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Summe jener Normen, welche die &lt;strong&gt;Grundbausteine &lt;/strong&gt;der &lt;strong&gt;Privatrechtsordnung &lt;/strong&gt;regeln.&lt;/p&gt;&lt;p&gt;-&amp;gt; Gemeinsame Grundlage aller weiteren Teilgebiete&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche 4 Schritte setzt die Subsumtion vorraus?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Genaue &lt;strong&gt;Erfassung&lt;/strong&gt; des zu beurteilenden &lt;strong&gt;Sachverhalts&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Erhebung der in&lt;strong&gt; Betracht kommenden &lt;/strong&gt;konkreten &lt;strong&gt;Rechtsnormen &lt;/strong&gt;und deren &lt;strong&gt;Tatbeständen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Unterstellen des &lt;strong&gt;Sachverhalts unter&lt;/strong&gt; den &lt;strong&gt;Tatbestand &lt;/strong&gt;der Rechtsnorm&lt;/li&gt;&lt;li&gt;Feststellung der &lt;strong&gt;resultierenden &lt;/strong&gt;abstrakt angeordneten &lt;strong&gt;Rechtsfolgen &lt;/strong&gt;und deren &lt;strong&gt;Übertragung &lt;/strong&gt;auf den konkreten &lt;strong&gt;Sachverhalt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Aus welchen 6 Schritten besteht die Anspruchsprüfung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;Lesen und Erfassen des Sachverhalts&lt;/li&gt;&lt;li&gt;Lesen der Fallfrage&lt;/li&gt;&lt;li&gt;Formulierung des Anspruchs (&lt;strong&gt;wer &lt;/strong&gt;will &lt;strong&gt;was &lt;/strong&gt;von &lt;strong&gt;wem&lt;/strong&gt;, aus welchem &lt;strong&gt;Rechtsgrund&lt;/strong&gt;) &lt;/li&gt;&lt;li&gt;Subsumtion&lt;/li&gt;&lt;li&gt;Rechtsfolgen&lt;/li&gt;&lt;li&gt;Beantwortung der Fallfrage&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Anspruchsprüfung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die rechtliche Begutachtung eines Sachverhalts&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Subsumtion?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der Vorgang, bei dem vom konkreten Rechtsanwender festgestellt wird, ob &lt;strong&gt;ein Sachverhalt dem Tatbestand einer Rechtsnorm entspricht.&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Rechtsfolge?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die von der Rechtsnorm angeordnete Konsequenz, wenn der Tatbestand der Norm erfüllt ist&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Aus welchen 2 Teilen setzt sich eine Rechtsnorm zusammen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Tatbestand und Rechtsfolge&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Sachverhalt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Ein tatsächliches Geschehen, das auf seine rechtliche Relevanz zu untersuchen ist.&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Tatbestand?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Jener Teil einer Rechtsnorm, in dem der Gesetzgeber die Lebenssituation abstrakt umschreibt&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Gesetzgebungstechniken sind bei der Schaffung von Sondergesetzen zu beachten?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Personenbezogene Anknüpfungen (KSchG, UGB)&lt;/li&gt;&lt;li&gt;Vertragstypenbezogene Anknüpfungen (Mietverträge, Verbraucherkreditverträge)&lt;/li&gt;&lt;li&gt;Vorgangsbezogene &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Anknüpfungen (Verkehrsunfall: EKHG, PHG, ... )&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Personen- und Vorgangsbezogene Anknüpfungen (PatVG - Patient leht med. Behandlung ab)&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Erbrecht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Summe jener Normen, welche die &lt;strong&gt;Rechtsfolge von Todes wegen&lt;/strong&gt; regeln.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Familienrecht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Summe jener Normen, welche&lt;strong&gt; familienrechtliche Beziehungen&lt;/strong&gt; regeln.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Sachenrecht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Summe jener Normen, welche sich &lt;strong&gt;mit dinglichen Rechten&lt;/strong&gt; an einer Sache beschäftigen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Schuldrecht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Summe jener &lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Normen, welche &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Schuldverhältnisse &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;regeln.&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;-&amp;gt; Beschäftigt sich mit gesetzlichen und vertraglichen Verpflichtungsgründen&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist ein Rechtsgeschäft?&lt;/p&gt;</t>
@@ -1264,7 +1372,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B144"/>
+  <dimension ref="A1:B162"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -2422,6 +2530,150 @@
         <v>287</v>
       </c>
     </row>
+    <row r="145" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Fix reference to wrong paragraph and typo
- § 842 ABGB -> § 862a ABGB
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
+++ b/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="346">
   <si>
     <t>Question</t>
   </si>
@@ -19,6 +19,12 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;Was ist die historische Interpretation?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Auslegung nach der "klaren Absicht des Gesetzgebers" , also der subjektiven Regelungsabsicht des Gesetzgebers.&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Was ist das Pandektensystem? &lt;/p&gt;</t>
   </si>
   <si>
@@ -37,742 +43,802 @@
     <t>&lt;p&gt;Der Erklärungsempfänger&lt;/p&gt;</t>
   </si>
   <si>
+    <t>&lt;p&gt;Welcher Zeitpunkt zählt als Empfangszeitpunkt laut Empfangstheorie wenn z.B.: eine Erklärung in einem Postfach hinterlegt wird?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der objektiv erste mögliche Zeitpunkt der Kenntnisnahme durch den Empfänger, z.B.: Ankunft des Briefs im Postfach (der Empfänger &lt;strong&gt;könnte&lt;/strong&gt; den Brief abholen), NICHT wenn der Empfänger &lt;strong&gt;tatsächlich&lt;/strong&gt; Abholt.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was sind die 5 Voraussetzungen für Angebotsannahme durch &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Willensbetätigung&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;?&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Rechtsgrundlage?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/864" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 864 ABGB&lt;/a&gt; &lt;/p&gt;&lt;ol&gt;&lt;li&gt;Willenserklärung nicht zu erwarten (Natur des Geschäfts, Verkehrssitte, Verzicht durch Anbieter)&lt;/li&gt;&lt;li&gt;Annahmehandlung: Annehmender Verfügt über die Sache in einer Weise, zu der er nur berechtigt ist, wenn er das Angebot annehmen will (z.B: Versand der bestellten Ware).&lt;/li&gt;&lt;li&gt;Annahmewille (Vertragsabschlusswille)&lt;/li&gt;&lt;li&gt;Rechtzeitigkeit der Annahme: Während der Geltungsdauer des Angebots; Willensbetätigung ist aber &lt;strong&gt;nicht zugangsbedürftig &lt;/strong&gt;-&amp;gt; es zählt Zeitpunkt der Annahmehandlung. &lt;/li&gt;&lt;li&gt;Kein Widerruf der Willensbetätigung: Widerruf der Annahme bis zur Kenntnisnahme des Anbietenden möglich.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Rechtsfolgen der Nichterfüllung einer Bedingung?&lt;/p&gt;&lt;p&gt;Wie muss eine Bedingung erfüllt werden?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Rechtserwerb wird verhindert bzw. Rechtsverlust herbeigeführt.&lt;/li&gt;&lt;li&gt;Muss nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/699" rel="noopener noreferrer" target="_blank"&gt;§ 699 ABGB&lt;/a&gt; &lt;strong&gt;stets genau erfüllt &lt;/strong&gt;werden.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Rechtsfolgen der Nichteinhaltung einer Auflage? &lt;/p&gt;&lt;p&gt;Wie muss eine Auflage erfüllt werden?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Einhaltung kann durch Klage oder Exekution erzwungen werden.&lt;/li&gt;&lt;li&gt;Nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/709" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 709 ABGB&lt;/a&gt; genügt die &lt;strong&gt;annähernde &lt;/strong&gt;Erfüllung, wenn die &lt;strong&gt;genaue&lt;/strong&gt; Erfüllung &lt;strong&gt;nicht möglich &lt;/strong&gt;ist.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Auflage?&lt;/p&gt;&lt;p&gt;Wie ist sie im Zweifel zu behandeln, Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/709" rel="noopener noreferrer" target="_blank"&gt;§ 709 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Die einem Empfänger einer Zuwendung im Zusammenhang mit einer &lt;strong&gt;letztwillligen Verfügung&lt;/strong&gt; oder einem &lt;strong&gt;unentgeltlichen Rechtsgeschäft unter Lebenden&lt;/strong&gt; auferlegte &lt;strong&gt;Verpflichtung &lt;/strong&gt;zur &lt;strong&gt;Vornahme eines bestimmten Verhaltens&lt;/strong&gt; bei &lt;strong&gt;sonstigem Verlust der Zuwendung&lt;/strong&gt;, wobei es unerheblich ist, in wessen Interesse das geforderte Verhalten ist.&lt;/li&gt;&lt;li&gt;Im zweifel als auflösende Bedingung nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/10" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 710 ABGB&lt;/a&gt; &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie werden Samstage, Sonntage und gesetzliche Feiertage bei Fristen gehandhabt?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Zählen in die Berechnung der Frist&lt;/li&gt;&lt;li&gt;Ist der letzte Tag der Frist ein Sa, So oder gesetzl. Feiertag, so läuft die Frist mit&lt;strong&gt; Ende des nächstfolgenden Werktages ab&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/903" rel="noopener noreferrer" target="_blank"&gt;§ 903 S3 ABGB&lt;/a&gt;, &lt;a href="https://www.ris.bka.gv.at/GeltendeFassung.wxe?Abfrage=Bundesnormen&amp;amp;Gesetzesnummer=10000765" rel="noopener noreferrer" target="_blank"&gt;Art. 5 EuFrÜb&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Rechtsgrundlagen für Fristen sind heranzuziehen, wenn weder Sondergesetze noch Parteien anders vereinbaren?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/902" rel="noopener noreferrer" target="_blank"&gt;§§ 902-904 ABGB&lt;/a&gt; und EuFrÜb (Europäisches Übereinkommen über die Berechnung von Frist)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Befristung?&lt;/p&gt;&lt;p&gt;Was ist der Unterschied zur Bedingung? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Eine von den &lt;strong&gt;Parteien gesetzte Beschränkung&lt;/strong&gt; des Rechtsgeschäftes, bei der &lt;strong&gt;Inkrafttreten&lt;/strong&gt; oder &lt;strong&gt;Außerkrafttreten &lt;/strong&gt;der Rechtswirkung entweder &lt;strong&gt;kalendrisch bestimmt&lt;/strong&gt;, oder von einem &lt;strong&gt;sicher eintretenden Ereignis&lt;/strong&gt; abhängig gemacht wird.&lt;/li&gt;&lt;li&gt;Unterschied: Bedingung hat ein ungewisses Ereignis.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Beispiel 1: "Wenn A stirbt ..." ist eine Befristung, aufgrund der Gewissheit des Eintretens.&lt;/p&gt;&lt;p&gt;Beispiel 2: "Sollte A das 90. Lebensjahr erreichen ... " ist eine Bedingung, weil Ungewiss.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Termin?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ein rechtlich erheblicher Zeitpunkt&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Frist?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Eine rechtlich erhebliche Zeitspanne&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Beeinflussing wider Treu und Glauben? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gelingt es jemandem, dem die Bedingung zum &lt;strong&gt;Nachteil &lt;/strong&gt;gereicht, sie zu &lt;strong&gt;vereiteln&lt;/strong&gt;, gilt die Bedingung als &lt;strong&gt;eingetreten&lt;/strong&gt;. &lt;/li&gt;&lt;li&gt;Gelingt es jemandem, dem die Bedingung zum &lt;strong&gt;Vorteil &lt;/strong&gt;gereicht, die Bedingung wider Treu und Glauben &lt;strong&gt;herbeizuführen&lt;/strong&gt;, gilt die Bedingung als &lt;strong&gt;ausgefallen&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Beispiel: X verspricht Y ihm sein Auto zu schenken, wenn die nächste Reperatur ansteht. Y sapotiert das Auto von X. Die Bedingung wurde wider Treu und Glauben herbeigeführt und gilt daher als ausgefallen und die Schenkung tritt nicht in kraft.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtsgrundlage für unmögliche aufschiebende und unmögliche auflösende Bedingungen? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/698" rel="noopener noreferrer" target="_blank" style="color: black; background-color: rgb(40, 45, 88);"&gt;§ 698 ABGB&lt;/a&gt;, für letzten Willen auch &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/898" rel="noopener noreferrer" target="_blank"&gt;§ 898 ABGB&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann ist eine Bedingung unmöglich?&lt;/p&gt;&lt;p&gt;Was ist unmöglich allgemein definiert?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Eine Bedingung ist &lt;strong&gt;unmöglich&lt;/strong&gt;, wenn sie aus &lt;strong&gt;tatsächlichen&lt;/strong&gt; oder &lt;strong&gt;rechtlichen Gründen &lt;/strong&gt;nicht eintreten kann.&lt;/li&gt;&lt;li&gt;Unmöglich ist, was &lt;strong&gt;objektiv gesehen&lt;/strong&gt; und &lt;strong&gt;nicht &lt;/strong&gt;nur &lt;strong&gt;vorrübergehend &lt;/strong&gt;sondern &lt;strong&gt;dauerhaft&lt;/strong&gt; &lt;strong&gt;unmöglich&lt;/strong&gt; ist und niemand erfüllen kann.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Bedingungen gelten nicht?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/697" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: black;"&gt;§ 697 ABGB&lt;/a&gt;&lt;/p&gt;&lt;p&gt;Unverständliche, unbestimmte, sowie gesetz- oder sittenwidrige Bestimmungen&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind bejahende (positive) Bedingungen?&lt;/p&gt;&lt;p&gt;Was sind verneinende (negative) Bedingungen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Positive&lt;/strong&gt;: wenn du deine Freundin heiratest, bekommst du ein Auto &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Negative&lt;/strong&gt;: Wenn du nicht rauchst, bekommst du ein Auto&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sind Rechtsbedingungen Bedingungen im Sinne von &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/696" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: black;"&gt;§ 696 ABGB&lt;/a&gt;? Warum schon/warum nicht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nein, sie sind gesetzliche Vorraussetzungen und daher &lt;strong&gt;unabhängig von der Aufnahme in den Vertrag&lt;/strong&gt; zu beachten.&lt;/p&gt;&lt;p&gt;(z.B.: Zustimmung des Gesetzlichen Vertreters zu einem Geschäft eines unmündigen Minderjährigen) &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Bedingung?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="ql-align-justify"&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/696" rel="noopener noreferrer" target="_blank" style="color: black;"&gt;§ 696 ABGB&lt;/a&gt;&lt;/p&gt;&lt;p class="ql-align-justify"&gt;&lt;span style="color: black; background-color: lightgrey;"&gt;Eine &lt;/span&gt;&lt;strong style="color: black; background-color: lightgrey;"&gt;Bedingung&lt;/strong&gt;&lt;span style="color: black; background-color: lightgrey;"&gt; ist ein ungewisses Ereignis, von dem ein Recht abhängig gemacht wird.&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine &lt;strong&gt;uneigentliche &lt;/strong&gt;Bedingung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Parteien wissen nicht, ob das Ereignis schon eingetreten ist.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine &lt;strong&gt;eigentliche &lt;/strong&gt;Bedingung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der Eintritt der rechtswirkungen ist von einem &lt;strong&gt;künftigen ungewissen&lt;/strong&gt; Ereignis abhängig.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtsgrundlage für die Wiederholung einer Bedingung? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/899" rel="noopener noreferrer" target="_blank"&gt;§ 899 ABGB&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Potestativbedingung?&lt;/p&gt;&lt;p&gt;Wie wird sie noch genannt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Das vereinbarte Ereignis ist steuerbar oder beinflussbar (z.B.: Vater schenkt Sohn ein Auto, wenn dieser seine Freundin heiratet)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Wollensbedingung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Zufallsbedingung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Das vereinbarte Ereignis ist von den Parteien nicht beeinflussbar oder steuerbar (z.B.: Vater schenkt Sohn ein Auto wenn er im Lotto gewinnt)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was sind die Rechtsfolgen einer auflösenden Bedingung?&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Ähnlichkeit zur Anfechtung?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Eine Auflösende Bedingung vernichtet das Geschäft ex-nunc (&lt;strong&gt;ab &lt;/strong&gt;dem &lt;strong&gt;Eintritt &lt;/strong&gt;der &lt;strong&gt;vereinbarten Bedingung&lt;/strong&gt;)&lt;/li&gt;&lt;li&gt;Ähnlichkeit zur Anfechtung: Vertrag kommt zunächst gültig zustande und Rechtswirkungen entfalten sich, erst später wird er vernichtet.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Rechtsfolgen einer aufschiebenden Bedingung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Zum Zeitpunkt der Vereinbarung entsteht eine Anwartschaft (&lt;strong&gt;Vorrecht&lt;/strong&gt;) auf die beabsichtigten Leistungen. &lt;/li&gt;&lt;li&gt;Bleibt die Bedingung aus, so wird dieses Vorrecht &lt;strong&gt;ex-tunc &lt;/strong&gt;(Rückwirkend) nichtig. &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie wird ermittelt ob die Parteien aufschiebende oder Auflösende Bedigungen vereinbart haben?&lt;/p&gt;&lt;p&gt;Kann die Art der Bedingungen für die einzelnen Parteien unterschiedlich sein?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Im Einzelfall durch Auslegung der Willenserklärungen zu ermitteln.&lt;/li&gt;&lt;li&gt;Art kann für die Parteien unterschiedlich sein, z.B.: bei Eigentumsvorbehalt (Auto gehört mir erst bei völliger Bezahlung. D.h.: Für Käufer ist es aufschiebende Bedingung, für Verkäufer auflösend [er "verliert" das Auto bei völliger Bezahlung durch den Käufer])&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine auflösende Bedingung?&lt;/p&gt;&lt;p&gt;Wie wird sie noch genannt?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/696" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: black;"&gt;§ 696 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Tritt sofort in Kraft, tritt jedoch in dem Moment &lt;strong&gt;außer Kraft&lt;/strong&gt;, in dem das ungewisse &lt;strong&gt;Ereignis eintritt.&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Resolutivbedingung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine aufschiebende Bedingung?&lt;/p&gt;&lt;p&gt;Wie wird sie noch genannt?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/696" rel="noopener noreferrer" target="_blank" style="color: black; background-color: rgb(40, 45, 88);"&gt;§ 696 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Tritt erst in jenem Augenblick &lt;strong&gt;in Kraft&lt;/strong&gt;, in welchem das ungewisse &lt;strong&gt;Ereignis eintritt.&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Suspensivbedigungung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Geschäftsirrtum?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ein &lt;strong&gt;Motiv &lt;/strong&gt;wurde zum &lt;strong&gt;Vertragsinhalt &lt;/strong&gt;oder sogar zur &lt;strong&gt;Bedigung&lt;/strong&gt; (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/901" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 901 ABGB&lt;/a&gt;), daher kann der Vertrag wegen Geschäftsirrtum &lt;strong&gt;angefochten &lt;/strong&gt;oder &lt;strong&gt;angepasst &lt;/strong&gt;werden.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Rechtsfolgen von einseitigen Irrtümern über Motive?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Da von der Unbeachtlichkeit von Motiven auszugehen ist, gibt es keine Rechtsfolgen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sind Motive beim Vertragsabschluss grundsätzlich zu beachten?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage für die Ausnahme?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Grundsätzlich ist von der Unbeachtlichkeit auszugehen.&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/901" rel="noopener noreferrer" target="_blank"&gt;§ 901 ABGB&lt;/a&gt; ist die Ausnahme (Motiv wird ausdrücklich zur Bedingung gemacht)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Zweifelsregel?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/915" rel="noopener noreferrer" target="_blank" style="background-color: yellow; color: black;"&gt;§ 915 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Bei entgeltlichen Rechtsgeschäften ist eine undeutliche Äußerung im Zweifel zum Nachteil desjenigen zu verstehen, der sich ihrer bedient hat.&lt;/li&gt;&lt;li&gt;Lässt sich kein eindeutiger Sinn ermitteln, so ist die Aussage wegen unbestimmtheit nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/869" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(115, 133, 197);"&gt;§ 869 ABGB&lt;/a&gt; ungütlig.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie kann ein auslegungsbedürftiger Vertrag mit der &lt;strong&gt;einfachen Vertragsinterpretation &lt;/strong&gt;ausgelegt werden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Unter Rückgriff auf:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;den &lt;strong&gt;subjektiven Willen der Parteien&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;den &lt;strong&gt;Objektiven Wortlaut der Erklärung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;sowie die &lt;strong&gt;Übung des redlichen Verkehrs&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche 3 Quellen für Vertragsvereinbarungen gibt es?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;essentiala negotii&lt;/strong&gt; durch Parteieinigung&lt;/li&gt;&lt;li&gt;&lt;strong&gt;naturalia negotii&lt;/strong&gt; fügt das Gesetz hinzu&lt;/li&gt;&lt;li&gt;&lt;strong&gt;accidentalia negotii&lt;/strong&gt; können die Parteien weiters vereinbaren&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Folge von &lt;strong&gt;verstecktem &lt;/strong&gt;Dissens über die Nebenpunkte?&lt;/p&gt;&lt;p&gt;Wie wird gegebenenfalls eine derart entstandene Lücke gefüllt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Es kommt drauf an, ob angenommen werden kann, dass der &lt;strong&gt;Vertrag auch ohne Einigung&lt;/strong&gt; über die &lt;strong&gt;offenen Nebepunkte geschlossen &lt;/strong&gt;worden wäre.&lt;/li&gt;&lt;li&gt;Dies ist idR der Fall, wenn die Nebenpunkte durch &lt;strong&gt;Gesetz oder Verkehrssitte&lt;/strong&gt; ergänzbar sind, und von den Parteien kein Vorbehalt diesbezüglich gemacht wurde.&lt;/li&gt;&lt;li&gt;Diese Lücke wird mittels &lt;strong&gt;dispositivem Recht&lt;/strong&gt; oder &lt;strong&gt;ergänzender Vertragsauslegung &lt;/strong&gt;gefüllt.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was wird höher gewertet, der &lt;strong&gt;erkennbare subjektive Wille&lt;/strong&gt; oder der &lt;strong&gt;objektive Wortlaut&lt;/strong&gt;, und &lt;strong&gt;warum&lt;/strong&gt;? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;Was sind die Folgen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/914" rel="noopener noreferrer" target="_blank" style="background-color: yellow; color: black;"&gt;§§ 914f ABGB&lt;/a&gt; iVm &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank"&gt;§ 863 ABGB&lt;/a&gt; &lt;/p&gt;&lt;ul&gt;&lt;li&gt;Der erkennbare Subjektive Wille: Es ist die erkennbare Absicht der Parteien zu erforschen, Der Erklärungsempfänger hat den im objektiven Erklärungswert zum Ausdruck kommenden &lt;strong&gt;wahren subjektiven Willen&lt;/strong&gt; zu ermitteln.&lt;/li&gt;&lt;li&gt;Folge: Bei Verträgen gilt primär der übereinstimmende wahre Wille der Parteien, selbst wenn der Wortlaut davon abweicht. &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der hypothetische Parteiwillen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Das, was die &lt;strong&gt;konkreten &lt;/strong&gt;Parteien &lt;strong&gt;vernünftigerweise&lt;/strong&gt; &lt;strong&gt;gewollt&lt;/strong&gt; &lt;strong&gt;hätten&lt;/strong&gt;, wenn ihnen die &lt;strong&gt;Unvollständigkeit &lt;/strong&gt;des &lt;strong&gt;Vertrages bewusst &lt;/strong&gt;gewesen wäre.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wie funktioniert die Lückenschließung durch &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;ergänzende Vertragsauslegung&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Verwendet:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;hypothetischen Parteiwillen&lt;/li&gt;&lt;li&gt;Übung des redlichen Verkehrs&lt;/li&gt;&lt;li&gt;Treu und Glauben&lt;/li&gt;&lt;li&gt;Verkehrsauffassung&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie funktioniert die Lückenschließung durch &lt;strong&gt;dispositives Recht&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Lücken sind durch &lt;strong&gt;gesetzliche Vorschriften&lt;/strong&gt; zu ergänzen&lt;/p&gt;&lt;ul&gt;&lt;li class="ql-indent-1"&gt;Außer es steht fest, dass die Parteien die Geltung des dispositiven Rechts &lt;strong&gt;nicht herbeiführen&lt;/strong&gt; wollten und &lt;strong&gt;dennoch keine Regelung&lt;/strong&gt; getroffen haben&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Einfluss der &lt;strong&gt;Übung des redlichen Verkehrs&lt;/strong&gt; auf den objektiven Wortlaut?&lt;/p&gt;&lt;p&gt;Welche Elemente sind zu beachten?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ist die Erklärung nicht eindeutig, so ist sie vom Empfänger entsprechend der &lt;strong&gt;Verkehrssitte&lt;/strong&gt;, also der Übung des redlichen Verkehrs zu verstehen.&lt;/li&gt;&lt;li&gt;Beachten:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Sprachgebrauch&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Art&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ort (z.B.: ortstypischer Dialekt)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Umstände (Verkehrskreis, Verbraucher, Unternehmer, ... )&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Rechtsgrundlage für die Auslegungsregeln für Verträge?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="ql-align-justify"&gt;&lt;span style="color: black; background-color: yellow;"&gt;§§ &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank" style="color: black; background-color: yellow;"&gt;863 Abs 2&lt;/a&gt;&lt;span style="color: black; background-color: yellow;"&gt;, &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/914" rel="noopener noreferrer" target="_blank" style="color: black; background-color: yellow;"&gt;914&lt;/a&gt;&lt;span style="color: black; background-color: yellow;"&gt;, &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/915" rel="noopener noreferrer" target="_blank" style="color: black; background-color: yellow;"&gt;915&lt;/a&gt;&lt;span style="color: black; background-color: yellow;"&gt; ABGB&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/ugb/paragraf/346" rel="noopener noreferrer" target="_blank" style="color: black; background-color: yellow;"&gt;§ 346 UGB&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann darf eine zurechenbare Willenserklärung nicht angenommen werden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wenn für den Empfänger zwar ein Vertrauenstatbestand vorlag, aber der Empfänger auf diese Handlung &lt;strong&gt;nicht vertraut&lt;/strong&gt; hat.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist &lt;strong&gt;fehlende Erklärungsbewusstsein&lt;/strong&gt; des Erklärenden?&lt;/p&gt;&lt;p&gt;Wann sind Erklärungen dennoch Zurechenbar?&lt;/p&gt;&lt;p&gt;Was hätte der Erklärende in dem Fall verhindern müssen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Unbewusst abgegebene Erklärungen&lt;/li&gt;&lt;li&gt;Nur dann zurechenbar, wenn sich der Erklärende fahrlässig verhalten hat &lt;/li&gt;&lt;li&gt;Verhindern, dass diese Erklärungen/Handlungen vom &lt;strong&gt;gutgläubigen Dritten&lt;/strong&gt; als &lt;strong&gt;Willenserklärungen angesehen &lt;/strong&gt;werden &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(&lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(226, 148, 20);"&gt;Erklärungsfahrlässigkeit&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein objektiv-redlicher Erklärungsempfänger?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wer sich bemüht, richtig zu verstehen, was der Erklärende ausdrücken möchte&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Bedeutungen der &lt;strong&gt;Willenstheorie&lt;/strong&gt;, &lt;strong&gt;Erklärungstheorie &lt;/strong&gt;und &lt;strong&gt;Vertrauenstheorie&lt;/strong&gt;, was ist bei der Erklärung Maßgebend?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Willenstheorie&lt;/strong&gt;: Wille des Erklärenden&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erklärungstheorie&lt;/strong&gt;: objektiver Wortlaut der Erklärung&lt;/li&gt;&lt;li&gt;Maßgebend: &lt;strong&gt;Vertrauenstheorie &lt;/strong&gt;(Abgeleitet von &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank"&gt;§ 863 ABGB)&lt;/a&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Die Erklärung aus der Sicht eines &lt;strong&gt;objektiv-redlichen Erklärungsempfängers&lt;/strong&gt;, alle Kenntnisse des wirklichen Empfängers, auch ungewöhnliche, inklusive. &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Worum geht es bei der Interpretation von Erklärungen und Verträgen?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Um die Ermittlung des Inhalts einer einzelnen Vertragsabschlusserklärung&lt;/li&gt;&lt;li&gt;Um die Ermittlung des Vertragsinhalts&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Folge von Dissens über Hauptpunkte?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;Ist es relevant ob offener oder versteckter Dissens?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/869" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 869 S2 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Kein Vertrag kommt zustande.&lt;/li&gt;&lt;li&gt;Unabhängig ob offener oder versteckter Dissens&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche 3 Arten des Dissens gibt es?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/869" rel="noopener noreferrer" target="_blank"&gt;§ 869 S2 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Dissens wegen Unvollständigkeit der Vereinbarung:&lt;/strong&gt; z.B.: Haupt oder Nebenpunkte sind offen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Dissens wegen Diskrepanz der Erklärungen&lt;/strong&gt;: Angebot- und Annahmeerklärung stimmen im Wortlaut nicht überein, und können auch durch Auslegung nicht zur Deckung gebracht werden&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Dissens wegen Mehrdeutigkeit oder Unverständlichkeit der Erklärungen&lt;/strong&gt;: Angebot und Annahme stimmen zwar im Wortlaut überein, sind aber objektiv mehrdeutig und werden von den Parteien unterschiedlich verstanden.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist &lt;strong&gt;versteckter &lt;/strong&gt;Dissens?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Zumindest eine Partei glaubt, dass in allen Punkten einigung erzielt wurde&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist &lt;strong&gt;offener &lt;/strong&gt;Dissens?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Beide Parteien wissen, dass sie sich noch nicht einig sind&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was kann (offener und versteckter) Dissens betreffen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Haupt- oder Nebenpunkte im Vertrag&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Kann es Erklärungsirrtum bei natürlichem Konsens geben?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nein, der Vertragsinhalt besteht nur aus dem subjektiven Willen beider Parteien (es gibt keinen objektiven Erklärungswert der abweichen könnte)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was wird höher bewertet, übereinstimmender subjektiver Wille, oder übereinstimmender objektiver Erklärungswert?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der übereinstimmende Subjektive Wille, der objektive Erklärungswert kann nämliich irrtümlich vom subjektiven Willen des Anbieters abweichen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Abgrenzung zwischen Konsens, Dissens und Erklärungsirrtum?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Konsens&lt;/strong&gt;: subjektiver Wille (der Parteien) oder objektiver Erklärungswert (der Erkärungen) stimmt überein.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Dissens&lt;/strong&gt;: Weder subjektiver Wille noch objektiver Erklärungswert stimmen überein&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erklärungsirrtum&lt;/strong&gt;: Der subjektive Wille einer Partei weicht vom objektiven Erklärungswert ab.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der objektive Erklärungswert? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der in den Vertrag eingesetzte Wert (z.B.: Preis), kann &lt;strong&gt;irrtümlich&lt;/strong&gt; vom subjektiven Willen des Anbieters abweichen&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der normative Konsens?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der Erklärungsempfänger vertraut auf den &lt;strong&gt;objektiven Erklärungswert&lt;/strong&gt;, aber der Vertragsinhalt entspricht nicht dem subjektiven Willen der anderen Partei (-&amp;gt; &lt;strong&gt;Fehler bei Angebotslegung&lt;/strong&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der natürliche Konsens?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der innere Wille beider Parteien stimmt überein&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Inhaltskontrolle der AGB?&lt;/p&gt;&lt;p&gt;Was sind die drei Ebenen und deren Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Soll den Kunden vor überschießenden AGB Schützen -&amp;gt; die Unterlegenheit des Kunden ausgleichen. Diese zivilrechtliche Kontrolle wird durch eine vorhergehende aufsichtsbehördliche Genehmigung oder Kontrolle &lt;strong&gt;nicht &lt;/strong&gt;ausgeschlossen.&lt;/li&gt;&lt;li&gt;3 Ebenen:&lt;/li&gt;&lt;/ul&gt;&lt;ol&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Einbeziehungskontrolle&lt;/strong&gt;: Prüfung ob die AGB in ihrer Gesamtheit von den Parteien erhoben wurde (Parteieneinigung, z.B.: Unterschriften)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Geltungskontrolle&lt;/strong&gt;: Alle Einzelbestimmungen der AGB, die tatsächlich Vertragsinhalt geworden sind, werden der Geltungskontrolle unterzogen (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/864a" rel="noopener noreferrer" target="_blank"&gt;§ 864a ABGB&lt;/a&gt;). &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Inhaltskontrolle&lt;/strong&gt;: Verbleibende Klauseln (Kein Verstoß gegen &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/879" rel="noopener noreferrer" target="_blank"&gt;§ 879 Abs 3 &lt;/a&gt;und &lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/6" rel="noopener noreferrer" target="_blank"&gt;§ 6 KSchG&lt;/a&gt;)&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Einbeziehungskontrolle: Was ist für die Geltung von AGB erforderlich/für den Abschluss?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Soweit nicht durch Gesetz oder Verordnung anders angeordnet, gelten AGB nur kraft &lt;strong&gt;ausdrücklicher oder konkludenter Vereinbarung &lt;/strong&gt;der Parteien (Willenseinigung &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/861" rel="noopener noreferrer" target="_blank"&gt;§ 861 ABGB&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Geltungskontrolle: Was sind die Rechtsfolgen eines Verstoßes einer Klausel gegen § 864a ABGB?&lt;/p&gt;&lt;p&gt;Wann wird die Unwirksamkeit von Amts wegen geprüft, wann nur auf Einwand (des Unterworfenen)?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Klausel ist nicht Vertragsbestandteil&lt;/li&gt;&lt;li&gt;Der Restvertrag gilt &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(&lt;/span&gt;&lt;strong style="color: rgb(226, 148, 20); background-color: rgb(40, 45, 88);"&gt;Restgültigkeit des Vertrags&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;)&lt;/span&gt;, nur die Klausel selbst ist nichtig.&lt;/li&gt;&lt;li&gt;Erscheint die Klausel nach dem Verfahrensstadiums des Zivilprozesses &lt;strong&gt;nicht offenkundig&lt;/strong&gt; bedenklich, so wird die Unwirksamkeit nicht amtswegig sondern nur bei darauf gerichteter Einwendung geprüft.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie funktioniert die Geltungskontrolle der AGBs?&lt;/p&gt;&lt;p&gt;Welche 4 Tatbestandselemente sind notwendig?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;Jede konkrete Einzelklausel der AGB wird betrachtet&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;4 &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;kumulative &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;Tatbestandselemente für &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/864a" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 864a ABGB&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;:&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bestimmung ungewöhnlichen Inhalts&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nachteiligkeit für den Partner des Aufstellers&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Überraschungseffekt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Kein besonderer Hinweis des Aufstelleres auf die ungewöhnliche Klausel&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Inhaltskontrolle: Nichtigkeit gemäß &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/879" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 879 Abs 3&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;:&lt;/span&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Was sind die zwei Voraussetzungen?&lt;/li&gt;&lt;li&gt;Was ist die Rechtsfolge?&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Voraussetzungen: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Keine Hauptleistung (= Nebenbestimmungen)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gröbliche &lt;/strong&gt;Benachteiligung des Unterworfenen:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Bloße Benachteiligung reicht nicht aus.&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Gröblich z.B.: Verdünnte Willensfreiheit, oder AGB weichen von Wertung des objektiven dispositiven Rechts stark ab.&lt;/li&gt;&lt;li&gt;Klausel nicht Vertragsbestandteil, also nichtig.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Restvertrag gilt (&lt;strong&gt;Restgültigkeit des Vertrags&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Relative Nichtigkeit einer Klausel ist nur auf Einwendung wahrzunehmen.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Entgeltliche/Unentgeltliche/Entgeltfremde Rechtsgeschäfte?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage für Entgeltliche Rechtsgeschäfte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;entgeltlich&lt;/strong&gt;: immer Zweiseitig, jede Partei bringt die eigene Leistung um die Gegenleistung zu erhalten (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/917" rel="noopener noreferrer" target="_blank"&gt;§ 917 ABGB&lt;/a&gt;). Leistung muss nicht Geld sein.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;unentgeltlich&lt;/strong&gt;: Ein Partner erhält keine Gegenleistung (Schenkungsvertrag)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;entgeltsfremd&lt;/strong&gt;: liegen vor, wenn ein Bürge nachträglich einem existierenden Darlehensvertrag beitritt, ohne dass sich die Konditionen für den Hauptschuldner ändern.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie verhalten sich Individualvereinbarungen zu den AGB?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Spezielle Individualvereinbarungen, selbst mündliche, verdrängen die AGB.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie funktionieren die 3 Ebenen der Inhaltskontrolle in der Übersicht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;Scheitern AGB an Einbeziehungskontrolle -&amp;gt; &lt;strong&gt;Bedingungswerk &lt;/strong&gt;(gesamte AGB) wird nicht Teil des Vertrags &lt;/li&gt;&lt;li&gt;Scheitern einzelne Bestimmungen an der Geltungskontrolle, so sind nur diese Bestimmungen nichtig&lt;/li&gt;&lt;li&gt;Scheitern einzelne Bestimmungen an der Inhaltskontrolle, so sind nur diese nichtig&lt;/li&gt;&lt;li&gt;Alle übrigen Bestimmungen bleiben Vertragsinhalt.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Inhaltskontrolle: Wie kann die Nichtigkeit von AGB für Verbraucher durchgesetzt werden? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;strong&gt;Einzelprozess &lt;/strong&gt;(Auch ohne Vorbringen des Verbrauchers)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verbandsklage &lt;/strong&gt;von den Interessenverbänden &lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/28" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§§ 28-29 KSchG&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Abmahnung &lt;/strong&gt;-&amp;gt; Konventionalstrafe (&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/28" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 28 Abs 2 KSchG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Überschießende Klauseln &lt;/strong&gt;in AGB: Bei Verstoß gegen &lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/6" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 6 Abs 1 und 2 KSchG&lt;/a&gt; wird von der Fortgeltung der Klauseln ausgegangen, wenn sie (für den Konsumenten) vorteilhafte Bestimmungen enthalten.&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Inhaltskontrolle: Wie wird das Transparenzgebot &lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/6" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 6 Abs 3 KSchG&lt;/a&gt; verstanden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Vertragsbestimmungen müssen den Verbraucher zuverlässig über seine Rechte und Pflichten informieren. Er soll möglichst &lt;strong&gt;durchschaubar, klar verständlich&lt;/strong&gt; und &lt;strong&gt;angepasst &lt;/strong&gt;an die Vertragsart so aufgeklärt werden, dass er &lt;strong&gt;nicht &lt;/strong&gt;von der &lt;strong&gt;Durchsetzung seiner Rechte abgehalten &lt;/strong&gt;wird, und ihm auch &lt;strong&gt;keine unberechtigten Pflichten auferlegt&lt;/strong&gt; werden.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Inhaltskontrolle: Abweichungen vom objektiven Recht&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Es wird nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/879" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 879 Abs 3&lt;/a&gt; &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;und &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/6" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 6 KSchG&lt;/a&gt; geprüft, ob Klauseln sachlich&lt;strong&gt; nicht gerechtfertigte unangemessene Abweichungen vom objektiven Recht&lt;/strong&gt; zulasten des unterworfenen enthalten.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Geltungskontrolle: Was ist der Überraschungseffekt (Überrumpelungs- bzw. Übertölpelungseffekt)&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Versteckte Klauseln die für den Unterworfenen überraschend sind.&lt;/li&gt;&lt;li&gt;Entfällt wenn diese Klauseln &lt;strong&gt;hervorgehoben &lt;/strong&gt;sind (fett, farbig, unterstrichen, ... ) oder &lt;strong&gt;mündlich &lt;/strong&gt;erklärt werden.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Entscheiden ist, ob dem Leser die ungewöhnliche Bestimmung aus dem Gesamteindruck der Urkunde auffällt.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Geltungskontrolle: Wann ist eine Bestimmung Nachteilig für den Partner des Aufstellers?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Weicht zulasten des Unterworfenen vom dispositiven objektiven Recht ab&lt;/li&gt;&lt;li&gt;Oder Stellt den Unterworfenen im Vergleich zum Aufsteller der AGB schlechter (aus der Sicht eines redlichen Vertragspartners)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Geltungskontrolle: Wie wird ungewöhnlicher Inhalt bestimmt?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Objektiv ungewöhnlich&lt;/strong&gt;: Wenn eine derartige Bestimmung in einem derartigen Vertrag üblicherweise (im redlichen Verkehr) nicht enthalten ist&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Subjektiv ungewöhnlich&lt;/strong&gt;:  Eine objektiv nicht ungewöhnliche Klausel kann subjektiv ungewöhnlich sein, wenn sie für den konkreten Vertragspartner im konkreten Zusammenhang, aus Sicht eines redlichen Aufstellers, überraschend sein musste und der Aufsteller nicht mit der Unterwerfung des Partners rechnen durfte.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Einbeziehungskontrolle: &lt;/span&gt;&lt;/p&gt;&lt;p&gt;Was sind kollidierende oder kreuzende AGB?&lt;/p&gt;&lt;p&gt;Was sind die Folgen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die AGB zweier Geschäftspartner sind punktuell nicht vereinbar&lt;/li&gt;&lt;li&gt;Folgen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Teildissens über die widersprüchlichen Punkte&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Die Beurteilung der Gültigkeit des Restvertrags folgt den Regeln über &lt;strong&gt;versteckten &lt;/strong&gt;und &lt;strong&gt;offenen &lt;/strong&gt;Dissens über Haupt- und Nebenpunkte.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nicht geregelte Punkte sind mit &lt;strong&gt;dispositivem Recht&lt;/strong&gt; und &lt;strong&gt;ergänzender Vertragsauslegung&lt;/strong&gt; zu ermitteln.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Einbeziehungskontrolle: &lt;/span&gt;&lt;/p&gt;&lt;p&gt;Wie kann ein Kunde den AGB zustimmen?&lt;/p&gt;&lt;p&gt;Können AGBs "Nachgeschoben" werden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ausdrücklich oder Konkludent&lt;/li&gt;&lt;li&gt;Einseitiges "Nachschieben" durch den Aufsteller der AGB &lt;strong&gt;reicht nicht&lt;/strong&gt; aus, eine &lt;strong&gt;Parteieneinigung &lt;/strong&gt;zur nachträglichen Einbeziehung von AGB ist &lt;strong&gt;aber nicht ausgeschlossen&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Einbeziehungskontrolle: &lt;/span&gt;Wie müssen AGB einbezogen werden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;ausdrücklicher &lt;strong&gt;Hinweis reicht&lt;/strong&gt;: "ich verweise auf meine AGB" (AGB müssen nicht real vorliegen) &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die „Verdünnung der Willensfreiheit“ des Kunden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Kunde kann "in der Schnelle" des Vertragsabschlusses den Inhalt umfangreicher AGB häufig nicht zur Kenntnis nehmen, oder ist sich der Reichweite nicht bewusst.&lt;/li&gt;&lt;li&gt;Kunde hat nur die Wahl die AGB Gesamt zu akzeptieren oder auf die Ware zu verzichten.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind AGB?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Allgemeine Geschäftsbedingungen sind vorformulierte standardisierte Vertragsbedingungen, die ein Vertragspartner für alle oder eine bestimmte Gruppe von Verträgen erstellt.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie funktioniert das Widerrufsrecht im Konsumentenschutz?&lt;/p&gt;&lt;p&gt;Was ist die Voraussetzung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nach § 3 KSchG: Verbraucher hat das Recht Angebot &lt;strong&gt;bis Vertragsabschluss&lt;/strong&gt; durch einseitigen Widerruf zu zerstören.&lt;/p&gt;&lt;p&gt;Voraussetzung: Vertragserklärung außerhalb des Geschäftsraumes des Unternehmens.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wo finden sich gesetzliche Rücktrittsrechte außerhalb von KschG und FAGG?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;H&lt;span style="background-color: rgb(255, 255, 255); color: rgb(77, 81, 86);"&gt;ypothekar- und Immobilienkreditgesetz (&lt;/span&gt;&lt;a href="https://www.ris.bka.gv.at/GeltendeFassung.wxe?Abfrage=Bundesnormen&amp;amp;Gesetzesnummer=20009367" rel="noopener noreferrer" target="_blank" style="background-color: rgb(255, 255, 255); color: rgb(77, 81, 86);"&gt;§ 13 HIKrG&lt;/a&gt;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(77, 81, 86);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Verbraucherkreditgesetz (&lt;a href="https://www.jusline.at/gesetz/vkrg/paragraf/13" rel="noopener noreferrer" target="_blank"&gt;§ 13 VKrG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Teilnutzungsgesetz (&lt;a href="https://www.jusline.at/gesetz/tng/paragraf/8" rel="noopener noreferrer" target="_blank"&gt;§ 8 TNG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Bauträgervertragsgesetz (&lt;a href="https://www.jusline.at/gesetz/btvg/paragraf/5" rel="noopener noreferrer" target="_blank"&gt;§ 5 BTVG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;...&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Voraussetzungen für einen Rücktritt von Fernabsatzverträgen?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/fagg/paragraf/11" rel="noopener noreferrer" target="_blank"&gt;§§ 11-18 FAGG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;§ 11 - Voraussetzungen&lt;/li&gt;&lt;li&gt;§ 18 - Kein Rücktrittsrecht&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Voraussetzungen für einen Rücktritt wegen Nichteintritts maßgeblicher Umstände? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/3a" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 3a KschG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Maßgebliche Umstände treten nicht oder nur in erheblich geringerem Maß als vom Unternehmer dargestellt ein&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Voraussetzungen für den Rücktritt vom Haustürgeschäft?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/3" rel="noopener noreferrer" target="_blank"&gt;§ 3 KschG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Weder in den vom &lt;strong&gt;Unternehmer für seine geschäftlichen Zwecke dauernd benützten Räumen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Noch bei&lt;strong&gt; einem von diesem dafür auf einer Messe oder einem Markt benützten Stand&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die 3 (wichtigsten) gesetzlichen Rücktrittsrechte des Käufers (insb. Verbrauchers)?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;Rücktritt vom Haustürgeschäft&lt;/li&gt;&lt;li&gt;Rücktritt wegen Nichteintritts maßgeblicher Umstände&lt;/li&gt;&lt;li&gt;Rücktritt von Fernabsatzverträgen&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Option/Optionsvertrag?&lt;/p&gt;&lt;p&gt;Was die rechtlichen Folgen?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Eine Partei räumt der anderen, oder einem Dritten, das Recht ein (unabhängig von einer weiteren rechtsgeschäftlichen Erklärung des Verpflichteten), ein inhaltlich &lt;strong&gt;im Vorhinein bestimmtes Schuldverhältnis&lt;/strong&gt; in Geltung zu setzen&lt;/li&gt;&lt;li&gt;Rechtsfolge: Der Optionsberechtigte kann &lt;strong&gt;nach Ausübung der Option&lt;/strong&gt; unmittelbar die vertragliche Hauptleistung einklagen.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Punktation? Rechtliche Grundlagen?&lt;/p&gt;&lt;p&gt;Was sind die Voraussetzungen?&lt;/p&gt;&lt;p&gt;Was die rechtlichen Folgen? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/885" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 885 ABGB&lt;/a&gt;: Vorläufige (nicht formelle) verbindliche Fixierung der Hauptpunkte eines Vertrages -&amp;gt; Vertrag kommt zustande.&lt;/li&gt;&lt;li&gt;Voraussetzungen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Unterliegt der Schriftform (Schriftlich + Unterschrift), erfordert also Bindungswillen beider Parteien&lt;/li&gt;&lt;li&gt;Rechtsfolgen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Klage auf vertraglich geschuldete Leistungen möglich&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zeitlich nicht begrenzt (anders als Vorvertrag) -&amp;gt; normale Verjährungsjahre&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Vorvertrag?&lt;/p&gt;&lt;p&gt;Wann und wie Lange ist er gültig?&lt;/p&gt;&lt;p&gt;Worauf kann geklagt werden?&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was die gesetzliche Grundlage?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/936" rel="noopener noreferrer" target="_blank"&gt;§ 936 ABGB&lt;/a&gt;: Vertrag über den künftigen Abschluss des von den Parteien in Aussicht genommenen Hauptvertrages.&lt;/li&gt;&lt;li&gt;Gilt nur:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Parteien haben sich über den wesentlichen Inhalt (z.B.: Ware und Preis) des Hauptvertrages geeinigt.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zeitpunkt für Hauptvertrag-Abschluss ist fixiert.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gilt max 1 Jahr ab fixiertem Zeitpunkt für Abschluss des Hauptvertrags.&lt;/li&gt;&lt;li&gt;Klage nur auf Abschluss des Hauptvertrags, nicht auf Leistungen aus dem Hauptvertrag.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;ECG&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;E-Commerce-Gesetz&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche gesetzlichen Grundlagen regeln Vertragsabschluss im E-Commerce?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Elektronische Willenserklärung -&amp;gt; es gelten grundsätzlich die allgemeinen Regelungen &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/861" rel="noopener noreferrer" target="_blank"&gt;§§ 861ff ABGB&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/ecg/paragraf/10" rel="noopener noreferrer" target="_blank"&gt;§§ 10 -12 ECG&lt;/a&gt;: Sondervorschriften über &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Abgabe einer Vertragserklärung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vertragsbestimmungen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Geschäftsbedingungen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zugang elektronischer Erklärungen.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was regelt das FAGG?&lt;/p&gt;&lt;p&gt;Was ist in Bezug auf Vertragsschluss besonders zu beachten?&lt;/p&gt;&lt;p&gt;Welche gesetzlichen Grundlagen gibt es?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/fagg/paragraf/1" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§§ 1 - 11 FAGG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/fagg/paragraf/1" rel="noopener noreferrer" target="_blank"&gt;§ 1 Abs 1 FAGG&lt;/a&gt; -&amp;gt; Fern- und Auswärtsgeschäfte zwischen Unternehmern und Verbrauchern.&lt;/li&gt;&lt;li&gt;Beachten: Informationspflichten vor Vertragsschluss&lt;/li&gt;&lt;li&gt;Art und Umfang der Informationserteilung abhängig von Vertragstypen und Vertragsschlusssituation (§§ 4 - 9 FAGG)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;FAGG&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Fern- und Auswertsgeschäfte-Gesetz&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Einfluss eines Kaufmännischen Bestätigungsschreiben auf einen Vertrag?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Grundsätzlich keine vertragsändernde Wirkung&lt;/li&gt;&lt;li&gt;Schweigen des Empfängers gilt nicht als Zustimmung zu Vertragsabschluss- oder Änderung, außer:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bestätigungsschreiben ergänzt bloß &lt;strong&gt;geringfügige Punkte&lt;/strong&gt;, die beim Vertragsabschluss &lt;strong&gt;bewusst von beiden Parteien&lt;/strong&gt; offen gelassen wurden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Empfänger wird &lt;strong&gt;nur begünstigt.&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Kreuzofferte? &lt;/p&gt;&lt;p&gt;Was ist die Auswirkung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;"Überkreuzung" am Postweg: Zwei künftige Vertragspartner übermitteln einander Angebote auf An- und Verkauf derselben Sache die inhaltlich identisch sind.&lt;/li&gt;&lt;li&gt;Vertrag wird mit Zugang der letzten Offerte perfekt; wenn Parteirollen zusammenpassen (Verkäufer+Käufer)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Angebot "ohne Obligo" (unverbindliches, freibleibendes Offert)?&lt;/p&gt;&lt;p&gt;Ist es gültig? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Beschränkung der Bindung an den Vertragsabschluss durch einseitige Annahme durch Klausel&lt;/li&gt;&lt;li&gt;Anbieter behält sich vor &lt;strong&gt;bis zur Annahme&lt;/strong&gt; durch Widerruf das Angebot zu zerstören&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Üblicherweise Widerruf nur bis Zugang bei Annehmenden, Klausel versucht also Widerrufzeitraum zu verlängern&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Frage: Darf der Anbieter das?&lt;/li&gt;&lt;li&gt;Im Zweifel nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/915" rel="noopener noreferrer" target="_blank"&gt;§ 915 ABGB&lt;/a&gt; vorgehen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Anbieter kann nach Zugang nicht mehr widerrufen, d.h. Angebot ist gar kein wirkliches Angebot da kein Bindungswille.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Annahmeerklärung des Annehmenden ist also eigentlich ein Angebot.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ursprünglicher Anbieter hat Redepflicht um abzulehnen, sonst kommt Vertrag nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/862a" rel="noopener noreferrer" target="_blank"&gt;§ 862a&lt;/a&gt; ABGB zustande&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was bedeutet "Protestatio facto contraria valet"?&lt;/p&gt;&lt;p&gt;Welche rechtlichen Fragen stellen sich daraus?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Protest entgegen den Fakten schadet nicht&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Fragen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Kann faktische Inanspruchnahme einer Leistung einen Vertrag zustandekommen lassen? &lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Auch wenn er klar äußert, dass er keinen Vertrag abschließen will? &lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Beispiel: Einsteigen in Öffentliches Verkehrsmittel, Benutzen von Parkplatz&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;Kann faktische Inanspruchnahme einer Leistung einen Vertrag zustandekommen lassen? &lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;Auch wenn er klar äußert, dass er keinen Vertrag abschließen will? &lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;Was bedeutet dies für "Protest entgegen den Fakten schadet nicht" in Ö? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank"&gt;§ 863 ABGB&lt;/a&gt;: Konkludente Handlung nur, wenn kein vernünftiger Grund daran zu zweifeln&lt;/li&gt;&lt;li&gt;Rechtslehre sagt: Nur ausdrückliche oder konkludente WE führt zu Vertrag&lt;/li&gt;&lt;li&gt;Daher bei Klarstellung das kein Wille zum Vertrag -&amp;gt; kein Vertrag&lt;/li&gt;&lt;li&gt;Zahlungen für Inanspruchnahme daher nicht aus Vertrag, aber z.B.: Bereicherungsrecht, Schadenersatzrecht.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;-&amp;gt; Protest gegen die Fakten schadet in Österreich!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der unterschied zwischen "Angebot an unbekannte Person" und "invitatio ad offerendum"?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Angebot an unbekannt:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bindungswille: Verkäufer gibt zu erkennen das präsentierte, reale Waren zum Verkauf an jeden stehen, solange Vorrat reicht (z.B.: Getränkeautomat)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Kann idR durch Willensbetätigung angenommen werden (Annahmehandlung nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/864" rel="noopener noreferrer" target="_blank"&gt;§ 864 ABGB&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Konkreter Unterschied: &lt;strong&gt;Beschränkung des Angebotes auf den real vorhandenen Vorrat&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Invitatio ad offerendum: Erklärender will sich erkennbar nicht gegenüber jedermann binden (z.B.: Flugblatt, Katalog)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Prinzip der kausalen Tradition (Lehre von Titel und Modus)? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/380" rel="noopener noreferrer" target="_blank"&gt;§ 380 ABGB&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/424" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(115, 133, 197);"&gt;§§ 424ff ABGB&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;, &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/1053" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(115, 133, 197);"&gt;§ 1053 ABGB&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;, &lt;/span&gt;&lt;/p&gt;&lt;p&gt;Zum Erwerb des Eigentumsrechts muss zum gültigen Verpflichtungsgeschäft (&lt;strong&gt;Titel&lt;/strong&gt;) auch ein Verfügungsgeschäft (&lt;strong&gt;Modus&lt;/strong&gt;) hinzutreten.&lt;/p&gt;&lt;p&gt;-&amp;gt; &lt;strong&gt;Man wird nicht bereits mit Abschluss des Kaufvertrages Eigentümer.&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie nennt man entgeltliche Rechtsgeschäfte noch? &lt;/p&gt;&lt;p&gt;Was ist die Bedeutung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Synallagmatische Verträge&lt;/li&gt;&lt;li&gt;Erbringt ein Teil seine Leistung nicht, muss auch der andere seine nicht erbringen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Schutznormen des KSchG? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/3" rel="noopener noreferrer" target="_blank"&gt;§ 3-6 KSchG&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/fagg/paragraf/11" rel="noopener noreferrer" target="_blank"&gt;§§ 11ff FAGG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Verbraucher kann von einem sog. Haustürgeschäft zurücktreten (grundlos innerhalb bestimmter Fristen) &lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; (§ 3 KSchG)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;besonderes Rücktrittsrecht &lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;(§ 3 KSchG, §§ 11ff FAGG)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Kostenvoranschlag gegenüber Verbraucher gilt als Garantie &lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; (§ 5 KSchG)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Bestimmte Klauseln in AGBs sind Unwirksam (§ 6 KSchG)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Realofferte? Was die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/864" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(136, 125, 220);"&gt;§ 864 Abs. 2 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Behalten, Verwenden, Verbrauchen einer Sache gilt nicht als Annahme eines Angebots, wenn sie dem Empfänger ohne dessen Veranlassung übersandt wurde.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Angebotsannahme: Rechtzeitigkeit der Annahme&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/862" rel="noopener noreferrer" target="_blank"&gt;§ 862 ABGB&lt;/a&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Angebot erlischt nach Geltungsdauer, diese muss eruiert werden:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Vom Erklärenden gesetzt (im Rahmen von &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/902" rel="noopener noreferrer" target="_blank"&gt;§§ 902f ABGB&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Sonst gesetzliche Frist nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/862" rel="noopener noreferrer" target="_blank"&gt;§ 862 S2 ABGB&lt;/a&gt; (inkl Postlauf des Angebots, Überlegungsfrist und Postlauf der Annahme)&lt;/li&gt;&lt;li&gt;Ausnahme &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/862a" rel="noopener noreferrer" target="_blank"&gt;§ 862a ABGB&lt;/a&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Verzögerung der nachweislich rechtzeitig abgesendeten Annahmeerklärung am Postweg (=Übermittlung)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Der Antragsteller kann aber &lt;strong&gt;unverzüglich &lt;/strong&gt;(ohne schuldhaftes Zögern) zurücktreten&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Realakte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Handlungen ohne Kundgabezweck die auch ohne Geschäftsfähigkeit und Rechtsfolgewillen Rechtsfolgen auslösen (z.B.: Urheberrechte durch Schaffen von Kunstwerk, Rechte und Pflichte durch Fund)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Willensmitteilung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Willenshandlungen ohne Rechtsfolgewillen (z.B. Mahnung zeigt dass Zahlung erwünscht ist)&lt;/li&gt;&lt;li&gt;Rechtsfolgen treten unabhängig von Rechtsfolgewillen des Handelnden ein (z.B.: Mahnung bewirkt Fälligkeit)&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Willensmitteilung kann kein Angebot/Annahme sein.&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Wissenserklärung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Nur auf Kundgabe von Fakten oder Kenntnissen gerichtet (Quittung, Mitteilung des Kontostantds, ... )&lt;/li&gt;&lt;li&gt;Vorschriften für Rechtsgeschäfte weitgehend auf &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wissenserklärung  angewandt, aber &lt;/span&gt;Angebot/Annahme durch &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wissenserklärung &lt;/span&gt;nicht möglich&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was kann eine stillschweigende/konkludente Willenserklärung sein?&lt;/p&gt;&lt;p&gt;Kann ein Unterlassen eine Willenserklärung sein? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Eindeutige Handlung nach Verkehrssitte ohne vernünftigen Grund daran zu zweifeln (z.B.: verzehren des aus dem Korb entnommenen Brots)&lt;/li&gt;&lt;li&gt;passives Unterlassen (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 863 ABGB&lt;/a&gt; ): Schweigen gilt nicht als Zustimmung, außer es besteht eine Redepflicht aus:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gesetz&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Verträgen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Übung des redlichen Verkehrs (z.B.: ständige Geschäftsverbindungen)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;vorvertragliche Aufklärungspflichten&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die 4 Voraussetzungen für die Annahme eines Angebots durch &lt;strong&gt;Willenserklärung&lt;/strong&gt;? Was ist die Rechtliche Grundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank"&gt;§ 863 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ol&gt;&lt;li&gt;Ausdrückliche oder konkludente Willenserklärung&lt;/li&gt;&lt;li&gt;Zugang der Willenserkärung&lt;/li&gt;&lt;li&gt;Rechtzeitigkeit der Annahme&lt;/li&gt;&lt;li&gt;Kein Widerruf der Annahme&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die 2 Grundvorraussetzungen für das Zustandekommen eines Vertrags? Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/861" rel="noopener noreferrer" target="_blank"&gt;§§ 861 ff ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Angebot + Annahme&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtsfähigkeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;gibt jedem Rechtssubjekt die Macht, seine Belange (seine eigene Rechtssphäre) nach freiem Belieben zu regeln.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Willenserklärung: &lt;/span&gt;Rechtsfolgewille (Geltungswille)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Der Handelnde ist an seiner Erklärung gebunden, wenn er in dem Bewusstsein handelt, rechtliche verbindliche Handlungen zu setzen, die erforderlichenfalls mit staatlichen Zwang durchsetzbar sind (gemäßigte Rechtsfolgentheorie).&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welches weitere Gesetz definiert Unternehmensformen die für die Auslegung des KSchG relevant sind?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;UGB 2007 (Unternehmensgesetzbuch)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Verbrauchergeschäfte? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/1" rel="noopener noreferrer" target="_blank"&gt;§ 1 &lt;/a&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/1" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;KSchG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;: &lt;/span&gt;Wenn an einem zweiseitigen RG einerseits ein Unternehmer, für den das RG zum Betrieb seines Unternehmens gehört, und andererseits ein Verbraucher, auf den das nicht zutrifft, beteiligt -&amp;gt; Anwendung des KSchG &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Abstrakte/Kausale Rechtsgeschäfte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;abstrakt&lt;/strong&gt;: Wenn sich der Zweck (Rechtsgrund, causa) einer Verpflichtungserklärung nicht entnehmen lässt, sind idR ungültig.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;kausal&lt;/strong&gt;: wenn sich aus ihnen der Rechtsgrund entnehmen lässt&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Verpflichtungs- und Verfügungsgeschäfte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Verpflichtung&lt;/strong&gt;: geben dem Gläubiger einen schuldrechtlichen Anspruch (Forderung) auf Lieferung der Sache, aber noch kein dingliches (Eigentums-)Recht an der Sache. z.B: Käufer wird erst Eigentümer, wenn die Sache durch &lt;strong&gt;Verfügungsgeschäft &lt;/strong&gt;vom Verkäufer übergeben wird.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verfügung&lt;/strong&gt;: Führt die Verschiebung des (sachenrechtlichen) Eigentumsrecht von Verkäufer an Käufer herbei. &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Ziel- und Dauerschuldverhältnisse?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ziel&lt;/strong&gt;: Ansprüche erlöschen durch die intendierte einmalige Leistungserbringung (Kaufvertrag: Lieferung + Bezahlung)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Dauer&lt;/strong&gt;: Wiederkehrende Leistungserbringung ohne Erlöschen&lt;strong&gt; &lt;/strong&gt;der Ansprüche ist vorgesehen (Strom, Zeitungsabo, unbefristeter Mietvertrag)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Konsensualverträge/Realverträge?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Konsensual&lt;/strong&gt;: Kommen durch bloße Einigung zustande  (Kaufvertrag, Mietvertrag, ...)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Real&lt;/strong&gt;: Erfordert zum Abschluss auch Sachübergabe (Darlehensvertrag, Leihvertrag und Verwahrungsvertrag)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Rechtsgeschäfte unter Lebenden, und von Todes wegen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Lebenden&lt;/strong&gt;: Wirkung tritt zu Lebzeiten der Partner ein (Kaufvertrag, Mietvertrag, .. )&lt;/li&gt;&lt;li&gt;&lt;strong&gt;von Todes wegen&lt;/strong&gt;: Tritt nach dem Tod mindest einer Partei ein (Erbvertrag, Testament, ... )&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind empfangsbedürftige und nicht empfangsbedürftige Rechtesgeschäfte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Testament nicht empfangsbedürftig&lt;/li&gt;&lt;li&gt;Kündigung, Angebotserklärung/Annahme, etc sind Empfangsbedürftig -&amp;gt; Empfangstheorie&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Einseitig/Zweiseitig verpflichtende Rechtsgeschäfte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Einseitig&lt;/strong&gt;: Nur ein Partner zur Leistung verpflichtet (Schenkung)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Zweiseitig &lt;/strong&gt;(ABGB nennt diese&lt;strong&gt; Gegenseitige Verträge&lt;/strong&gt;): Beide Seiten verpflichtet (Kaufvertrag, ... )&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Ein-, Zwei- und mehrseitige Rechtsgeschäfte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Differenzierung anhand der Anzahl der erforderlichen Willenserkärungen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ein&lt;/strong&gt;: Testament, Auslobung, Kündigung, ...&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Zwei&lt;/strong&gt;: Kaufvertrag, ...&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Mehr&lt;/strong&gt;: Gesellschaftsvertrag&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Rechtsgeschäft im juristischen Sinn?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ein Tatbestand, der aus einer oder mehreren Willensäußerungen von Rechtssubjekten besteht, an welche die Privatrechtsordnung den Eintritt von Rechtsfolgen knüpft.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann begrenzen Drittwirkungen der Grundrechte die Privatautonomie?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Keine unmittelbare Drittwirkung der Grundrechte, aber:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Interpretation von Generalklauseln (z.B. Sittenwidrigkeit) können in die Interpretation privatrechtlicher Normen einfließen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Fiskalgeltung der Grundrechte: Gebietskörperschaften sind an die Grundrechte gebunden, auch wenn sie privatrechtlich Handeln. &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Kontrahierungszwang? Wodurch kann er entstehen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Zwang zum Vertragsabschluss&lt;/li&gt;&lt;li&gt;Entsteht durch:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gesetzliche Anordnung (z.B.: bei Monopol, Gefährdung der Nahversorgung)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Auch ohne ausdrückliche Gesetzliche Vorschrift bei faktischer Monopolstellung eines Vertragspartners (Nichtabschluss würde sonst rechtswidriges/sittenwidriges Verhalten darstellen)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche drei Arten der Grenzen der Privatautonomie gibt es?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gesetzliche Vorschriften / zwingendes Recht&lt;/li&gt;&lt;li&gt;Begrenzung der Abschlussfreiheit durch Kontrahierungszwang&lt;/li&gt;&lt;li&gt;Drittwirkung der Grundrechte&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die 7 Inhalte der Privatautonomie?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Abschlussfreiheit (ob, wann und mit wem Vertrag geschlossen wird)&lt;/li&gt;&lt;li&gt;Inhaltsfreiheit&lt;/li&gt;&lt;li&gt;Typenfreiheit (neue Vertragstypen zu schaffen)&lt;/li&gt;&lt;li&gt;Beendigungsfreiheit&lt;/li&gt;&lt;li&gt;Änderungsfreiheit&lt;/li&gt;&lt;li&gt;Formfreiheit&lt;/li&gt;&lt;li&gt;Testierfreiheit (ob und wie der Verstorbene letztwillig testiert)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Verhältnis der Auslegungsmethoden zueinander?&lt;/p&gt;&lt;p&gt;Gibt es eine Reihenfolge?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Der Gesetzgeber gibt in &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/6" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§§ 6, 7 ABGB&lt;/a&gt; keine Reihenfolge vor, daher geht man von der &lt;strong&gt;Gleichrangigkeit &lt;/strong&gt;aus.&lt;/li&gt;&lt;li&gt;Alle zur Verfügung stehenden Methoden sollen herangezogen werden.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Authentische Interpretation?&lt;/p&gt;&lt;p&gt;Wie wird sie noch genannt?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/8" rel="noopener noreferrer" target="_blank" style="color: rgb(115, 133, 197); background-color: rgb(40, 45, 88);"&gt;§ 8 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Der Gesetzgeber erklärt in einem späteren Gesetz, wie ein zuvor erlassene Regelung zu verstehen ist.&lt;/li&gt;&lt;li&gt;Legalinterpretation&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtsgrundlage für die Methoden der Auslegung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/6" rel="noopener noreferrer" target="_blank"&gt;§§ 6, 7 ABGB&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann wird die teleologische Interpretation eingesetzt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li class="ql-align-justify"&gt;&lt;strong&gt;keine Gesetzesmaterialien &lt;/strong&gt;zur Verfügung stehen.&lt;/li&gt;&lt;li class="ql-align-justify"&gt;der Regelungszweck zwar festgestellt werden kann, aber nicht mehr passend erscheint und daher&lt;strong&gt; der aktuelle Regelungszweck ermittelt werden muss.&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Konstellationen auftreten, die vom Regelungskonzept des &lt;strong&gt;historischen Gesetzgebers nicht erfasst und nicht bedacht waren.&amp;nbsp;&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die teleologische Interpretation?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Feststellung von &lt;strong&gt;Sinn &lt;/strong&gt;und &lt;strong&gt;Zweck &lt;/strong&gt;der Norm.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wovon hängt der &lt;strong&gt;Bedeutungsgehalt &lt;/strong&gt;eines Wortes ab?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="ql-align-justify"&gt;Abhängig davon, ob ein &lt;strong&gt;allgemeiner&lt;/strong&gt;, &lt;strong&gt;fachspezifischer &lt;/strong&gt;oder &lt;strong&gt;rechtlicher&lt;/strong&gt; Sprachgebrauch herangezogen wird.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Wortinterpretation?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Es wird hinterfragt, welche Bedeutung den Worten, Wortkombinationen und Sätzen des Gesetzgebers zukommen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die systematische Interpretation?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Bedeutung der Worte in Ihrem Zusammehang wird ermittelt.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Womit wird die Absicht des Gesetzgebers in der historischen Interpretation ermittelt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p class="ql-align-justify"&gt;Mit den &lt;strong&gt;Gesetzesmaterialien&lt;/strong&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li class="ql-align-justify"&gt;Regierungsvorlagen&lt;/li&gt;&lt;li class="ql-align-justify"&gt;Ministerialentwürfe&lt;/li&gt;&lt;li class="ql-align-justify"&gt;Initiativanträge samt Erläuterungen&lt;/li&gt;&lt;li class="ql-align-justify"&gt;Kommissions- und Ausschussberichte&lt;/li&gt;&lt;li&gt;Stenographische Protokolle des Nationalrats&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Wann erlischt ein Angebot?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/862" rel="noopener noreferrer" target="_blank"&gt;§ 862 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;nach Ablauf der gesetzten oder gesetzlichen Pflicht&lt;/li&gt;&lt;li&gt;bei Ablehnung&lt;/li&gt;&lt;li&gt;Insolvenz des Antragstellers&lt;/li&gt;&lt;li&gt;Tod oder nachträgliche Geschäftsunfähigkeit des Antragstellers oder Erklärungsempfängers, wenn der Wille aus den Umständen hervorgeht&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Welcher Zeitpunkt zählt als Empfangszeitpunkt laut Empfangstheorie wenn z.B.: eine Erklärung in einem Postfach hinterlegt wird?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Der objektiv erste mögliche Zeitpunkt der Kenntnisnahme durch den Empfänger, z.B.: Ankunft des Briefs im Postfach (der Empfänger &lt;strong&gt;könnte&lt;/strong&gt; den Brief abholen), NICHT wenn der Empfänger &lt;strong&gt;tatsächlich&lt;/strong&gt; Abholt.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was sind die 5 Voraussetzungen für Angebotsannahme durch &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Willensbetätigung&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;?&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Rechtsgrundlage?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/864" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 864 ABGB&lt;/a&gt; &lt;/p&gt;&lt;ol&gt;&lt;li&gt;Willenserklärung nicht zu erwarten (Natur des Geschäfts, Verkehrssitte, Verzicht durch Anbieter)&lt;/li&gt;&lt;li&gt;Annahmehandlung: Annehmender Verfügt über die Sache in einer Weise, zu der er nur berechtigt ist, wenn er das Angebot annehmen will (z.B: Versand der bestellten Ware).&lt;/li&gt;&lt;li&gt;Annahmewille (Vertragsabschlusswille)&lt;/li&gt;&lt;li&gt;Rechtzeitigkeit der Annahme: Während der Geltungsdauer des Angebots; Willensbetätigung ist aber &lt;strong&gt;nicht zugangsbedürftig &lt;/strong&gt;-&amp;gt; es zählt Zeitpunkt der Annahmehandlung. &lt;/li&gt;&lt;li&gt;Kein Widerruf der Willensbetätigung: Widerruf der Annahme bis zur Kenntnisnahme des Anbietenden möglich.&lt;/li&gt;&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die Rechtsfolgen der Nichterfüllung einer Bedingung?&lt;/p&gt;&lt;p&gt;Wie muss eine Bedingung erfüllt werden?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Rechtserwerb wird verhindert bzw. Rechtsverlust herbeigeführt.&lt;/li&gt;&lt;li&gt;Muss nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/699" rel="noopener noreferrer" target="_blank"&gt;§ 699 ABGB&lt;/a&gt; &lt;strong&gt;stets genau erfüllt &lt;/strong&gt;werden.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die Rechtsfolgen der Nichteinhaltung einer Auflage? &lt;/p&gt;&lt;p&gt;Wie muss eine Auflage erfüllt werden?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Einhaltung kann durch Klage oder Exekution erzwungen werden.&lt;/li&gt;&lt;li&gt;Nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/709" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 709 ABGB&lt;/a&gt; genügt die &lt;strong&gt;annähernde &lt;/strong&gt;Erfüllung, wenn die &lt;strong&gt;genaue&lt;/strong&gt; Erfüllung &lt;strong&gt;nicht möglich &lt;/strong&gt;ist.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine Auflage?&lt;/p&gt;&lt;p&gt;Wie ist sie im Zweifel zu behandeln, Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/709" rel="noopener noreferrer" target="_blank"&gt;§ 709 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Die einem Empfänger einer Zuwendung im Zusammenhang mit einer &lt;strong&gt;letztwillligen Verfügung&lt;/strong&gt; oder einem &lt;strong&gt;unentgeltlichen Rechtsgeschäft unter Lebenden&lt;/strong&gt; auferlegte &lt;strong&gt;Verpflichtung &lt;/strong&gt;zur &lt;strong&gt;Vornahme eines bestimmten Verhaltens&lt;/strong&gt; bei &lt;strong&gt;sonstigem Verlust der Zuwendung&lt;/strong&gt;, wobei es unerheblich ist, in wessen Interesse das geforderte Verhalten ist.&lt;/li&gt;&lt;li&gt;Im zweifel als auflösende Bedingung nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/10" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 710 ABGB&lt;/a&gt; &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie werden Samstage, Sonntage und gesetzliche Feiertage bei Fristen gehandhabt?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Zählen in die Berechnung der Frist&lt;/li&gt;&lt;li&gt;Ist der letzte Tag der Frist ein Sa, So oder gesetzl. Feiertag, so läuft die Frist mit&lt;strong&gt; Ende des nächstfolgenden Werktages ab&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/903" rel="noopener noreferrer" target="_blank"&gt;§ 903 S3 ABGB&lt;/a&gt;, &lt;a href="https://www.ris.bka.gv.at/GeltendeFassung.wxe?Abfrage=Bundesnormen&amp;amp;Gesetzesnummer=10000765" rel="noopener noreferrer" target="_blank"&gt;Art. 5 EuFrÜb&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Welche Rechtsgrundlagen für Fristen sind heranzuziehen, wenn weder Sondergesetze noch Parteien anders vereinbaren?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/902" rel="noopener noreferrer" target="_blank"&gt;§§ 902-904 ABGB&lt;/a&gt; und EuFrÜb (Europäisches Übereinkommen über die Berechnung von Frist)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine Befristung?&lt;/p&gt;&lt;p&gt;Was ist der Unterschied zur Bedingung? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Eine von den &lt;strong&gt;Parteien gesetzte Beschränkung&lt;/strong&gt; des Rechtsgeschäftes, bei der &lt;strong&gt;Inkrafttreten&lt;/strong&gt; oder &lt;strong&gt;Außerkrafttreten &lt;/strong&gt;der Rechtswirkung entweder &lt;strong&gt;kalendrisch bestimmt&lt;/strong&gt;, oder von einem &lt;strong&gt;sicher eintretenden Ereignis&lt;/strong&gt; abhängig gemacht wird.&lt;/li&gt;&lt;li&gt;Unterschied: Bedingung hat ein ungewisses Ereignis.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Beispiel 1: "Wenn A stirbt ..." ist eine Befristung, aufgrund der Gewissheit des Eintretens.&lt;/p&gt;&lt;p&gt;Beispiel 2: "Sollte A das 90. Lebensjahr erreichen ... " ist eine Bedingung, weil Ungewiss.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist ein Termin?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Ein rechtlich erheblicher Zeitpunkt&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine Frist?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Eine rechtlich erhebliche Zeitspanne&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Beeinflussing wider Treu und Glauben? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Gelingt es jemandem, dem die Bedingung zum &lt;strong&gt;Nachteil &lt;/strong&gt;gereicht, sie zu &lt;strong&gt;vereiteln&lt;/strong&gt;, gilt die Bedingung als &lt;strong&gt;eingetreten&lt;/strong&gt;. &lt;/li&gt;&lt;li&gt;Gelingt es jemandem, dem die Bedingung zum &lt;strong&gt;Vorteil &lt;/strong&gt;gereicht, die Bedingung wider Treu und Glauben &lt;strong&gt;herbeizuführen&lt;/strong&gt;, gilt die Bedingung als &lt;strong&gt;ausgefallen&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Beispiel: X verspricht Y ihm sein Auto zu schenken, wenn die nächste Reperatur ansteht. Y sapotiert das Auto von X. Die Bedingung wurde wider Treu und Glauben herbeigeführt und gilt daher als ausgefallen und die Schenkung tritt nicht in kraft.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Rechtsgrundlage für unmögliche aufschiebende und unmögliche auflösende Bedingungen? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/698" rel="noopener noreferrer" target="_blank" style="color: black; background-color: rgb(40, 45, 88);"&gt;§ 698 ABGB&lt;/a&gt;, für letzten Willen auch &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/898" rel="noopener noreferrer" target="_blank"&gt;§ 898 ABGB&lt;/a&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wann ist eine Bedingung unmöglich?&lt;/p&gt;&lt;p&gt;Was ist unmöglich allgemein definiert?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Eine Bedingung ist &lt;strong&gt;unmöglich&lt;/strong&gt;, wenn sie aus &lt;strong&gt;tatsächlichen&lt;/strong&gt; oder &lt;strong&gt;rechtlichen Gründen &lt;/strong&gt;nicht eintreten kann.&lt;/li&gt;&lt;li&gt;Unmöglich ist, was &lt;strong&gt;objektiv gesehen&lt;/strong&gt; und &lt;strong&gt;nicht &lt;/strong&gt;nur &lt;strong&gt;vorrübergehend &lt;/strong&gt;sondern &lt;strong&gt;dauerhaft&lt;/strong&gt; &lt;strong&gt;unmöglich&lt;/strong&gt; ist und niemand erfüllen kann.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Welche Bedingungen gelten nicht?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/697" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: black;"&gt;§ 697 ABGB&lt;/a&gt;&lt;/p&gt;&lt;p&gt;Unverständliche, unbestimmte, sowie gesetz- oder sittenwidrige Bestimmungen&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind bejahende (positive) Bedingungen?&lt;/p&gt;&lt;p&gt;Was sind verneinende (negative) Bedingungen?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Positive&lt;/strong&gt;: wenn du deine Freundin heiratest, bekommst du ein Auto &lt;/p&gt;&lt;p&gt;&lt;strong&gt;Negative&lt;/strong&gt;: Wenn du nicht rauchst, bekommst du ein Auto&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Sind Rechtsbedingungen Bedingungen im Sinne von &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/696" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: black;"&gt;§ 696 ABGB&lt;/a&gt;? Warum schon/warum nicht?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Nein, sie sind gesetzliche Vorraussetzungen und daher &lt;strong&gt;unabhängig von der Aufnahme in den Vertrag&lt;/strong&gt; zu beachten.&lt;/p&gt;&lt;p&gt;(z.B.: Zustimmung des Gesetzlichen Vertreters zu einem Geschäft eines unmündigen Minderjährigen) &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine Bedingung?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p class="ql-align-justify"&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/696" rel="noopener noreferrer" target="_blank" style="color: black;"&gt;§ 696 ABGB&lt;/a&gt;&lt;/p&gt;&lt;p class="ql-align-justify"&gt;&lt;span style="color: black; background-color: lightgrey;"&gt;Eine &lt;/span&gt;&lt;strong style="color: black; background-color: lightgrey;"&gt;Bedingung&lt;/strong&gt;&lt;span style="color: black; background-color: lightgrey;"&gt; ist ein ungewisses Ereignis, von dem ein Recht abhängig gemacht wird.&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine &lt;strong&gt;uneigentliche &lt;/strong&gt;Bedingung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Die Parteien wissen nicht, ob das Ereignis schon eingetreten ist.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine &lt;strong&gt;eigentliche &lt;/strong&gt;Bedingung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Der Eintritt der rechtswirkungen ist von einem &lt;strong&gt;künftigen ungewissen&lt;/strong&gt; Ereignis abhängig.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Rechtsgrundlage für die Wiederholung einer Bedingung? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/899" rel="noopener noreferrer" target="_blank"&gt;§ 899 ABGB&lt;/a&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine Potestativbedingung?&lt;/p&gt;&lt;p&gt;Wie wird sie noch genannt?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Das vereinbarte Ereignis ist steuerbar oder beinflussbar (z.B.: Vater schenkt Sohn ein Auto, wenn dieser seine Freundin heiratet)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Wollensbedingung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine Zufallsbedingung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Das vereinbarte Ereignis ist von den Parteien nicht beeinflussbar oder steuerbar (z.B.: Vater schenkt Sohn ein Auto wenn er im Lotto gewinnt)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was sind die Rechtsfolgen einer auflösenden Bedingung?&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Ähnlichkeit zur Anfechtung?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Eine Auflösende Bedingung vernichtet das Geschäft ex-nunc (&lt;strong&gt;ab &lt;/strong&gt;dem &lt;strong&gt;Eintritt &lt;/strong&gt;der &lt;strong&gt;vereinbarten Bedingung&lt;/strong&gt;) &lt;/li&gt;&lt;li&gt;Ähnlichkeit zur Anfechtung: Vertrag kommt zunächst gültig zustande und Rechtsswirkungen entfalten sich, erst später wird er vernichtet.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die Rechtsfolgen einer aufschiebenden Bedingung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Zum Zeitpunkt der Vereinbarung entsteht eine Anwartschaft (&lt;strong&gt;Vorrecht&lt;/strong&gt;) auf die beabsichtigten Leistungen. &lt;/li&gt;&lt;li&gt;Bleibt die Bedingung aus, so wird dieses Vorrecht &lt;strong&gt;ex-tunc &lt;/strong&gt;(Rückwirkend) nichtig. &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie wird ermittelt ob die Parteien aufschiebende oder Auflösende Bedigungen vereinbart haben?&lt;/p&gt;&lt;p&gt;Kann die Art der Bedingungen für die einzelnen Parteien unterschiedlich sein?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Im Einzelfall durch Auslegung der Willenserklärungen zu ermitteln.&lt;/li&gt;&lt;li&gt;Art kann für die Parteien unterschiedlich sein, z.B.: bei Eigentumsvorbehalt (Auto gehört mir erst bei völliger Bezahlung. D.h.: Für Käufer ist es aufschiebende Bedingung, für Verkäufer auflösend [er "verliert" das Auto bei völliger Bezahlung durch den Käufer])&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine auflösende Bedingung?&lt;/p&gt;&lt;p&gt;Wie wird sie noch genannt?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/696" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: black;"&gt;§ 696 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Tritt sofort in Kraft, tritt jedoch in dem Moment &lt;strong&gt;außer Kraft&lt;/strong&gt;, in dem das ungewisse &lt;strong&gt;Ereignis eintritt.&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Resolutivbedingung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine aufschiebende Bedingung?&lt;/p&gt;&lt;p&gt;Wie wird sie noch genannt?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/696" rel="noopener noreferrer" target="_blank" style="color: black; background-color: rgb(40, 45, 88);"&gt;§ 696 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Tritt erst in jenem Augenblick &lt;strong&gt;in Kraft&lt;/strong&gt;, in welchem das ungewisse &lt;strong&gt;Ereignis eintritt.&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Suspensivbedigungung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der Geschäftsirrtum?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Ein &lt;strong&gt;Motiv &lt;/strong&gt;wurde zum &lt;strong&gt;Vertragsinhalt &lt;/strong&gt;oder sogar zur &lt;strong&gt;Bedigung&lt;/strong&gt; (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/901" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 901 ABGB&lt;/a&gt;), daher kann der Vertrag wegen Geschäftsirrtum &lt;strong&gt;angefochten &lt;/strong&gt;oder &lt;strong&gt;angepasst &lt;/strong&gt;werden.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die Rechtsfolgen von einseitigen Irrtümern über Motive?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Da von der Unbeachtlichkeit von Motiven auszugehen ist, gibt es keine Rechtsfolgen.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Sind Motive beim Vertragsabschluss grundsätzlich zu beachten?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage für die Ausnahme?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Grundsätzlich ist von der Unbeachtlichkeit auszugehen.&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/901" rel="noopener noreferrer" target="_blank"&gt;§ 901 ABGB&lt;/a&gt; ist die Ausnahme (Motiv wird ausdrücklich zur Bedingung gemacht)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Zweifelsregel?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/915" rel="noopener noreferrer" target="_blank" style="background-color: yellow; color: black;"&gt;§ 915 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Bei entgeltlichen Rechtsgeschäften ist eine undeutliche Äußerung im Zweifel zum Nachteil desjenigen zu verstehen, der sich ihrer bedient hat.&lt;/li&gt;&lt;li&gt;Lässt sich kein eindeutiger Sinn ermitteln, so ist die Aussage wegen unbestimmtheit nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/869" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(115, 133, 197);"&gt;§ 869 ABGB&lt;/a&gt; ungütlig.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie kann ein auslegungsbedürftiger Vertrag mit der &lt;strong&gt;einfachen Vertragsinterpretation &lt;/strong&gt;ausgelegt werden?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Unter Rückgriff auf:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;den &lt;strong&gt;subjektiven Willen der Parteien&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;den &lt;strong&gt;Objektiven Wortlaut der Erklärung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;sowie die &lt;strong&gt;Übung des redlichen Verkehrs&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Welche 3 Quellen für Vertragsvereinbarungen gibt es?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;essentiala negotii&lt;/strong&gt; durch Parteieinigung&lt;/li&gt;&lt;li&gt;&lt;strong&gt;naturalia negotii&lt;/strong&gt; fügt das Gesetz hinzu&lt;/li&gt;&lt;li&gt;&lt;strong&gt;accidentalia negotii&lt;/strong&gt; können die Parteien weiters vereinbaren&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Folge von &lt;strong&gt;verstecktem &lt;/strong&gt;Dissens über die Nebenpunkte?&lt;/p&gt;&lt;p&gt;Wie wird gegebenenfalls eine derart entstandene Lücke gefüllt?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Es kommt drauf an, ob angenommen werden kann, dass der &lt;strong&gt;Vertrag auch ohne Einigung&lt;/strong&gt; über die &lt;strong&gt;offenen Nebepunkte geschlossen &lt;/strong&gt;worden wäre.&lt;/li&gt;&lt;li&gt;Dies ist idR der Fall, wenn die Nebenpunkte durch &lt;strong&gt;Gesetz oder Verkehrssitte&lt;/strong&gt; ergänzbar sind, und von den Parteien kein Vorbehalt diesbezüglich gemacht wurde.&lt;/li&gt;&lt;li&gt;Diese Lücke wird mittels &lt;strong&gt;dispositivem Recht&lt;/strong&gt; oder &lt;strong&gt;ergänzender Vertragsauslegung &lt;/strong&gt;gefüllt.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was wird höher gewertet, der &lt;strong&gt;erkennbare subjektive Wille&lt;/strong&gt; oder der &lt;strong&gt;objektive Wortlaut&lt;/strong&gt;, und &lt;strong&gt;warum&lt;/strong&gt;? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;Was sind die Folgen?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/914" rel="noopener noreferrer" target="_blank" style="background-color: yellow; color: black;"&gt;§§ 914f ABGB&lt;/a&gt; iVm &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank"&gt;§ 863 ABGB&lt;/a&gt; &lt;/p&gt;&lt;ul&gt;&lt;li&gt;Der erkennbare Subjektive Wille: Es ist die erkennbare Absicht der Parteien zu erforschen, Der Erklärungsempfänger hat den im objektiven Erklärungswert zum Ausdruck kommenden &lt;strong&gt;wahren subjektiven Willen&lt;/strong&gt; zu ermitteln.&lt;/li&gt;&lt;li&gt;Folge: Bei Verträgen gilt primär der übereinstimmende wahre Wille der Parteien, selbst wenn der Wortlaut davon abweicht. &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der hypothetische Parteiwillen?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Das, was die &lt;strong&gt;konkreten &lt;/strong&gt;Parteien &lt;strong&gt;vernünftigerweise&lt;/strong&gt; &lt;strong&gt;gewollt&lt;/strong&gt; &lt;strong&gt;hätten&lt;/strong&gt;, wenn ihnen die &lt;strong&gt;Unvollständigkeit &lt;/strong&gt;des &lt;strong&gt;Vertrages bewusst &lt;/strong&gt;gewesen wäre.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wie funktioniert die Lückenschließung durch &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;ergänzende Vertragsauslegung&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Verwendet:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;hypothetischen Parteiwillen&lt;/li&gt;&lt;li&gt;Übung des redlichen Verkehrs&lt;/li&gt;&lt;li&gt;Treu und Glauben&lt;/li&gt;&lt;li&gt;Verkehrsauffassung&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie funktioniert die Lückenschließung durch &lt;strong&gt;dispositives Recht&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Lücken sind durch &lt;strong&gt;gesetzliche Vorschriften&lt;/strong&gt; zu ergänzen&lt;/p&gt;&lt;ul&gt;&lt;li class="ql-indent-1"&gt;Außer es steht fest, dass die Parteien die Geltung des dispositiven Rechts &lt;strong&gt;nicht herbeiführen&lt;/strong&gt; wollten und &lt;strong&gt;dennoch keine Regelung&lt;/strong&gt; getroffen haben&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der Einfluss der &lt;strong&gt;Übung des redlichen Verkehrs&lt;/strong&gt; auf den objektiven Wortlaut?&lt;/p&gt;&lt;p&gt;Welche Elemente sind zu beachten?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Ist die Erklärung nicht eindeutig, so ist sie vom Empfänger entsprechend der &lt;strong&gt;Verkehrssitte&lt;/strong&gt;, also der Übung des redlichen Verkehrs zu verstehen.&lt;/li&gt;&lt;li&gt;Beachten:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Sprachgebrauch&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Art&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ort (z.B.: ortstypischer Dialekt)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Umstände (Verkehrskreis, Verbraucher, Unternehmer, ... )&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Rechtsgrundlage für die Auslegungsregeln für Verträge?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p class="ql-align-justify"&gt;&lt;span style="color: black; background-color: yellow;"&gt;§§ &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank" style="color: black; background-color: yellow;"&gt;863 Abs 2&lt;/a&gt;&lt;span style="color: black; background-color: yellow;"&gt;, &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/914" rel="noopener noreferrer" target="_blank" style="color: black; background-color: yellow;"&gt;914&lt;/a&gt;&lt;span style="color: black; background-color: yellow;"&gt;, &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/915" rel="noopener noreferrer" target="_blank" style="color: black; background-color: yellow;"&gt;915&lt;/a&gt;&lt;span style="color: black; background-color: yellow;"&gt; ABGB&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/ugb/paragraf/346" rel="noopener noreferrer" target="_blank" style="color: black; background-color: yellow;"&gt;§ 346 UGB&lt;/a&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wann darf eine zurechenbare Willenserklärung nicht angenommen werden?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wenn für den Empfänger zwar ein Vertrauenstatbestand vorlag, aber der Empfänger auf diese Handlung &lt;strong&gt;nicht vertraut&lt;/strong&gt; hat.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist &lt;strong&gt;fehlende Erklärungsbewusstsein&lt;/strong&gt; des Erklärenden?&lt;/p&gt;&lt;p&gt;Wann sind Erklärungen dennoch Zurechenbar?&lt;/p&gt;&lt;p&gt;Was hätte der Erklärende in dem Fall verhindern müssen?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Unbewusst abgegebene Erklärungen&lt;/li&gt;&lt;li&gt;Nur dann zurechenbar, wenn sich der Erklärende fahrlässig verhalten hat &lt;/li&gt;&lt;li&gt;Verhindern, dass diese Erklärungen/Handlungen vom &lt;strong&gt;gutgläubigen Dritten&lt;/strong&gt; als &lt;strong&gt;Willenserklärungen angesehen &lt;/strong&gt;werden &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(&lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(226, 148, 20);"&gt;Erklärungsfahrlässigkeit&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist ein objektiv-redlicher Erklärungsempfänger?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wer sich bemüht, richtig zu verstehen, was der Erklärende ausdrücken möchte&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die Bedeutungen der &lt;strong&gt;Willenstheorie&lt;/strong&gt;, &lt;strong&gt;Erklärungstheorie &lt;/strong&gt;und &lt;strong&gt;Vertrauenstheorie&lt;/strong&gt;, was ist bei der Erklärung Maßgebend?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Willenstheorie&lt;/strong&gt;: Wille des Erklärenden&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erklärungstheorie&lt;/strong&gt;: objektiver Wortlaut der Erklärung&lt;/li&gt;&lt;li&gt;Maßgebend: &lt;strong&gt;Vertrauenstheorie &lt;/strong&gt;(Abgeleitet von &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank"&gt;§ 863 ABGB)&lt;/a&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Die Erklärung aus der Sicht eines &lt;strong&gt;objektiv-redlichen Erklärungsempfängers&lt;/strong&gt;, alle Kenntnisse des wirklichen Empfängers, auch ungewöhnliche, inklusive. &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Worum geht es bei der Interpretation von Erklärungen und Verträgen?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Um die Ermittlung des Inhalts einer einzelnen Vertragsabschlusserklärung&lt;/li&gt;&lt;li&gt;Um die Ermittlung des Vertragsinhalts&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Folge von Dissens über Hauptpunkte?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;Ist es relevant ob offener oder versteckter Dissens?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/869" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 869 S2 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Kein Vertrag kommt zustande.&lt;/li&gt;&lt;li&gt;Unabhängig ob offener oder versteckter Dissens&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Welche 3 Arten des Dissens gibt es?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/869" rel="noopener noreferrer" target="_blank"&gt;§ 869 S2 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Dissens wegen Unvollständigkeit der Vereinbarung:&lt;/strong&gt; z.B.: Haupt oder Nebenpunkte sind offen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Dissens wegen Diskrepanz der Erklärungen&lt;/strong&gt;: Angebot- und Annahmeerklärung stimmen im Wortlaut nicht überein, und können auch durch Auslegung nicht zur Deckung gebracht werden&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Dissens wegen Mehrdeutigkeit oder Unverständlichkeit der Erklärungen&lt;/strong&gt;: Angebot und Annahme stimmen zwar im Wortlaut überein, sind aber objektiv mehrdeutig und werden von den Parteien unterschiedlich verstanden.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist &lt;strong&gt;versteckter &lt;/strong&gt;Dissens?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Zumindest eine Partei glaubt, dass in allen Punkten einigung erzielt wurde&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist &lt;strong&gt;offener &lt;/strong&gt;Dissens?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Beide Parteien wissen, dass sie sich noch nicht einig sind&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was kann (offener und versteckter) Dissens betreffen?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Haupt- oder Nebenpunkte im Vertrag&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Kann es Erklärungsirrtum bei natürlichem Konsens geben?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Nein, der Vertragsinhalt besteht nur aus dem subjektiven Willen beider Parteien (es gibt keinen objektiven Erklärungswert der abweichen könnte)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was wird höher bewertet, übereinstimmender subjektiver Wille, oder übereinstimmender objektiver Erklärungswert?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Der übereinstimmende Subjektive Wille, der objektive Erklärungswert kann nämliich irrtümlich vom subjektiven Willen des Anbieters abweichen.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Abgrenzung zwischen Konsens, Dissens und Erklärungsirrtum?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Konsens&lt;/strong&gt;: subjektiver Wille (der Parteien) oder objektiver Erklärungswert (der Erkärungen) stimmt überein.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Dissens&lt;/strong&gt;: Weder subjektiver Wille noch objektiver Erklärungswert stimmen überein&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erklärungsirrtum&lt;/strong&gt;: Der subjektive Wille einer Partei weicht vom objektiven Erklärungswert ab.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der objektive Erklärungswert? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Der in den Vertrag eingesetzte Wert (z.B.: Preis), kann &lt;strong&gt;irrtümlich&lt;/strong&gt; vom subjektiven Willen des Anbieters abweichen&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der normative Konsens?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Der Erklärungsempfänger vertraut auf den &lt;strong&gt;objektiven Erklärungswert&lt;/strong&gt;, aber der Vertragsinhalt entspricht nicht dem subjektiven Willen der anderen Partei (-&amp;gt; &lt;strong&gt;Fehler bei Angebotslegung&lt;/strong&gt;)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der natürliche Konsens?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Der innere Wille beider Parteien stimmt überein&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Inhaltskontrolle der AGB?&lt;/p&gt;&lt;p&gt;Was sind die drei Ebenen und deren Rechtsgrundlage?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Soll den Kunden vor überschießenden AGB Schützen -&amp;gt; die Unterlegenheit des Kunden ausgleichen. Diese zivilrechtliche Kontrolle wird durch eine vorhergehende aufsichtsbehördliche Genehmigung oder Kontrolle &lt;strong&gt;nicht &lt;/strong&gt;ausgeschlossen.&lt;/li&gt;&lt;li&gt;3 Ebenen:&lt;/li&gt;&lt;/ul&gt;&lt;ol&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Einbeziehungskontrolle&lt;/strong&gt;: Prüfung ob die AGB in ihrer Gesamtheit von den Parteien erhoben wurde (Parteieneinigung, z.B.: Unterschriften)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Geltungskontrolle&lt;/strong&gt;: Alle Einzelbestimmungen der AGB, die tatsächlich Vertragsinhalt geworden sind, werden der Geltungskontrolle unterzogen (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/864a" rel="noopener noreferrer" target="_blank"&gt;§ 864a ABGB&lt;/a&gt;). &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Inhaltskontrolle&lt;/strong&gt;: Verbleibende Klauseln (Kein Verstoß gegen &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/879" rel="noopener noreferrer" target="_blank"&gt;§ 879 Abs 3 &lt;/a&gt;und &lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/6" rel="noopener noreferrer" target="_blank"&gt;§ 6 KSchG&lt;/a&gt;)&lt;/li&gt;&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Einbeziehungskontrolle: Was ist für die Geltung von AGB erforderlich/für den Abschluss?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Soweit nicht durch Gesetz oder Verordnung anders angeordnet, gelten AGB nur kraft &lt;strong&gt;ausdrücklicher oder konkludenter Vereinbarung &lt;/strong&gt;der Parteien (Willenseinigung &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/861" rel="noopener noreferrer" target="_blank"&gt;§ 861 ABGB&lt;/a&gt;)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Geltungskontrolle: Was sind die Rechtsfolgen eines Verstoßes einer Klausel gegen § 864a ABGB?&lt;/p&gt;&lt;p&gt;Wann wird die Unwirksamkeit von Amts wegen geprüft, wann nur auf Einwand (des Unterworfenen)?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Klausel ist nicht Vertragsbestandteil&lt;/li&gt;&lt;li&gt;Der Restvertrag gilt &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(&lt;/span&gt;&lt;strong style="color: rgb(226, 148, 20); background-color: rgb(40, 45, 88);"&gt;Restgültigkeit des Vertrags&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;)&lt;/span&gt;, nur die Klausel selbst ist nichtig.&lt;/li&gt;&lt;li&gt;Erscheint die Klausel nach dem Verfahrensstadiums des Zivilprozesses &lt;strong&gt;nicht offenkundig&lt;/strong&gt; bedenklich, so wird die Unwirksamkeit nicht amtswegig sondern nur bei darauf gerichteter Einwendung geprüft.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie funktioniert die Geltungskontrolle der AGBs?&lt;/p&gt;&lt;p&gt;Welche 4 Tatbestandselemente sind notwendig?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;Jede konkrete Einzelklausel der AGB wird betrachtet&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;4 &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;kumulative &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;Tatbestandselemente für &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/864a" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 864a ABGB&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;:&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bestimmung ungewöhnlichen Inhalts&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nachteiligkeit für den Partner des Aufstellers&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Überraschungseffekt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Kein besonderer Hinweis des Aufstelleres auf die ungewöhnliche Klausel&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Inhaltskontrolle: Nichtigkeit gemäß &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/879" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 879 Abs 3&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;:&lt;/span&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Was sind die zwei Voraussetzungen?&lt;/li&gt;&lt;li&gt;Was ist die Rechtsfolge?&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Voraussetzungen: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Keine Hauptleistung (= Nebenbestimmungen)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gröbliche &lt;/strong&gt;Benachteiligung des Unterworfenen:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Bloße Benachteiligung reicht nicht aus.&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Gröblich z.B.: Verdünnte Willensfreiheit, oder AGB weichen von Wertung des objektiven dispositiven Rechts stark ab.&lt;/li&gt;&lt;li&gt;Klausel nicht Vertragsbestandteil, also nichtig.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Restvertrag gilt (&lt;strong&gt;Restgültigkeit des Vertrags&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Relative Nichtigkeit einer Klausel ist nur auf Einwendung wahrzunehmen.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind Entgeltliche/Unentgeltliche/Entgeltfremde Rechtsgeschäfte?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage für Entgeltliche Rechtsgeschäfte?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;entgeltlich&lt;/strong&gt;: immer Zweiseitig, jede Partei bringt die eigene Leistung um die Gegenleistung zu erhalten (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/917" rel="noopener noreferrer" target="_blank"&gt;§ 917 ABGB&lt;/a&gt;). Leistung muss nicht Geld sein.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;unentgeltlich&lt;/strong&gt;: Ein Partner erhält keine Gegenleistung (Schenkungsvertrag)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;entgeltsfremd&lt;/strong&gt;: liegen vor, wenn ein Bürge nachträglich einem existierenden Darlehensvertrag beitritt, ohne dass sich die Konditionen für den Hauptschuldner ändern.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie verhalten sich Individualvereinbarungen zu den AGB?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Spezielle Individualvereinbarungen, selbst mündliche, verdrängen die AGB.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie funktionieren die 3 Ebenen der Inhaltskontrolle in der Übersicht?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;&lt;li&gt;Scheitern AGB an Einbeziehungskontrolle -&amp;gt; &lt;strong&gt;Bedingungswerk &lt;/strong&gt;(gesamte AGB) wird nicht Teil des Vertrags &lt;/li&gt;&lt;li&gt;Scheitern einzelne Bestimmungen an der Geltungskontrolle, so sind nur diese Bestimmungen nichtig&lt;/li&gt;&lt;li&gt;Scheitern einzelne Bestimmungen an der Inhaltskontrolle, so sind nur diese nichtig&lt;/li&gt;&lt;li&gt;Alle übrigen Bestimmungen bleiben Vertragsinhalt.&lt;/li&gt;&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Inhaltskontrolle: Wie kann die Nichtigkeit von AGB für Verbraucher durchgesetzt werden? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;&lt;li&gt;&lt;strong&gt;Einzelprozess &lt;/strong&gt;(Auch ohne Vorbringen des Verbrauchers)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verbandsklage &lt;/strong&gt;von den Interessenverbänden &lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/28" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§§ 28-29 KSchG&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Abmahnung &lt;/strong&gt;-&amp;gt; Konventionalstrafe (&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/28" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 28 Abs 2 KSchG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Überschießende Klauseln &lt;/strong&gt;in AGB: Bei Verstoß gegen &lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/6" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 6 Abs 1 und 2 KSchG&lt;/a&gt; wird von der Fortgeltung der Klauseln ausgegangen, wenn sie (für den Konsumenten) vorteilhafte Bestimmungen enthalten.&lt;/li&gt;&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Inhaltskontrolle: Wie wird das Transparenzgebot &lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/6" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 6 Abs 3 KSchG&lt;/a&gt; verstanden?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Die Vertragsbestimmungen müssen den Verbraucher zuverlässig über seine Rechte und Pflichten informieren. Er soll möglichst &lt;strong&gt;durchschaubar, klar verständlich&lt;/strong&gt; und &lt;strong&gt;angepasst &lt;/strong&gt;an die Vertragsart so aufgeklärt werden, dass er &lt;strong&gt;nicht &lt;/strong&gt;von der &lt;strong&gt;Durchsetzung seiner Rechte abgehalten &lt;/strong&gt;wird, und ihm auch &lt;strong&gt;keine unberechtigten Pflichten auferlegt&lt;/strong&gt; werden.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Inhaltskontrolle: Abweichungen vom objektiven Recht&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Es wird nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/879" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 879 Abs 3&lt;/a&gt; &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;und &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/6" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 6 KSchG&lt;/a&gt; geprüft, ob Klauseln sachlich&lt;strong&gt; nicht gerechtfertigte unangemessene Abweichungen vom objektiven Recht&lt;/strong&gt; zulasten des unterworfenen enthalten.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Geltungskontrolle: Was ist der Überraschungseffekt (Überrumpelungs- bzw. Übertölpelungseffekt)&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Versteckte Klauseln die für den Unterworfenen überraschend sind.&lt;/li&gt;&lt;li&gt;Entfällt wenn diese Klauseln &lt;strong&gt;hervorgehoben &lt;/strong&gt;sind (fett, farbig, unterstrichen, ... ) oder &lt;strong&gt;mündlich &lt;/strong&gt;erklärt werden.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Entscheiden ist, ob dem Leser die ungewöhnliche Bestimmung aus dem Gesamteindruck der Urkunde auffällt.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Geltungskontrolle: Wann ist eine Bestimmung Nachteilig für den Partner des Aufstellers?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Weicht zulasten des Unterworfenen vom dispositiven objektiven Recht ab&lt;/li&gt;&lt;li&gt;Oder Stellt den Unterworfenen im Vergleich zum Aufsteller der AGB schlechter (aus der Sicht eines redlichen Vertragspartners)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Geltungskontrolle: Wie wird ungewöhnlicher Inhalt bestimmt?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Objektiv ungewöhnlich&lt;/strong&gt;: Wenn eine derartige Bestimmung in einem derartigen Vertrag üblicherweise (im redlichen Verkehr) nicht enthalten ist&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Subjektiv ungewöhnlich&lt;/strong&gt;:  Eine objektiv nicht ungewöhnliche Klausel kann subjektiv ungewöhnlich sein, wenn sie für den konkreten Vertragspartner im konkreten Zusammenhang, aus Sicht eines redlichen Aufstellers, überraschend sein musste und der Aufsteller nicht mit der Unterwerfung des Partners rechnen durfte.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Einbeziehungskontrolle: &lt;/span&gt;&lt;/p&gt;&lt;p&gt;Was sind kollidierende oder kreuzende AGB?&lt;/p&gt;&lt;p&gt;Was sind die Folgen?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Die AGB zweier Geschäftspartner sind punktuell nicht vereinbar&lt;/li&gt;&lt;li&gt;Folgen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Teildissens über die widersprüchlichen Punkte&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Die Beurteilung der Gültigkeit des Restvertrags folgt den Regeln über &lt;strong&gt;versteckten &lt;/strong&gt;und &lt;strong&gt;offenen &lt;/strong&gt;Dissens über Haupt- und Nebenpunkte.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nicht geregelte Punkte sind mit &lt;strong&gt;dispositivem Recht&lt;/strong&gt; und &lt;strong&gt;ergänzender Vertragsauslegung&lt;/strong&gt; zu ermitteln.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Einbeziehungskontrolle: &lt;/span&gt;&lt;/p&gt;&lt;p&gt;Wie kann ein Kunde den AGB zustimmen?&lt;/p&gt;&lt;p&gt;Können AGBs "Nachgeschoben" werden?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Ausdrücklich oder Konkludent&lt;/li&gt;&lt;li&gt;Einseitiges "Nachschieben" durch den Aufsteller der AGB &lt;strong&gt;reicht nicht&lt;/strong&gt; aus, eine &lt;strong&gt;Parteieneinigung &lt;/strong&gt;zur nachträglichen Einbeziehung von AGB ist &lt;strong&gt;aber nicht ausgeschlossen&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Einbeziehungskontrolle: &lt;/span&gt;Wie müssen AGB einbezogen werden?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;ausdrücklicher &lt;strong&gt;Hinweis reicht&lt;/strong&gt;: "ich verweise auf meine AGB" (AGB müssen nicht real vorliegen) &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die „Verdünnung der Willensfreiheit“ des Kunden?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Kunde kann "in der Schnelle" des Vertragsabschlusses den Inhalt umfangreicher AGB häufig nicht zur Kenntnis nehmen, oder ist sich der Reichweite nicht bewusst.&lt;/li&gt;&lt;li&gt;Kunde hat nur die Wahl die AGB Gesamt zu akzeptieren oder auf die Ware zu verzichten.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind AGB?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Allgemeine Geschäftsbedingungen sind vorformulierte standardisierte Vertragsbedingungen, die ein Vertragspartner für alle oder eine bestimmte Gruppe von Verträgen erstellt.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie funktioniert das Widerrufsrecht im Konsumentenschutz?&lt;/p&gt;&lt;p&gt;Was ist die Voraussetzung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Nach § 3 KSchG: Verbraucher hat das Recht Angebot &lt;strong&gt;bis Vertragsabschluss&lt;/strong&gt; durch einseitigen Widerruf zu zerstören.&lt;/p&gt;&lt;p&gt;Voraussetzung: Vertragserklärung außerhalb des Geschäftsraumes des Unternehmens.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wo finden sich gesetzliche Rücktrittsrechte außerhalb von KschG und FAGG?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;H&lt;span style="background-color: rgb(255, 255, 255); color: rgb(77, 81, 86);"&gt;ypothekar- und Immobilienkreditgesetz (&lt;/span&gt;&lt;a href="https://www.ris.bka.gv.at/GeltendeFassung.wxe?Abfrage=Bundesnormen&amp;amp;Gesetzesnummer=20009367" rel="noopener noreferrer" target="_blank" style="background-color: rgb(255, 255, 255); color: rgb(77, 81, 86);"&gt;§ 13 HIKrG&lt;/a&gt;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(77, 81, 86);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Verbraucherkreditgesetz (&lt;a href="https://www.jusline.at/gesetz/vkrg/paragraf/13" rel="noopener noreferrer" target="_blank"&gt;§ 13 VKrG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Teilnutzungsgesetz (&lt;a href="https://www.jusline.at/gesetz/tng/paragraf/8" rel="noopener noreferrer" target="_blank"&gt;§ 8 TNG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Bauträgervertragsgesetz (&lt;a href="https://www.jusline.at/gesetz/btvg/paragraf/5" rel="noopener noreferrer" target="_blank"&gt;§ 5 BTVG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;...&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die Voraussetzungen für einen Rücktritt von Fernabsatzverträgen?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/fagg/paragraf/11" rel="noopener noreferrer" target="_blank"&gt;§§ 11-18 FAGG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;§ 11 - Voraussetzungen&lt;/li&gt;&lt;li&gt;§ 18 - Kein Rücktrittsrecht&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die Voraussetzungen für einen Rücktritt wegen Nichteintritts maßgeblicher Umstände? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/3a" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 3a KschG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Maßgebliche Umstände treten nicht oder nur in erheblich geringerem Maß als vom Unternehmer dargestellt ein&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die Voraussetzungen für den Rücktritt vom Haustürgeschäft?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/3" rel="noopener noreferrer" target="_blank"&gt;§ 3 KschG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Weder in den vom &lt;strong&gt;Unternehmer für seine geschäftlichen Zwecke dauernd benützten Räumen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Noch bei&lt;strong&gt; einem von diesem dafür auf einer Messe oder einem Markt benützten Stand&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die 3 (wichtigsten) gesetzlichen Rücktrittsrechte des Käufers (insb. Verbrauchers)?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;&lt;li&gt;Rücktritt vom Haustürgeschäft&lt;/li&gt;&lt;li&gt;Rücktritt wegen Nichteintritts maßgeblicher Umstände&lt;/li&gt;&lt;li&gt;Rücktritt von Fernabsatzverträgen&lt;/li&gt;&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Option/Optionsvertrag?&lt;/p&gt;&lt;p&gt;Was die rechtlichen Folgen?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Eine Partei räumt der anderen, oder einem Dritten, das Recht ein (unabhängig von einer weiteren rechtsgeschäftlichen Erklärung des Verpflichteten), ein inhaltlich &lt;strong&gt;im Vorhinein bestimmtes Schuldverhältnis&lt;/strong&gt; in Geltung zu setzen&lt;/li&gt;&lt;li&gt;Rechtsfolge: Der Optionsberechtigte kann &lt;strong&gt;nach Ausübung der Option&lt;/strong&gt; unmittelbar die vertragliche Hauptleistung einklagen.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Punktation? Rechtliche Grundlagen?&lt;/p&gt;&lt;p&gt;Was sind die Voraussetzungen?&lt;/p&gt;&lt;p&gt;Was die rechtlichen Folgen? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/885" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 885 ABGB&lt;/a&gt;: Vorläufige (nicht formelle) verbindliche Fixierung der Hauptpunkte eines Vertrages -&amp;gt; Vertrag kommt zustande.&lt;/li&gt;&lt;li&gt;Voraussetzungen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Unterliegt der Schriftform (Schriftlich + Unterschrift), erfordert also Bindungswillen beider Parteien&lt;/li&gt;&lt;li&gt;Rechtsfolgen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Klage auf vertraglich geschuldete Leistungen möglich&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zeitlich nicht begrenzt (anders als Vorvertrag) -&amp;gt; normale Verjährungsjahre&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist ein Vorvertrag, was die gesetzliche Grundlage?&lt;/p&gt;&lt;p&gt;Wann und wie Lange ist er gültig?&lt;/p&gt;&lt;p&gt;Worauf kann geklagt werden?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/936" rel="noopener noreferrer" target="_blank"&gt;§ 936 ABGB&lt;/a&gt;: Vertrag über den künftigen Abschluss des von den Parteien in Aussicht genommenen Hauptvertrages.&lt;/li&gt;&lt;li&gt;Gilt nur:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Parteien haben sich über den wesentlichen Inhalt (z.B.: Ware und Preis) des Hauptvertrages geeinigt.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zeitpunkt für Hauptvertrag-Abschluss ist fixiert.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gilt max 1 Jahr&lt;/li&gt;&lt;li&gt;Klage nur auf Abschluss des Hauptvertrags, nicht auf Leistungen aus dem Hauptvertrag.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;ECG&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;E-Commerce-Gesetz&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Welche gesetzlichen Grundlagen regeln Vertragsabschluss im E-Commerce?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Elektronische Willenserklärung -&amp;gt; es gelten grundsätzlich die allgemeinen Regelungen &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/861" rel="noopener noreferrer" target="_blank"&gt;§§ 861ff ABGB&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/ecg/paragraf/10" rel="noopener noreferrer" target="_blank"&gt;§§ 10 -12 ECG&lt;/a&gt;: Sondervorschriften über &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Abgabe einer Vertragserklärung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vertragsbestimmungen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Geschäftsbedingungen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zugang elektronischer Erklärungen.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was regelt das FAGG?&lt;/p&gt;&lt;p&gt;Was ist in Bezug auf Vertragsschluss besonders zu beachten?&lt;/p&gt;&lt;p&gt;Welche gesetzlichen Grundlagen gibt es?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/fagg/paragraf/1" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§§ 1 - 11 FAGG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/fagg/paragraf/1" rel="noopener noreferrer" target="_blank"&gt;§ 1 Abs 1 FAGG&lt;/a&gt; -&amp;gt; Fern- und Auswärtsgeschäfte zwischen Unternehmern und Verbrauchern.&lt;/li&gt;&lt;li&gt;Beachten: Informationspflichten vor Vertragsschluss&lt;/li&gt;&lt;li&gt;Art und Umfang der Informationserteilung abhängig von Vertragstypen und Vertragsschlusssituation (§§ 4 - 9 FAGG)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;FAGG&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Fern- und Auswertsgeschäfte-Gesetz&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der Einfluss eines Kaufmännischen Bestätigungsschreiben auf einen Vertrag?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Grundsätzlich keine vertragsändernde Wirkung&lt;/li&gt;&lt;li&gt;Schweigen des Empfängers gilt nicht als Zustimmung zu Vertragsabschluss- oder Änderung, außer:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bestätigungsschreiben ergänzt bloß &lt;strong&gt;geringfügige Punkte&lt;/strong&gt;, die beim Vertragsabschluss &lt;strong&gt;bewusst von beiden Parteien&lt;/strong&gt; offen gelassen wurden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Empfänger wird &lt;strong&gt;nur begünstigt.&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine Kreuzofferte? &lt;/p&gt;&lt;p&gt;Was ist die Auswirkung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;"Überkreuzung" am Postweg: Zwei künftige Vertragspartner übermitteln einander Angebote auf An- und Verkauf derselben Sache die inhaltlich identisch sind.&lt;/li&gt;&lt;li&gt;Vertrag wird mit Zugang der letzten Offerte perfekt; wenn Parteirollen zusammenpassen (Verkäufer+Käufer)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist ein Angebot "ohne Obligo" (unverbindliches, freibleibendes Offert)?&lt;/p&gt;&lt;p&gt;Ist es gültig? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Beschränkung der Bindung an den Vertragsabschluss durch einseitige Annahme durch Klausel&lt;/li&gt;&lt;li&gt;Anbieter behält sich vor &lt;strong&gt;bis zur Annahme&lt;/strong&gt; durch Widerruf das Angebot zu zerstören&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Üblicherweise Widerruf nur bis Zugang bei Annehmenden, Klausel versucht also Widerrufzeitraum zu verlängern&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Frage: Darf der Anbieter das?&lt;/li&gt;&lt;li&gt;Im Zweifel nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/915" rel="noopener noreferrer" target="_blank"&gt;§ 915 ABGB&lt;/a&gt; vorgehen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Anbieter kann nach Zugang nicht mehr widerrufen, d.h. Angebot ist gar kein wirkliches Angebot da kein Bindungswille.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Annahmeerklärung des Annehmenden ist also eigentlich ein Angebot.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ursprünglicher Anbieter hat Redepflicht um abzulehnen, sonst kommt Vertrag nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/842a" rel="noopener noreferrer" target="_blank"&gt;§ 842a&lt;/a&gt; ABGB zustande&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was bedeutet "Protestatio facto contraria valet"?&lt;/p&gt;&lt;p&gt;Welche rechtlichen Fragen stellen sich daraus?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Protest entgegen den Fakten schadet nicht&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Fragen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Kann faktische Inanspruchnahme einer Leistung einen Vertrag zustandekommen lassen? &lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Auch wenn er klar äußert, dass er keinen Vertrag abschließen will? &lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Beispiel: Einsteigen in Öffentliches Verkehrsmittel, Benutzen von Parkplatz&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;Kann faktische Inanspruchnahme einer Leistung einen Vertrag zustandekommen lassen? &lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;Auch wenn er klar äußert, dass er keinen Vertrag abschließen will? &lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;Was bedeutet dies für "Protest entgegen den Fakten schadet nicht" in Ö? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank"&gt;§ 863 ABGB&lt;/a&gt;: Konkludente Handlung nur, wenn kein vernünftiger Grund daran zu zweifeln&lt;/li&gt;&lt;li&gt;Rechtslehre sagt: Nur ausdrückliche oder konkludente WE führt zu Vertrag&lt;/li&gt;&lt;li&gt;Daher bei Klarstellung das kein Wille zum Vertrag -&amp;gt; kein Vertrag&lt;/li&gt;&lt;li&gt;Zahlungen für Inanspruchnahme daher nicht aus Vertrag, aber z.B.: Bereicherungsrecht, Schadenersatzrecht.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;-&amp;gt; Protest gegen die Fakten schadet in Österreich!&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der unterschied zwischen "Angebot an unbekannte Person" und "invitatio ad offerendum"?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Angebot an unbekannt:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bindungswille: Verkäufer gibt zu erkennen das präsentierte, reale Waren zum Verkauf an jeden stehen, solange Vorrat reicht (z.B.: Getränkeautomat)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Kann idR durch Willensbetätigung angenommen werden (Annahmehandlung nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/864" rel="noopener noreferrer" target="_blank"&gt;§ 864 ABGB&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Konkreter Unterschied: &lt;strong&gt;Beschränkung des Angebotes auf den real vorhandenen Vorrat&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Invitatio ad offerendum: Erklärender will sich erkennbar nicht gegenüber jedermann binden (z.B.: Flugblatt, Katalog)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das Prinzip der kausalen Tradition (Lehre von Titel und Modus)? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/380" rel="noopener noreferrer" target="_blank"&gt;§ 380 ABGB&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/424" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(115, 133, 197);"&gt;§§ 424ff ABGB&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;, &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/1053" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(115, 133, 197);"&gt;§ 1053 ABGB&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;, &lt;/span&gt;&lt;/p&gt;&lt;p&gt;Zum Erwerb des Eigentumsrechts muss zum gültigen Verpflichtungsgeschäft (&lt;strong&gt;Titel&lt;/strong&gt;) auch ein Verfügungsgeschäft (&lt;strong&gt;Modus&lt;/strong&gt;) hinzutreten.&lt;/p&gt;&lt;p&gt;-&amp;gt; &lt;strong&gt;Man wird nicht bereits mit Abschluss des Kaufvertrages Eigentümer.&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie nennt man entgeltliche Rechtsgeschäfte noch? &lt;/p&gt;&lt;p&gt;Was ist die Bedeutung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Synallagmatische Verträge&lt;/li&gt;&lt;li&gt;Erbringt ein Teil seine Leistung nicht, muss auch der andere seine nicht erbringen&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die Schutznormen des KSchG? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/3" rel="noopener noreferrer" target="_blank"&gt;§ 3-6 KSchG&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/fagg/paragraf/11" rel="noopener noreferrer" target="_blank"&gt;§§ 11ff FAGG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Verbraucher kann von einem sog. Haustürgeschäft zurücktreten (grundlos innerhalb bestimmter Fristen) &lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; (§ 3 KSchG)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;besonderes Rücktrittsrecht &lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;(§ 3 KSchG, §§ 11ff FAGG)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Kostenvoranschlag gegenüber Verbraucher gilt als Garantie &lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; (§ 5 KSchG)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Bestimmte Klauseln in AGBs sind Unwirksam (§ 6 KSchG)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine Realofferte? Was die Rechtsgrundlage?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/864" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(136, 125, 220);"&gt;§ 864 Abs. 2 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Behalten, Verwenden, Verbrauchen einer Sache gilt nicht als Annahme eines Angebots, wenn sie dem Empfänger ohne dessen Veranlassung übersandt wurde.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Angebotsannahme: Rechtzeitigkeit der Annahme&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/862" rel="noopener noreferrer" target="_blank"&gt;§ 862 ABGB&lt;/a&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Angebot erlischt nach Geltungsdauer, diese muss eruiert werden:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Vom Erklärenden gesetzt (im Rahmen von &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/902" rel="noopener noreferrer" target="_blank"&gt;§§ 902f ABGB&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Sonst gesetzliche Frist nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/862" rel="noopener noreferrer" target="_blank"&gt;§ 862 S2 ABGB&lt;/a&gt; (inkl Postlauf des Angebots, Überlegungsfrist und Postlauf der Annahme)&lt;/li&gt;&lt;li&gt;Ausnahme &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/862a" rel="noopener noreferrer" target="_blank"&gt;§ 862a ABGB&lt;/a&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Verzögerung der nachweislich rechtzeitig abgesendeten Annahmeerklärung am Postweg (=Übermittlung)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Der Antragsteller kann aber &lt;strong&gt;unverzüglich &lt;/strong&gt;(ohne schuldhaftes Zögern) zurücktreten&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind Realakte?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Handlungen ohne Kundgabezweck die auch ohne Geschäftsfähigkeit und Rechtsfolgewillen Rechtsfolgen auslösen (z.B.: Urheberrechte durch Schaffen von Kunstwerk, Rechte und Pflichte durch Fund)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine Willensmitteilung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Willenshandlungen ohne Rechtsfolgewillen (z.B. Mahnung zeigt dass Zahlung erwünscht ist)&lt;/li&gt;&lt;li&gt;Rechtsfolgen treten unabhängig von Rechtsfolgewillen des Handelnden ein (z.B.: Mahnung bewirkt Fälligkeit)&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Willensmitteilung kann kein Angebot/Annahme sein.&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine Wissenserklärung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Nur auf Kundgabe von Fakten oder Kenntnissen gerichtet (Quittung, Mitteilung des Kontostantds, ... )&lt;/li&gt;&lt;li&gt;Vorschriften für Rechtsgeschäfte weitgehend auf &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wissenserklärung  angewandt, aber &lt;/span&gt;Angebot/Annahme durch &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wissenserklärung &lt;/span&gt;nicht möglich&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was kann eine stillschweigende/konkludente Willenserklärung sein?&lt;/p&gt;&lt;p&gt;Kann ein Unterlassen eine Willenserklärung sein? &lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Eindeutige Handlung nach Verkehrssitte ohne vernünftigen Grund daran zu zweifeln (z.B.: verzehren des aus dem Korb entnommenen Brots)&lt;/li&gt;&lt;li&gt;passives Unterlassen (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 863 ABGB&lt;/a&gt; ): Schweigen gilt nicht als Zustimmung, außer es besteht eine Redepflicht aus:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gesetz&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Verträgen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Übung des redlichen Verkehrs (z.B.: ständige Geschäftsverbindungen)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;vorvertragliche Aufklärungspflichten&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die 4 Voraussetzungen für die Annahme eines Angebots durch &lt;strong&gt;Willenserklärung&lt;/strong&gt;? Was ist die Rechtliche Grundlage?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/863" rel="noopener noreferrer" target="_blank"&gt;§ 863 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ol&gt;&lt;li&gt;Ausdrückliche oder konkludente Willenserklärung&lt;/li&gt;&lt;li&gt;Zugang der Willenserkärung&lt;/li&gt;&lt;li&gt;Rechtzeitigkeit der Annahme&lt;/li&gt;&lt;li&gt;Kein Widerruf der Annahme&lt;/li&gt;&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die 2 Grundvorraussetzungen für das Zustandekommen eines Vertrags? Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/861" rel="noopener noreferrer" target="_blank"&gt;§§ 861 ff ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Angebot + Annahme&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Rechtsfähigkeit?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;gibt jedem Rechtssubjekt die Macht, seine Belange (seine eigene Rechtssphäre) nach freiem Belieben zu regeln.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Willenserklärung: &lt;/span&gt;Rechtsfolgewille (Geltungswille)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Der Handelnde ist an seiner Erklärung gebunden, wenn er in dem Bewusstsein handelt, rechtliche verbindliche Handlungen zu setzen, die erforderlichenfalls mit staatlichen Zwang durchsetzbar sind (gemäßigte Rechtsfolgentheorie).&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Welches weitere Gesetz definiert Unternehmensformen die für die Auslegung des KSchG relevant sind?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;UGB 2007 (Unternehmensgesetzbuch)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind Verbrauchergeschäfte? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/1" rel="noopener noreferrer" target="_blank"&gt;§ 1 &lt;/a&gt;&lt;a href="https://www.jusline.at/gesetz/kschg/paragraf/1" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;KSchG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;: &lt;/span&gt;Wenn an einem zweiseitigen RG einerseits ein Unternehmer, für den das RG zum Betrieb seines Unternehmens gehört, und andererseits ein Verbraucher, auf den das nicht zutrifft, beteiligt -&amp;gt; Anwendung des KSchG &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind Abstrakte/Kausale Rechtsgeschäfte?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;abstrakt&lt;/strong&gt;: Wenn sich der Zweck (Rechtsgrund, causa) einer Verpflichtungserklärung nicht entnehmen lässt, sind idR ungültig.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;kausal&lt;/strong&gt;: wenn sich aus ihnen der Rechtsgrund entnehmen lässt&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind Verpflichtungs- und Verfügungsgeschäfte?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Verpflichtung&lt;/strong&gt;: geben dem Gläubiger einen schuldrechtlichen Anspruch (Forderung) auf Lieferung der Sache, aber noch kein dingliches (Eigentums-)Recht an der Sache. z.B: Käufer wird erst Eigentümer, wenn die Sache durch &lt;strong&gt;Verfügungsgeschäft &lt;/strong&gt;vom Verkäufer übergeben wird.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verfügung&lt;/strong&gt;: Führt die Verschiebung des (sachenrechtlichen) Eigentumsrecht von Verkäufer an Käufer herbei. &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind Ziel- und Dauerschuldverhältnisse?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ziel&lt;/strong&gt;: Ansprüche erlöschen durch die intendierte einmalige Leistungserbringung (Kaufvertrag: Lieferung + Bezahlung)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Dauer&lt;/strong&gt;: Wiederkehrende Leistungserbringung ohne Erlöschen&lt;strong&gt; &lt;/strong&gt;der Ansprüche ist vorgesehen (Strom, Zeitungsabo, unbefristeter Mietvertrag)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind Konsensualverträge/Realverträge?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Konsensual&lt;/strong&gt;: Kommen durch bloße Einigung zustande  (Kaufvertrag, Mietvertrag, ...)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Real&lt;/strong&gt;: Erfordert zum Abschluss auch Sachübergabe (Darlehensvertrag, Leihvertrag und Verwahrungsvertrag)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind Rechtsgeschäfte unter Lebenden, und von Todes wegen?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Lebenden&lt;/strong&gt;: Wirkung tritt zu Lebzeiten der Partner ein (Kaufvertrag, Mietvertrag, .. )&lt;/li&gt;&lt;li&gt;&lt;strong&gt;von Todes wegen&lt;/strong&gt;: Tritt nach dem Tod mindest einer Partei ein (Erbvertrag, Testament, ... )&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind empfangsbedürftige und nicht empfangsbedürftige Rechtesgeschäfte?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Testament nicht empfangsbedürftig&lt;/li&gt;&lt;li&gt;Kündigung, Angebotserklärung/Annahme, etc sind Empfangsbedürftig -&amp;gt; Empfangstheorie&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind Einseitig/Zweiseitig verpflichtende Rechtsgeschäfte?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Einseitig&lt;/strong&gt;: Nur ein Partner zur Leistung verpflichtet (Schenkung)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Zweiseitig &lt;/strong&gt;(ABGB nennt diese&lt;strong&gt; Gegenseitige Verträge&lt;/strong&gt;): Beide Seiten verpflichtet (Kaufvertrag, ... )&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind Ein-, Zwei- und mehrseitige Rechtsgeschäfte?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Differenzierung anhand der Anzahl der erforderlichen Willenserkärungen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ein&lt;/strong&gt;: Testament, Auslobung, Kündigung, ...&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Zwei&lt;/strong&gt;: Kaufvertrag, ...&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Mehr&lt;/strong&gt;: Gesellschaftsvertrag&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist ein Rechtsgeschäft im juristischen Sinn?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Ein Tatbestand, der aus einer oder mehreren Willensäußerungen von Rechtssubjekten besteht, an welche die Privatrechtsordnung den Eintritt von Rechtsfolgen knüpft.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wann begrenzen Drittwirkungen der Grundrechte die Privatautonomie?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Keine unmittelbare Drittwirkung der Grundrechte, aber:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Interpretation von Generalklauseln (z.B. Sittenwidrigkeit) können in die Interpretation privatrechtlicher Normen einfließen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Fiskalgeltung der Grundrechte: Gebietskörperschaften sind an die Grundrechte gebunden, auch wenn sie privatrechtlich Handeln. &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der Kontrahierungszwang? Wodurch kann er entstehen?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Zwang zum Vertragsabschluss&lt;/li&gt;&lt;li&gt;Entsteht durch:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gesetzliche Anordnung (z.B.: bei Monopol, Gefährdung der Nahversorgung)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Auch ohne ausdrückliche Gesetzliche Vorschrift bei faktischer Monopolstellung eines Vertragspartners (Nichtabschluss würde sonst rechtswidriges/sittenwidriges Verhalten darstellen)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Welche drei Arten der Grenzen der Privatautonomie gibt es?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Gesetzliche Vorschriften / zwingendes Recht&lt;/li&gt;&lt;li&gt;Begrenzung der Abschlussfreiheit durch Kontrahierungszwang&lt;/li&gt;&lt;li&gt;Drittwirkung der Grundrechte&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die 7 Inhalte der Privatautonomie?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Abschlussfreiheit (ob, wann und mit wem Vertrag geschlossen wird)&lt;/li&gt;&lt;li&gt;Inhaltsfreiheit&lt;/li&gt;&lt;li&gt;Typenfreiheit (neue Vertragstypen zu schaffen)&lt;/li&gt;&lt;li&gt;Beendigungsfreiheit&lt;/li&gt;&lt;li&gt;Änderungsfreiheit&lt;/li&gt;&lt;li&gt;Formfreiheit&lt;/li&gt;&lt;li&gt;Testierfreiheit (ob und wie der Verstorbene letztwillig testiert)&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;p&gt;Was ist die Interpretation?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Interpretation ist die&lt;strong&gt; Ermittlung des maßgeblichen Sinns&lt;/strong&gt; einer Rechtsnorm. &lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Der Rechtsanwender versucht den Sinn einer Vorschrift „richtig“ zu verstehen.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist der Allgemeine Teil des Zivilrechts?&lt;/p&gt;</t>
@@ -1372,7 +1438,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B162"/>
+  <dimension ref="A1:B173"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -2674,6 +2740,94 @@
         <v>323</v>
       </c>
     </row>
+    <row r="163" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Add cards for chapter 5
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
+++ b/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="378">
   <si>
     <t>Question</t>
   </si>
@@ -82,7 +82,7 @@
     <t>&lt;p&gt;Welche Rechtsgrundlagen für Fristen sind heranzuziehen, wenn weder Sondergesetze noch Parteien anders vereinbaren?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/902" rel="noopener noreferrer" target="_blank"&gt;§§ 902-904 ABGB&lt;/a&gt; und EuFrÜb (Europäisches Übereinkommen über die Berechnung von Frist)&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/902" rel="noopener noreferrer" target="_blank"&gt;§§ 902-904 ABGB&lt;/a&gt; und EuFrÜb (Europäisches Übereinkommen über die Berechnung von Fristen)&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist eine Befristung?&lt;/p&gt;&lt;p&gt;Was ist der Unterschied zur Bedingung? &lt;/p&gt;</t>
@@ -775,6 +775,114 @@
     <t>&lt;ul&gt;&lt;li&gt;Abschlussfreiheit (ob, wann und mit wem Vertrag geschlossen wird)&lt;/li&gt;&lt;li&gt;Inhaltsfreiheit&lt;/li&gt;&lt;li&gt;Typenfreiheit (neue Vertragstypen zu schaffen)&lt;/li&gt;&lt;li&gt;Beendigungsfreiheit&lt;/li&gt;&lt;li&gt;Änderungsfreiheit&lt;/li&gt;&lt;li&gt;Formfreiheit&lt;/li&gt;&lt;li&gt;Testierfreiheit (ob und wie der Verstorbene letztwillig testiert)&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
+    <t>&lt;p&gt;Was ist die &lt;strong&gt;Anspruchskonkurrenz &lt;/strong&gt;/ Anspruchsgrundlagenkonkurrenz ?&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was bedeutet dies für den Berechtigten?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ein Sonderfall der Alternativen Konkurrenz&lt;/li&gt;&lt;li&gt;Die alternativen Rechtsfolgen zielen alle auf einen identischen Leistungsinhalt ab.&lt;/li&gt;&lt;li&gt;Der Berechtigte darf frei wählen, auf welche Rechtsgrundlage er seinen Anspruch stützt, der Leistungsinhalt bleibt aber gleich. &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die &lt;strong&gt;Alternative Konkurrenz&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was bedeutet dies für den Berechtigten?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Der Berechtigte darf sich nur für eine der Alternativrechtsfolgen entscheiden &lt;/li&gt;&lt;li&gt;Entsprechend darf er nicht alle Ansprüche beanspruchen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die &lt;strong&gt;Kumulative Konkurrenz&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;Was bedeutet dies für den Berechtigten?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Einzelne &lt;strong&gt;Rechte &lt;/strong&gt;werden aus &lt;strong&gt;unterschiedlichen Gründen gewährt&lt;/strong&gt;, und bringen &lt;strong&gt;einander nicht&lt;/strong&gt; zum &lt;strong&gt;Erlöschen &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Der Berechtigte darf alle Ansprüche beanspruchen, man spricht von man spricht von &lt;strong&gt;Anspruchshäufung&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtsfolgenkonkurrenz?&lt;/p&gt;&lt;p&gt;Welche 3 Arten gibt es? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Wenn die &lt;strong&gt;Rechtsfolgen &lt;/strong&gt;mehrerer Normen &lt;strong&gt;prinzipiell vereinbar &lt;/strong&gt;sind, kommen die &lt;strong&gt;Normen nebeneinander &lt;/strong&gt;zur Anwendung.&lt;/li&gt;&lt;li&gt;Arten:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Kumulative Konkurrenz&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Alternative Konkurrenz&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Anspruchskonkurrenz / Anspruchsgrundlagenkonkurrenz&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann ist eine Norm spezieller als eine andere?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wenn sie mindestens ein&lt;strong&gt; zusätzliches Tatbestandsmerkmal &lt;/strong&gt;aufweist.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Gesetzeskonkurrenz?&lt;/p&gt;&lt;p&gt;Wie wird sie gelöst?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die Rechtsfolgen zweier oder mehrerer Tatbestände sind nicht vereinbar.&lt;/li&gt;&lt;li&gt;Gelöst durch Derogation (Ersetzen) oder aufgrund der Spezalität (speziellere Norm verdrängt die allgemeinere) &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann ist eine teleologische Reduktion notwendig?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wenn nach dem &lt;strong&gt;erkennbaren Sinn und Zweck&lt;/strong&gt; der Norm, gewisse &lt;strong&gt;Konstellationen nicht erfasst&lt;/strong&gt; sein sollen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Zweck der teleologischen Reduktion?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Einschränkung &lt;/strong&gt;des Anwendungsbereichs einer &lt;strong&gt;überschießend formulierten&lt;/strong&gt; &lt;strong&gt;Norm&lt;/strong&gt;. &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Rechtsfolge &lt;/strong&gt;wird für jene Sachverhalte &lt;strong&gt;ausgeschlossen&lt;/strong&gt;, die vom &lt;strong&gt;Sinn &lt;/strong&gt;und &lt;strong&gt;Zweck &lt;/strong&gt;der Norm &lt;strong&gt;nicht&lt;/strong&gt; &lt;strong&gt;erfasst &lt;/strong&gt;sein sollen.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die natürlichen Rechtsgrundsätze?&lt;/p&gt;&lt;p&gt;Wann werden sie angewendet?&lt;/p&gt;&lt;p&gt;Kommen sie häufig zum Einsatz?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrunldage? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Der Rückgriff auf die &lt;strong&gt;allgemeinen Wertprinzipien&lt;/strong&gt; die der gesamten Rechtsordnung zugrunde liegen.&lt;/li&gt;&lt;li&gt;Nach § 7 ABGB werden sie angewendet, wenn &lt;strong&gt;weder Gesetzes- noch Rechtsanalogie&lt;/strong&gt; zu einer &lt;strong&gt;Lösung &lt;/strong&gt;des Sachverhalts führen&lt;/li&gt;&lt;li&gt;Stellen die&lt;strong&gt; ultima ratio&lt;/strong&gt; (letztmöglicher Weg) dar, daher selten Angewendet.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann wird die teleologische Interpretation eingesetzt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;keine&lt;/strong&gt; &lt;strong&gt;Gesetzesmaterialien&lt;/strong&gt; zur Verfügung stehen.&lt;/li&gt;&lt;li&gt;der &lt;strong&gt;Regelungszweck&lt;/strong&gt; zwar &lt;strong&gt;festgestellt&lt;/strong&gt; werden kann,&lt;strong&gt; aber nicht mehr passend erscheint&lt;/strong&gt; und daher der aktuelle Regelungszweck ermittelt werden muss.&lt;/li&gt;&lt;li&gt;Konstellationen auftreten, die vom &lt;strong&gt;Regelungskonzept&lt;/strong&gt; des &lt;strong&gt;historischen Gesetzgebers nicht erfasst &lt;/strong&gt;und nicht bedacht waren.&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist der Größenschluss vom "Größeren" auf das "Kleinere"? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wenn der Gesetzgeber eine Rechtsfolge &lt;strong&gt;nicht einmal &lt;/strong&gt;für einen gewichtigeren „&lt;strong&gt;größeren&lt;/strong&gt;“ Fall vorgesehen hat, so gilt diese &lt;strong&gt;erst recht nicht &lt;/strong&gt;für einen weniger gewichtigen „&lt;strong&gt;kleineren&lt;/strong&gt;“ Fall.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die teleologische Interpretation?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Feststellung von &lt;strong&gt;Sinn &lt;/strong&gt;und &lt;strong&gt;Zweck &lt;/strong&gt;der Norm.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtsanalogie bzw. Gesamtanalogie?&lt;/p&gt;&lt;p&gt;Was ist der Unterschied zur Gesetzesanalogie?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Orientiert sich an einer &lt;strong&gt;Vielzahl von Normen&lt;/strong&gt;. Es wird ein &lt;strong&gt;allgemeines Prinzip abgeleitet&lt;/strong&gt; und auf den von der Rechtsordnung &lt;strong&gt;nicht geregelten Sachverhalt angewendet&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;Unterschied: Gesetzesanalogie verwendet einzelne Rechtsnorm&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Größenschluss vom "Kleineren" auf das "Größere"? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wenn der Gesetzgeber eine Rechtsfolge zwar nur für einen „&lt;strong&gt;kleineren&lt;/strong&gt;“ Fall &lt;strong&gt;vorgesehen &lt;/strong&gt;hat, aber der Zweck der Regelung auch den „größeren“ Fall erfasst, so gilt diese &lt;strong&gt;umso mehr&lt;/strong&gt; auch für den „&lt;strong&gt;größeren&lt;/strong&gt;“ Fall.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Gesetzesanalogie bzw. Einzelanalogie?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Lücke wird geschlossen, indem der &lt;strong&gt;Anwendungsbereich &lt;/strong&gt;einer Rechtsnorm auf einen&lt;strong&gt; noch nicht erfassten Sachverhalt&lt;/strong&gt; erstreckt wird. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Umkehrschluss zur planwidrigen Lücke?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Aus dem &lt;strong&gt;Fehlen &lt;/strong&gt;einer &lt;strong&gt;Regelung &lt;/strong&gt;wird abgeleitet, dass die in den &lt;strong&gt;vorhandenen&lt;/strong&gt; &lt;strong&gt;Bestimmungen vorgesehenen Rechtsfolgen &lt;/strong&gt;auf den &lt;strong&gt;nicht geregelten&lt;/strong&gt; Sachverhalt &lt;strong&gt;nicht angewendet&lt;/strong&gt; werden soll.&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann liegt eine planwidrige Lücke vor?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Eine Lücke liegt nur dann vor, wenn die vom Gesetzgeber getroffene Regelung &lt;strong&gt;unvollständig &lt;/strong&gt;und &lt;strong&gt;ergänzungsbedürftig &lt;/strong&gt;erscheint und, &lt;/li&gt;&lt;li&gt;wenn alle zur Verfügung stehenden &lt;strong&gt;Auslegungsmethoden &lt;/strong&gt;an ihre &lt;strong&gt;Grenzen &lt;/strong&gt;gestoßen sind, &lt;/li&gt;&lt;li&gt;der Sachverhalt also &lt;strong&gt;nicht &lt;/strong&gt;dem gesetzlichen &lt;strong&gt;Tatbestand &lt;/strong&gt;einer &lt;strong&gt;existierenden&lt;/strong&gt; &lt;strong&gt;Norm&lt;/strong&gt; &lt;strong&gt;unterstellt &lt;/strong&gt;werden kann.&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Analogie?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Analogie ist ein &lt;strong&gt;Ähnlichkeitsschluss&lt;/strong&gt;, bei dem eine vom Gesetzgeber &lt;strong&gt;ungewollte planwidrige Lücke &lt;/strong&gt;der Rechtsordnung &lt;strong&gt;geschlossen&lt;/strong&gt; wird. &lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Das heißt, Rechtsfolgen, die die Rechtsordnung für &lt;strong&gt;ähnliche Konstellationen &lt;/strong&gt;vorsieht, werden auf den &lt;strong&gt;planwidrig nicht &lt;/strong&gt;von der Regelung &lt;strong&gt;erfassten &lt;/strong&gt;Sachverhalt angewandt.&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Was ist das Verhältnis der Auslegungsmethoden zueinander?&lt;/p&gt;&lt;p&gt;Gibt es eine Reihenfolge?&lt;/p&gt;</t>
   </si>
   <si>
@@ -793,22 +901,10 @@
     <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/6" rel="noopener noreferrer" target="_blank"&gt;§§ 6, 7 ABGB&lt;/a&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Wann wird die teleologische Interpretation eingesetzt?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li class="ql-align-justify"&gt;&lt;strong&gt;keine Gesetzesmaterialien &lt;/strong&gt;zur Verfügung stehen.&lt;/li&gt;&lt;li class="ql-align-justify"&gt;der Regelungszweck zwar festgestellt werden kann, aber nicht mehr passend erscheint und daher&lt;strong&gt; der aktuelle Regelungszweck ermittelt werden muss.&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Konstellationen auftreten, die vom Regelungskonzept des &lt;strong&gt;historischen Gesetzgebers nicht erfasst und nicht bedacht waren.&amp;nbsp;&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die teleologische Interpretation?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Feststellung von &lt;strong&gt;Sinn &lt;/strong&gt;und &lt;strong&gt;Zweck &lt;/strong&gt;der Norm.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Wovon hängt der &lt;strong&gt;Bedeutungsgehalt &lt;/strong&gt;eines Wortes ab?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p class="ql-align-justify"&gt;Abhängig davon, ob ein &lt;strong&gt;allgemeiner&lt;/strong&gt;, &lt;strong&gt;fachspezifischer &lt;/strong&gt;oder &lt;strong&gt;rechtlicher&lt;/strong&gt; Sprachgebrauch herangezogen wird.&lt;/p&gt;</t>
+    <t>&lt;p&gt;Abhängig davon, ob ein &lt;strong&gt;allgemeiner&lt;/strong&gt;, &lt;strong&gt;fachspezifischer &lt;/strong&gt;oder &lt;strong&gt;rechtlicher &lt;/strong&gt;Sprachgebrauch herangezogen wird.&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist die Wortinterpretation?&lt;/p&gt;</t>
@@ -826,7 +922,7 @@
     <t>&lt;p&gt;Womit wird die Absicht des Gesetzgebers in der historischen Interpretation ermittelt?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p class="ql-align-justify"&gt;Mit den &lt;strong&gt;Gesetzesmaterialien&lt;/strong&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li class="ql-align-justify"&gt;Regierungsvorlagen&lt;/li&gt;&lt;li class="ql-align-justify"&gt;Ministerialentwürfe&lt;/li&gt;&lt;li class="ql-align-justify"&gt;Initiativanträge samt Erläuterungen&lt;/li&gt;&lt;li class="ql-align-justify"&gt;Kommissions- und Ausschussberichte&lt;/li&gt;&lt;li&gt;Stenographische Protokolle des Nationalrats&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;p class="ql-align-justify"&gt;Mit den &lt;strong&gt;Gesetzesmaterialien&lt;/strong&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Regierungsvorlagen&lt;/li&gt;&lt;li&gt;Ministerialentwürfe&lt;/li&gt;&lt;li&gt;Initiativanträge samt Erläuterungen&lt;/li&gt;&lt;li&gt;Kommissions- und Ausschussberichte&lt;/li&gt;&lt;li&gt;Stenographische Protokolle des Nationalrats&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Wann erlischt ein Angebot?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
@@ -1438,7 +1534,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B173"/>
+  <dimension ref="A1:B189"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -2828,6 +2924,134 @@
         <v>345</v>
       </c>
     </row>
+    <row r="174" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Add cards for chapter 3
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
+++ b/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="412">
   <si>
     <t>Question</t>
   </si>
@@ -19,6 +19,90 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;Was ist die Systematik einer OGH Entscheidung?&lt;/p&gt;&lt;p&gt;Beispiel: &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;8 Ob 14/17t&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;8 Ob 14/17t&lt;/span&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;8: Senat&lt;/li&gt;&lt;li&gt;O: Oberster Gerichtshof&lt;/li&gt;&lt;li&gt;b: bürgerlich-rechtliche Angelegenheiten&lt;/li&gt;&lt;li&gt;14: fortlaufende Nummer des Geschäftsfalls&lt;/li&gt;&lt;li&gt;17: Jahr des Einlangens einer Rechtssache beim OGH&lt;/li&gt;&lt;li&gt;T: bei neueren Entscheidungen wird ein Prüfzeichen nachgestellt&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;In welchem Fall kommt Case Law in Österreich zum Einsatz?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/oghg/paragraf/8" rel="noopener noreferrer" target="_blank"&gt;§ 8 OGHG&lt;/a&gt;: &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Entscheidungen eines verstärkten Senats &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Richterrecht: Was ist Case Law?&lt;/p&gt;&lt;p&gt;Wie verhält es sich in den USA und in Österreich?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage in Ö? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Entscheidung eines Falles schaft für zukünftige Fälle &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;gültiges Recht&lt;/span&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;USA: Kommt oft zur Anwendung.&lt;/li&gt;&lt;li&gt;Ö: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Richterrecht ist &lt;strong&gt;keine Rechts&lt;/strong&gt;(entstehungs)&lt;strong&gt;quelle&lt;/strong&gt; (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/12" rel="noopener noreferrer" target="_blank"&gt;§ 12 ABGB&lt;/a&gt;), Gerichte wenden Recht an und schaffen es nicht.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Gewohnheitsrecht bzw. wodurch entsteht es?&lt;/p&gt;&lt;p&gt;Ist es ein gesetztes Recht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ensteht durch &lt;strong&gt;lange&lt;/strong&gt; und &lt;strong&gt;gleichmäßige &lt;/strong&gt;und &lt;strong&gt;allgemeine getätigte Übung &lt;/strong&gt;eines bestimmten Verhaltens mit &lt;strong&gt;Rechtsüberzeugung&lt;/strong&gt;. Die Rechtsunterworfenen sind überzeugt davon, rechtlich dazu verpflichtet zu sein.&lt;/li&gt;&lt;li&gt;Nein, es ist nicht niedergeschrieben.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist nachgiebiges Recht?&lt;/p&gt;&lt;p&gt;Wie wird es noch genannt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Kann durch Parteienvereinbarung geändert werden, bleibt aber dort Anwendbar, wo die Vereinbarung &lt;strong&gt;ergänzungsbedürftig &lt;/strong&gt;ist.&lt;/li&gt;&lt;li&gt;Dispositives Recht&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist relativ zwingendes Recht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Kann durch &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Parteienvereinbarung  nur &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;nicht&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;zum Nachteil &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;des &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;besonders Geschützten &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;abgeändert werden. (z.B.: Mietrecht, Normen können zugunsten des Mieters geändert werden)&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist absolut zwingendes Recht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Kann durch Parteienvereinbarung nicht abgeändert werden.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist formelles Recht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Regelt den &lt;strong&gt;Ablauf des Verfahrens &lt;/strong&gt;der Rechtsdurchsetzung vor den staatlichen Behörden (StPO, ... )&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist materielles Recht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Setzt sich mit der &lt;strong&gt;inhaltlichen Ordnung&lt;/strong&gt; des menschlichen Zusammenlebens auseinander (KSchG, PHG, ... )&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche drei Dimensionen der Geltung gibt es für eine Rechtsnorm?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Zeit&lt;/strong&gt;: Die Geltung einer Rechtsnorm beginnt mit dem Tag folgend&lt;strong&gt; &lt;/strong&gt;auf die Freigabe im Bundesgesetzblatt im RIS oder an dem für die Geltung festgesetzten Zeitpunkt. &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Raum (Territorialitätsprinzip):&lt;/strong&gt; Die Geltung einer Norm beschränkt sich auf den Staat in dem die Norm geschaffen wurde &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Kenntnis &lt;/strong&gt;(&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/2" rel="noopener noreferrer" target="_blank"&gt;§ 2 ABGB&lt;/a&gt;): Die Geltung ist &lt;strong&gt;nicht&lt;/strong&gt; von der Kenntnis des Rechtsunterworfenen abhängig.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Internationale Privatrecht?&lt;/p&gt;&lt;p&gt;Welches österr. Gesetz regelt dies in Ö?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Wenn ein &lt;strong&gt;Sachverhalt Auslandsberührung &lt;/strong&gt;aufweist und &lt;strong&gt;kein&lt;/strong&gt; &lt;strong&gt;Einheitsprivatrecht&lt;/strong&gt; existiert.&lt;/li&gt;&lt;li&gt;Enthält das Kollionsrecht, und regelt welche nationale Rechtsordnung auf einen internationalen Sachverhalt angwenedet wird. &lt;/li&gt;&lt;li&gt;Das Bundesgesetz über das internationale Privatrecht (IPRG)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Einheitsprivatrecht?&lt;/p&gt;&lt;p&gt;Was ist die wichtigste Materie darin?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Entsteht durch den Abschluss von Staatsverträgen, enthält staatenübergreifende einheitliche Regelungen.&lt;/li&gt;&lt;li&gt;Wichtigste Materie: UN-KaufR (Übereinkommen der UN über Verträge über den Internationalen Warenkauf)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann können EU Richtlinien unmittelbar (auf/zwischen Bürgern) wirken?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wenn:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Die unmittelbare Wirkung &lt;strong&gt;zugunsten &lt;/strong&gt;der Rechtsunterworfenen ist&lt;/li&gt;&lt;li&gt;Inhaltlich &lt;strong&gt;unbedingt &lt;/strong&gt;und &lt;strong&gt;hinreichend genau &lt;/strong&gt;determiniert sind&lt;/li&gt;&lt;li&gt;Die &lt;strong&gt;Transformationsfrist abgelaufen &lt;/strong&gt;ist&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann kann das EU Primärrecht unmittelbar&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; (auf/zwischen Bürgern) &lt;/span&gt;Bürgern wirken?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wenn es:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Rechtlich &lt;strong&gt;vollkommen &lt;/strong&gt;ist&lt;/li&gt;&lt;li&gt;&lt;strong&gt;unbedingt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Keine weiteren Vollzugsmaßnahmen &lt;/strong&gt;erfordert&lt;/li&gt;&lt;li&gt;Mitgliedsstaaten &lt;strong&gt;keinen Entscheidungsspielraum &lt;/strong&gt;haben&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Was ist die historische Interpretation?&lt;/p&gt;</t>
   </si>
   <si>
@@ -773,6 +857,24 @@
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;Abschlussfreiheit (ob, wann und mit wem Vertrag geschlossen wird)&lt;/li&gt;&lt;li&gt;Inhaltsfreiheit&lt;/li&gt;&lt;li&gt;Typenfreiheit (neue Vertragstypen zu schaffen)&lt;/li&gt;&lt;li&gt;Beendigungsfreiheit&lt;/li&gt;&lt;li&gt;Änderungsfreiheit&lt;/li&gt;&lt;li&gt;Formfreiheit&lt;/li&gt;&lt;li&gt;Testierfreiheit (ob und wie der Verstorbene letztwillig testiert)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Sekunddärrecht im Europäischen Recht?&lt;/p&gt;&lt;p&gt;Welche zwei Arten gibt es?&lt;/p&gt;&lt;p&gt;Worauf wirken sie?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;EU &lt;strong&gt;Verordnungen&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Sind sofort für die &lt;strong&gt;Mitgliedstaaten&lt;/strong&gt; und deren &lt;strong&gt;Bürger &lt;/strong&gt;gültig, es muss &lt;strong&gt;kein nationales Gesetz&lt;/strong&gt; erlassen werden.&lt;/li&gt;&lt;li&gt;EU &lt;strong&gt;Richtlinien&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Richten sich &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;idR&lt;/span&gt; an die Mitgliedstaaten, nicht die Bürger&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nationale Parlamente führen eine &lt;strong&gt;Transformation&lt;/strong&gt; in nationales Recht durch. Für die Bürger gilt das nationale Gesetz nicht die Richtlinie.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Primärrecht im Europäischen Recht?&lt;/p&gt;&lt;p&gt;Auf wen wirkt es?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Durch die Mitgliedstaaten unterzeichnete Beitrittsverträge.&lt;/p&gt;&lt;p&gt;Wirkt primär auf die Mitgliedstaaten, idR nicht unmittelbar auf die Bürger&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die zentrale Rechtsquelle des Privatrechts im Österreichischen Recht?&lt;/p&gt;&lt;p&gt;Wer sind die Gesetzgebungsorgane?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die Österreichische Rechtsordnung&lt;/li&gt;&lt;li&gt;Das Parlament und die Landtage&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist die &lt;strong&gt;Anspruchskonkurrenz &lt;/strong&gt;/ Anspruchsgrundlagenkonkurrenz ?&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was bedeutet dies für den Berechtigten?&lt;/span&gt;&lt;/p&gt;</t>
@@ -1534,7 +1636,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B189"/>
+  <dimension ref="A1:B206"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -3052,6 +3154,142 @@
         <v>377</v>
       </c>
     </row>
+    <row r="190" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>411</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Add cards for chapter 6
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
+++ b/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="460">
   <si>
     <t>Question</t>
   </si>
@@ -19,6 +19,150 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;Was ist die Testierfähigkeit?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Fähigkeit über ein Testament über die Erbnachfolge zu verfügen.&lt;/li&gt;&lt;li&gt;Legaldefinition siehe &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/566" rel="noopener noreferrer" target="_blank"&gt;§ 566 ABGB&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Ehefähigkeit?&lt;/p&gt;&lt;p&gt;Was sind die Voraussetzungen?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die Fähigkeit, einen Ehevertrag abschließen zu können.&lt;/li&gt;&lt;li&gt;Vorrausetzungen: Volljährigkeit und Entscheidungsfähigkeit &lt;a href="https://www.jusline.at/gesetz/eheg/paragraf/1" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(136, 125, 220);"&gt;§ 1 Abs 1 EheG&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wird die Handlungsfähigkeit einer vertretenen Person eingeschränkt?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;gem &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/242" rel="noopener noreferrer" target="_blank"&gt;§ 242 AGBG&lt;/a&gt; nicht eingeschränkt&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Rechtsgrundlage für die gerichtliche Erwachsenenvertretung?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/271" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§§ 271ff ABGB&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Rechtsgrundlage für die gesetzliche Erwachsenenvertretung?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/268" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§§ 268ff ABGB&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtsgrundlage für gewählte Erwachsenenvertretung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/264" rel="noopener noreferrer" target="_blank"&gt;§§ 264ff ABGB&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die gesetzlichen Altersgrenzen für das &lt;strong&gt;schrittweise Entstehen der&lt;/strong&gt; &lt;strong&gt;Geschäftsfähigkeit&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;Welche Geschäftsfähigkeiten hat das Rechtssubjekt jeweils?&lt;/p&gt;&lt;p&gt;Was ist die jeweilige Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kinder&lt;/strong&gt;: 0-7 Jahre: völlig Geschäfts&lt;strong&gt;unfähig&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ausnahme: &lt;/li&gt;&lt;li class="ql-indent-2"&gt;"übliche Geschäfte" &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/170" rel="noopener noreferrer" target="_blank"&gt;§ 170 Abs 3 ABGB&lt;/a&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Schenkungen annehmen &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/865" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 865 Abs 2 ABGB&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Unmündige Minderjährige&lt;/strong&gt;: 7-14 Jahre: &lt;strong&gt;beschränkt &lt;/strong&gt;Geschäftsfähig &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Besitzerwerb &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/310" rel="noopener noreferrer" target="_blank"&gt;§ 310 ABGB&lt;/a&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ausnahmen wie Kind&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Mündige Minderjährige&lt;/strong&gt;: 14-18 Jahre: &lt;strong&gt;beschränkt &lt;/strong&gt;Geschäftsfähig &lt;/li&gt;&lt;li class="ql-indent-1"&gt;freie Verfügung über Einkommen und überlassene Sachen &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/170" rel="noopener noreferrer" target="_blank"&gt;§ 170 Abs 2 ABGB&amp;nbsp;&lt;/a&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;selbständig zu Dienstleistungen verpflichten &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/171" rel="noopener noreferrer" target="_blank"&gt;§ 171 ABGB&lt;/a&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Medizinische Entscheidungen &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/173" rel="noopener noreferrer" target="_blank"&gt;§ 173 ABGB&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Volljährige&lt;/strong&gt;: über 18 Jahre:  &lt;strong&gt;Voll &lt;/strong&gt;Geschäftsfähig &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/865" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 865 Abs 1 ABGB&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Deliktfähigkeit? &lt;/p&gt;&lt;p&gt;Wann beginnt sie, was ist die Rechtsgrundlage?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage für die &lt;strong&gt;Schadenshaftung &lt;/strong&gt;in dem Zusammenhang? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Fähigkeit, durch &lt;strong&gt;eigenes schuldhaftes Verhalten Schadenersatzpflichten &lt;/strong&gt;zu begründen.&lt;/li&gt;&lt;li&gt;Beginnt mit Vollendung des 14. Lebensjahres gem. &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/176" rel="noopener noreferrer" target="_blank"&gt;§ 176 ABGB &lt;/a&gt;&lt;/li&gt;&lt;li&gt;Haftung: &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/1307" rel="noopener noreferrer" target="_blank"&gt;§§ 1307-1310 ABGB&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie werden Geschäfte aus der Zeit vor der Volljährigkeit wirksam?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Müssen schriftlich anerkannt werden &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/168" rel="noopener noreferrer" target="_blank"&gt;§ 168 ABGB&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Rechtsgrundlagen sind Relevant für die gesetzliche Vertretung bei altersbedingter Geschäftsunfähigkeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;§§ &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/158" rel="noopener noreferrer" target="_blank"&gt;158&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/167" rel="noopener noreferrer" target="_blank"&gt;167&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/177" rel="noopener noreferrer" target="_blank"&gt;177&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/178" rel="noopener noreferrer" target="_blank"&gt;178&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/181" rel="noopener noreferrer" target="_blank"&gt;181 &lt;/a&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;ABGB&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche zwei Arten der Geschäftsunfähigkeit gibt es? &lt;/p&gt;&lt;p&gt;Was sind die Folgen? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Geschäftsunfähigkeit &lt;strong&gt;mangels ausreichenden&lt;/strong&gt; &lt;strong&gt;Alters&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Führt zu &lt;strong&gt;gesetzlicher&lt;/strong&gt; &lt;strong&gt;Vertretung &lt;/strong&gt;(z.B.: Eltern)&lt;/li&gt;&lt;li&gt;Geschäftsunfähigkeit &lt;strong&gt;mangels&lt;/strong&gt; &lt;strong&gt;ausreichenden&lt;/strong&gt; &lt;strong&gt;Geisteszustandes&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Führt zu &lt;strong&gt;Vorsorgebevollmächtigtem &lt;/strong&gt;bzw &lt;strong&gt;Erwachsenenvertreter &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Geschäftsfähigkeit?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;&lt;p&gt;Was ist die Vorraussetzung, wann wird diese vermutet? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Legaldefinition siehe &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/865" rel="noopener noreferrer" target="_blank"&gt;§ 865 ABGB&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Voraussetzung ist Entscheidungsfähigkeit, wird bei Volljährigen vermutet.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Handlungsfähigkeit?&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Rechtsgrundlage?&lt;/span&gt;&lt;/p&gt;&lt;p&gt;Wer ist in der Regel voll Handlungsfähig?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Legaldefinition siehe &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/24" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 24 Abs 1 ABGB&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Voll Handlungsfähig: &lt;strong&gt;Geistig&lt;/strong&gt; &lt;strong&gt;gesunde&lt;/strong&gt; &lt;strong&gt;Erwachsene&lt;/strong&gt;, die &lt;strong&gt;bewusstes&lt;/strong&gt;, vom &lt;strong&gt;eigenen&lt;/strong&gt; &lt;strong&gt;Willen&lt;/strong&gt; &lt;strong&gt;gesteuertes &lt;/strong&gt;Verhalten an den Tag legen.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie muss die Entscheidungsfähigkeit beurteilt werden? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Situationsbezogen&lt;/strong&gt;, &lt;strong&gt;personenbezogen&lt;/strong&gt;, &lt;strong&gt;anlassbezogen &lt;/strong&gt;auf die jeweils maßgebende Materie.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann fehlt die Entscheidungsfähigkeit einer Person jedenfalls?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Bei &lt;strong&gt;psychischer&lt;/strong&gt; &lt;strong&gt;Krankheit &lt;/strong&gt;oder &lt;strong&gt;vergleichbarer&lt;/strong&gt; &lt;strong&gt;Bewusstseinsstörung &lt;/strong&gt;(geistige Behinderung, Koma, ... )&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Entscheidungsfähigkeit?&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Rechtsgrundlage?&lt;/span&gt;&lt;/p&gt;&lt;p&gt;Wofür ist sie Vorraussetzung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Legaldefinition siehe &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/24" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 24 Abs 2 ABGB&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;Voraussetzung für &lt;/span&gt;&lt;strong style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;rechterhebliches Handeln&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Haben ungeborene (nasciturus) Rechtsfähigkeit?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Bedingte und beschränkte Teilrechtsfähigkeit nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/22" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;§ 22 ABGB&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Kommorientenpräsumtion?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/teg/paragraf/11" rel="noopener noreferrer" target="_blank"&gt;§ 11 TEG&lt;/a&gt;&lt;/p&gt;&lt;p&gt;Lässt sich nicht feststellen, wer zuerst gestorben ist, so wird vermutet dass sie zugleich gestorben sind.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie läuft das Todeserklärungsverfahren ab?&lt;/p&gt;&lt;p&gt;Was passiert wenn der Todeszeitpunkt nicht festgestellt werden kann, was ist die Rechtsgrundlage dafür?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Eingeleitet über &lt;strong&gt;Antrag &lt;/strong&gt;eines Interessenten (z.B.: Ehegatten) und endet mit &lt;strong&gt;richterlichem Beschluss&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/teg/paragraf/23" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;§ 23 TEG&lt;/a&gt; der wahrscheinlichste Zeitpunkt wird festgelegt&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann endet die Rechtsfähigkeit?&lt;/p&gt;&lt;p&gt;Welche zwei Optionen gibt es?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Mit dem Tod.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Tod &lt;/strong&gt;im medizinischen/juristischen Sinn: &lt;strong&gt;Hirntot&lt;/strong&gt;, Gehirnströme &lt;strong&gt;irreversibel &lt;/strong&gt;und &lt;strong&gt;vollständig &lt;/strong&gt;erloschen (auch bei künstlicher Aufrechterhaltung ist Rechtsfähigkeit erloschen)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Todeserklärung des Verschollenen&lt;/strong&gt; nach dem Todeserklärungsgesetz (&lt;a href="https://www.jusline.at/gesetz/teg/paragraf/1" rel="noopener noreferrer" target="_blank"&gt;§ 1 TEG&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Voraussetzungen der Todeserklärung nach &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/teg/paragraf/3" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(115, 133, 197);"&gt;§§ 3-8 TEG&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann beginnt die Rechtsfähigkeit?&lt;/p&gt;&lt;p&gt;Was sind die Rechtlichen Grundlagen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Beginnt mit &lt;strong&gt;vollendeter Lebendgeburt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/hebg/paragraf/8" rel="noopener noreferrer" target="_blank"&gt;§ 8 HebG&lt;/a&gt; unterscheidet Lebend von Totgeburt&lt;/li&gt;&lt;li&gt;Im Zweifel lebendgeburt vermutet: &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/23" rel="noopener noreferrer" target="_blank"&gt;§ 23 ABGB&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtsfähigkeit?&lt;/p&gt;&lt;p&gt;Wie lange hält sie an?&lt;/p&gt;&lt;p&gt;Was ist die Gesetzliche Grundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Fähigkeit Träger von Rechten und Pflichten zu sein&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/16" rel="noopener noreferrer" target="_blank"&gt;§ 16 ABGB&lt;/a&gt;: Lebenslänglich&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Rechtsobjekte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Gegenstand der Rechte (eines Rechtssubjekts) bzw des Rechtsverkehrs&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Rechtssubjekte?&lt;/p&gt;&lt;p&gt;Welche Arten gibt es?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Träger von Rechten und Pflichten (&lt;strong&gt;rechtsfähig&lt;/strong&gt;)&lt;/li&gt;&lt;li&gt;Natürliche Personen und juristische Personen (GmbH, Gebietskörperschaft, ... )&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Was ist die Systematik einer OGH Entscheidung?&lt;/p&gt;&lt;p&gt;Beispiel: &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;8 Ob 14/17t&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
@@ -82,7 +226,7 @@
     <t>&lt;p&gt;Was ist das Internationale Privatrecht?&lt;/p&gt;&lt;p&gt;Welches österr. Gesetz regelt dies in Ö?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;Wenn ein &lt;strong&gt;Sachverhalt Auslandsberührung &lt;/strong&gt;aufweist und &lt;strong&gt;kein&lt;/strong&gt; &lt;strong&gt;Einheitsprivatrecht&lt;/strong&gt; existiert.&lt;/li&gt;&lt;li&gt;Enthält das Kollionsrecht, und regelt welche nationale Rechtsordnung auf einen internationalen Sachverhalt angwenedet wird. &lt;/li&gt;&lt;li&gt;Das Bundesgesetz über das internationale Privatrecht (IPRG)&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;ul&gt;&lt;li&gt;Wenn ein &lt;strong&gt;Sachverhalt Auslandsberührung &lt;/strong&gt;aufweist und &lt;strong&gt;kein&lt;/strong&gt; &lt;strong&gt;Einheitsprivatrecht&lt;/strong&gt; existiert.&lt;/li&gt;&lt;li&gt;Enthält das Kollionsrecht, und regelt welche nationale Rechtsordnung auf einen internationalen Sachverhalt angewendet wird.&lt;/li&gt;&lt;li&gt;Das Bundesgesetz über das internationale Privatrecht (IPRG)&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist das Einheitsprivatrecht?&lt;/p&gt;&lt;p&gt;Was ist die wichtigste Materie darin?&lt;/p&gt;</t>
@@ -97,7 +241,7 @@
     <t>&lt;p&gt;Wenn:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Die unmittelbare Wirkung &lt;strong&gt;zugunsten &lt;/strong&gt;der Rechtsunterworfenen ist&lt;/li&gt;&lt;li&gt;Inhaltlich &lt;strong&gt;unbedingt &lt;/strong&gt;und &lt;strong&gt;hinreichend genau &lt;/strong&gt;determiniert sind&lt;/li&gt;&lt;li&gt;Die &lt;strong&gt;Transformationsfrist abgelaufen &lt;/strong&gt;ist&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Wann kann das EU Primärrecht unmittelbar&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; (auf/zwischen Bürgern) &lt;/span&gt;Bürgern wirken?&lt;/p&gt;</t>
+    <t>&lt;p&gt;Wann kann das EU Primärrecht unmittelbar&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; (auf/zwischen Bürgern) &lt;/span&gt;wirken?&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Wenn es:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Rechtlich &lt;strong&gt;vollkommen &lt;/strong&gt;ist&lt;/li&gt;&lt;li&gt;&lt;strong&gt;unbedingt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Keine weiteren Vollzugsmaßnahmen &lt;/strong&gt;erfordert&lt;/li&gt;&lt;li&gt;Mitgliedsstaaten &lt;strong&gt;keinen Entscheidungsspielraum &lt;/strong&gt;haben&lt;/li&gt;&lt;/ul&gt;</t>
@@ -859,7 +1003,7 @@
     <t>&lt;ul&gt;&lt;li&gt;Abschlussfreiheit (ob, wann und mit wem Vertrag geschlossen wird)&lt;/li&gt;&lt;li&gt;Inhaltsfreiheit&lt;/li&gt;&lt;li&gt;Typenfreiheit (neue Vertragstypen zu schaffen)&lt;/li&gt;&lt;li&gt;Beendigungsfreiheit&lt;/li&gt;&lt;li&gt;Änderungsfreiheit&lt;/li&gt;&lt;li&gt;Formfreiheit&lt;/li&gt;&lt;li&gt;Testierfreiheit (ob und wie der Verstorbene letztwillig testiert)&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist das Sekunddärrecht im Europäischen Recht?&lt;/p&gt;&lt;p&gt;Welche zwei Arten gibt es?&lt;/p&gt;&lt;p&gt;Worauf wirken sie?&lt;/p&gt;</t>
+    <t>&lt;p&gt;Was ist das Sekundärrecht im Europäischen Recht?&lt;/p&gt;&lt;p&gt;Welche zwei Arten gibt es?&lt;/p&gt;&lt;p&gt;Worauf wirken sie?&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;EU &lt;strong&gt;Verordnungen&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Sind sofort für die &lt;strong&gt;Mitgliedstaaten&lt;/strong&gt; und deren &lt;strong&gt;Bürger &lt;/strong&gt;gültig, es muss &lt;strong&gt;kein nationales Gesetz&lt;/strong&gt; erlassen werden.&lt;/li&gt;&lt;li&gt;EU &lt;strong&gt;Richtlinien&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Richten sich &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;idR&lt;/span&gt; an die Mitgliedstaaten, nicht die Bürger&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nationale Parlamente führen eine &lt;strong&gt;Transformation&lt;/strong&gt; in nationales Recht durch. Für die Bürger gilt das nationale Gesetz nicht die Richtlinie.&lt;/li&gt;&lt;/ul&gt;</t>
@@ -1033,7 +1177,7 @@
     <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/862" rel="noopener noreferrer" target="_blank"&gt;§ 862 ABGB&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;nach Ablauf der gesetzten oder gesetzlichen Pflicht&lt;/li&gt;&lt;li&gt;bei Ablehnung&lt;/li&gt;&lt;li&gt;Insolvenz des Antragstellers&lt;/li&gt;&lt;li&gt;Tod oder nachträgliche Geschäftsunfähigkeit des Antragstellers oder Erklärungsempfängers, wenn der Wille aus den Umständen hervorgeht&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist die Interpretation?&lt;/p&gt;</t>
+    <t>&lt;p&gt;Was ist die Interpretation einer Rechtsnorm?&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Interpretation ist die&lt;strong&gt; Ermittlung des maßgeblichen Sinns&lt;/strong&gt; einer Rechtsnorm. &lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Der Rechtsanwender versucht den Sinn einer Vorschrift „richtig“ zu verstehen.&lt;/p&gt;</t>
@@ -1636,7 +1780,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B206"/>
+  <dimension ref="A1:B230"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -3290,6 +3434,198 @@
         <v>411</v>
       </c>
     </row>
+    <row r="207" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A208" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A211" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A213" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A214" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A215" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A216" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A217" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A218" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A219" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A221" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A222" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A224" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A226" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Add cards for chapter 7, 8
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
+++ b/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="508">
   <si>
     <t>Question</t>
   </si>
@@ -19,6 +19,162 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;Was sind die 4 weiteren (neben den 4 Haupteinteilungen) Unterscheidungen von Sachen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Einfache&lt;/strong&gt; und &lt;strong&gt;zusammengsetzte &lt;/strong&gt;Sachen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Einzel&lt;/strong&gt; und &lt;strong&gt;Gesamtsachen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bzw. &lt;strong&gt;vertretbare &lt;/strong&gt;(Unterscheidung nur durch Zahl oder Gewicht, z.B.: Zucker) und &lt;strong&gt;unvertretbare &lt;/strong&gt;(Unterscheidung durch individuelle Merkmale: handgefertigte Maßkleidung, Tischlerei-Einrichtung) Sachen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Teilbare &lt;/strong&gt;und unteilbare Sachen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Herrenlose&lt;/strong&gt; und im &lt;strong&gt;Eigentum eines&lt;/strong&gt; &lt;strong&gt;Rechtssubjekt &lt;/strong&gt;stehende Sachen (&lt;strong&gt;privat &lt;/strong&gt;oder &lt;strong&gt;öffentlich&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die 4 Haupteinteilungen von Sachen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Körperliche &lt;/strong&gt;(Möbel, Wasser) und &lt;strong&gt;Unkörperliche &lt;/strong&gt;Sachen (Forderungen, Patentrechte)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Bewegliche&lt;/strong&gt; (Nahrungsmittel, geschnittenes Gras) und &lt;strong&gt;Unbewegliche &lt;/strong&gt;Sache (Grundstücke, nicht geerntete Früchte) &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verbrauchbare&lt;/strong&gt; (Energie) und &lt;strong&gt;Unverbrauchbare &lt;/strong&gt;Sachen (Bücher)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Schätzbare &lt;/strong&gt;(Geld, Buch) und &lt;strong&gt;Unschätzbare &lt;/strong&gt;Sachen ( Erinnerungsstücke, Zeugnisse, Urkunden)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Rechtsgrundlagen Regeln die &lt;strong&gt;Einteilung der Sachen&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/287" rel="noopener noreferrer" target="_blank"&gt;§§ 287-306 ABGB&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Zession?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Forderungsabtretung von Altgläubiger auf Neugläubiger&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie werden Forderungen übertragen?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Durch Zession (=Abtretung) ( &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/1392" rel="noopener noreferrer" target="_blank"&gt;§§ 1392 ff&lt;/a&gt; ) von Altgläubiger auf Neugläubiger übertragen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Intabulationsprinzip?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Bei einer &lt;strong&gt;Liegenschaft &lt;/strong&gt;(unbewegliche Sache) ist für den Erwerb des Eigentums die &lt;strong&gt;Eintragung in das Grundbuch &lt;/strong&gt;erforderlich.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Traditionsprinzip?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Eine &lt;strong&gt;bewegliche &lt;/strong&gt;Sache (z.B.: PKW) muss an den Erwerber &lt;strong&gt;übergeben &lt;/strong&gt;werden.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Sachen im Sinne eines Rechtsobjekts?&lt;/p&gt;&lt;p&gt;Sind auch Tiere Sachen?&lt;/p&gt;&lt;p&gt;Was sind die Rechtsgrundlagen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Alle &lt;strong&gt;körperlichen &lt;/strong&gt;und &lt;strong&gt;unkörperlichen Gegenstände&lt;/strong&gt; ( &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/285" rel="noopener noreferrer" target="_blank"&gt;§ 285 ABGB&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Tiere sind nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/285a" rel="noopener noreferrer" target="_blank"&gt;§ 285a ABGB &lt;/a&gt;keine Sachen, jedoch gelten in diesem Fall gemäß &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/285a" rel="noopener noreferrer" target="_blank"&gt;§ 285a S2 ABGB &lt;/a&gt;für Tiere die gleichen Vorschriften da es hier keine Abweichende Regelung gibt.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Rechtsobjekt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Alles was &lt;strong&gt;Gegenstand &lt;/strong&gt;eines &lt;strong&gt;Rechtes &lt;/strong&gt;oder einer &lt;strong&gt;Pflicht &lt;/strong&gt;eines &lt;strong&gt;Rechtssubjektes &lt;/strong&gt;sein kann.&lt;/li&gt;&lt;li&gt;Rechtsobjekte sind Sachen, nicht aber natürliche Personen.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist das &lt;/span&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(226, 148, 20);"&gt;Anmeldesystem &lt;/span&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(Gründung von juristischen Personen)? Wovon ist es Teil?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gilt für &lt;strong&gt;ideelle Vereine&lt;/strong&gt; (ohne Gewinnabsicht)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Vereinsbehörde &lt;/strong&gt;kann den Verein innerhalb von &lt;strong&gt;4 Wochen nach&lt;/strong&gt; Gründungsakt und &lt;strong&gt;Anmeldung untersagen&lt;/strong&gt;, läuft diese Frist ab entsteht der Verein.&lt;/li&gt;&lt;li&gt;Daher Teil des Normativsystems&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist das &lt;/span&gt;&lt;strong style="color: rgb(226, 148, 20); background-color: rgb(40, 45, 88);"&gt;Normativsystem &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(Gründung von juristischen Personen)?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Juristische Person entsteht erst durch einen &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(226, 148, 20);"&gt;staatlichen&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(226, 148, 20);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(226, 148, 20);"&gt;konstitutiven Gründungsakt&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;. Die Verleihung der Konzession &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;muss&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; stattfinden, wenn die gesetzlichen Voraussetzungen erfüllt sind.&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Entstehung mit &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;konstitutiver Eintragung &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;im &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Firmenbuch &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;abgeschlossen.&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;Was ist die Wissenszurechnung bei juristischen Personen?&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;Was sind die Rechtsgrundlagen? &lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Das Wissen der &lt;strong&gt;handelnden &lt;/strong&gt;Person wird an die &lt;strong&gt;vertretene juristische &lt;/strong&gt;Person zugerechnet.&lt;/p&gt;&lt;p&gt;Relevant für &lt;strong&gt;Irrtumsanfechtung &lt;/strong&gt;( § 871 ABGB ) und &lt;strong&gt;gutgläubigen Erwerb&lt;/strong&gt; von Sachen ( § 367 )&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wie funktioniert die Deliktsfähigkeit einer juristischen Person?&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wie funktioniert die Haftung?&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was sind die Rechtsgrundlagen? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Können naturgemäß &lt;strong&gt;selbst keine Delikte&lt;/strong&gt; begehen&lt;/li&gt;&lt;li&gt;Haftung für Verschulden von:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Organen &lt;/strong&gt;in Ausübung ihrer Funktion&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Machthabern&lt;/strong&gt; bzw. &lt;strong&gt;Repräsentanten &lt;/strong&gt;(&lt;strong&gt;Leitungs &lt;/strong&gt;oder &lt;strong&gt;Überwachungs&lt;/strong&gt;funktion) &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gem §§ &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/1313a" rel="noopener noreferrer" target="_blank"&gt;1313a&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/1315" rel="noopener noreferrer" target="_blank"&gt;1315 &lt;/a&gt;ABGB für Gehilfen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie funktioniert die Geschäftsfähigkeit einer juristischen Person?&lt;/p&gt;&lt;p&gt;Wer kann Geschäfte abschließen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;j. P. können nicht selbst nach außen auftreten, daher schließen (in der Satzung vorgesehene) &lt;strong&gt;Vertretungsorgane &lt;/strong&gt;die Geschäfte als Vertreter ab.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Vertretungsorgane &lt;/strong&gt;oder von ihnen mittels &lt;strong&gt;Vollmachtserteilung &lt;/strong&gt;berechtigte natürliche Personen (Prokurist, Handlungsbevollmächtigter, sonstige Vertreter)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sind juristische Personen Handlungsfähig?&lt;/p&gt;&lt;p&gt;Was ist in diesem Kontext das &lt;strong&gt;Trennungsprinzip&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Sie können &lt;strong&gt;nicht &lt;/strong&gt;unmittelbar &lt;strong&gt;selbst handeln&lt;/strong&gt;, sie brauchen dazu &lt;strong&gt;natürliche Personen&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;&lt;strong style="color: rgb(226, 148, 20); background-color: rgb(40, 45, 88);"&gt;Rechte&lt;/strong&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; &lt;/strong&gt;&lt;strong style="color: rgb(226, 148, 20); background-color: rgb(40, 45, 88);"&gt;und Pflichten&lt;/strong&gt;&lt;span style="color: rgb(226, 148, 20); background-color: rgb(40, 45, 88);"&gt; &lt;/span&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;der &lt;/span&gt;&lt;strong style="color: rgb(226, 148, 20); background-color: rgb(40, 45, 88);"&gt;juristischen&lt;/strong&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; &lt;/strong&gt;&lt;span style="color: rgb(226, 148, 20); background-color: rgb(40, 45, 88);"&gt;Personen &lt;/span&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;sind von denen der handelnden &lt;/span&gt;&lt;strong style="color: rgb(226, 148, 20); background-color: rgb(40, 45, 88);"&gt;natürlichen&lt;/strong&gt;&lt;span style="color: rgb(226, 148, 20); background-color: rgb(40, 45, 88);"&gt; Personen &lt;/span&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;streng zu &lt;/span&gt;&lt;strong style="color: rgb(226, 148, 20); background-color: rgb(40, 45, 88);"&gt;trennen&lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;.&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was besagt die Ultra-vires-Lehre in bezug auf juristische Personen?&lt;/p&gt;&lt;p&gt;Wird sie im Privatrecht anerkannt - Warum/Warum nicht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Rechtsfähigkeit nur gegeben, wenn die &lt;strong&gt;Statuten &lt;/strong&gt;der &lt;strong&gt;juristischen Person &lt;/strong&gt;diese Rechtsfähigkeit &lt;strong&gt;vorsehen&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;Wird im Privatrecht abgelehnt, weil die &lt;strong&gt;Geschäftspartner &lt;/strong&gt;diese Grenzen &lt;strong&gt;nicht leicht&lt;/strong&gt; &lt;strong&gt;erkennen &lt;/strong&gt;können, und dies die &lt;strong&gt;Verkehrssicherheit&lt;/strong&gt; &lt;strong&gt;belastet&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Rechtsfähigkeit haben juristische Personen?&lt;/p&gt;&lt;p&gt;Welche Grenzen gibt es?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Grundsätzlich die &lt;strong&gt;gleiche unbeschränkte Rechtsfähigkeit &lt;/strong&gt;wie &lt;strong&gt;natürliche Personen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Grenzen durch die &lt;strong&gt;Natur&lt;/strong&gt; &lt;strong&gt;der Sache &lt;/strong&gt;(z.B.: Keine &lt;strong&gt;Familien&lt;/strong&gt;- und &lt;strong&gt;Persönlichkeitsrechte&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist das &lt;/span&gt;&lt;strong&gt;System der freien Bildung&lt;/strong&gt; juristischer Personen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Juristische Person entsteht &lt;strong&gt;ausschließlich &lt;/strong&gt;durch &lt;strong&gt;privatrechtlichen Gründungsakt&lt;/strong&gt;, zum Zeitpunkt der Vornahme des Akts (Abschluss des Gesellschaftsvertrags)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das &lt;strong&gt;Konzessionssystem &lt;/strong&gt;(Gründung von juristischen Personen)?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Juristische Person entsteht erst durch einen &lt;strong&gt;staatlichen konstitutiven Gründungsakt&lt;/strong&gt;. Es liegt im &lt;strong&gt;Ermessen der Behörde&lt;/strong&gt;, die &lt;strong&gt;Konzession&lt;/strong&gt; zu verleihen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie werden juristische Personen des Privatrechts gegründet?&lt;/p&gt;&lt;p&gt;Welche 3 Gründungsysteme gibt es?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Durch Kombination von:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;privatrechtlichen&lt;/strong&gt; &lt;strong&gt;Gründungsakt &lt;/strong&gt;(Gesellschaftsvertrag) &lt;/li&gt;&lt;li&gt;öffentlich-rechtlichen Akt der &lt;strong&gt;Anerkennung durch die Rechtsordnung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Gründungssysteme:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Konzessionssystem&lt;/li&gt;&lt;li&gt;Normativsystem&lt;/li&gt;&lt;li&gt;System der freien Bildung juristischer Personen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie werden juristische Personen des öffentlichen Rechts gegründet?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Durch &lt;strong&gt;staatlichen Gründungsakt &lt;/strong&gt;(eigene Sondergesetze)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind teilrechtsfähige Geblide?&lt;/p&gt;&lt;p&gt;Beispiele?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ihnen werden Kraft Gesetzes nur &lt;strong&gt;einzelne Rechte &lt;/strong&gt;und &lt;strong&gt;Pflichten&lt;/strong&gt; zugewiesen.&lt;/li&gt;&lt;li&gt;Beispiele: Bundesschulen, Geologische Bundesanstalt&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche vollrechtsfähigen Juristischen Personen gibt es?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;z.B.: &lt;strong&gt;Kapitalgesellschaften&lt;/strong&gt; (AG, KG, OG, GmbH) sowie &lt;strong&gt;Vereine&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind juristische Personen?&lt;/p&gt;&lt;p&gt;Was ist die Entscheidende Abgrenzung von moralischen Personen?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Rechtsfähige Personenvereinigungen &lt;/strong&gt;und &lt;strong&gt;Vermögensmassen &lt;/strong&gt;die Voll- oder Teilrechtsfähigkeit haben können.&lt;/li&gt;&lt;li&gt;Abgrenzung: Die Interessen der Gesellschaft stehen deutlich vor den Interessen der einzelnen Mitglieder&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/26" rel="noopener noreferrer" target="_blank"&gt;§ 26 ABGB&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Moralische Personen?&lt;/p&gt;&lt;p&gt;Was sind Beispiele?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gemeinschaften die &lt;strong&gt;nicht&lt;/strong&gt; &lt;strong&gt;selbst rechtsfähig &lt;/strong&gt;sind sondern, &lt;strong&gt;sondern &lt;/strong&gt;die in der Gemeinschaft verbundenen &lt;strong&gt;Personen&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;Beispiele:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Miteigentümergemeinschaft (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/825" rel="noopener noreferrer" target="_blank"&gt;§§ 825ff ABGB&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erbengemeinschaft (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/550" rel="noopener noreferrer" target="_blank"&gt;§ 550 ABGB&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gesellschaft bürgerlichen Rechts (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/1175" rel="noopener noreferrer" target="_blank"&gt;§§ 1175 ff ABGB&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die natürlichen Rechtsgrundsätze?&lt;/p&gt;&lt;p&gt;Wann werden sie angewendet?&lt;/p&gt;&lt;p&gt;Kommen sie häufig zum Einsatz?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Der Rückgriff auf die &lt;strong&gt;allgemeinen Wertprinzipien&lt;/strong&gt; die der gesamten Rechtsordnung zugrunde liegen.&lt;/li&gt;&lt;li&gt;Nach &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/7" rel="noopener noreferrer" target="_blank"&gt;§ 7 ABGB&lt;/a&gt; werden sie angewendet, wenn &lt;strong&gt;weder Gesetzes- noch Rechtsanalogie&lt;/strong&gt; zu einer &lt;strong&gt;Lösung &lt;/strong&gt;des Sachverhalts führen&lt;/li&gt;&lt;li&gt;Stellen die&lt;strong&gt; ultima ratio&lt;/strong&gt; (letztmöglicher Weg) dar, daher selten Angewendet.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Was ist die Testierfähigkeit?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
   </si>
   <si>
@@ -34,7 +190,7 @@
     <t>&lt;p&gt;Wird die Handlungsfähigkeit einer vertretenen Person eingeschränkt?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;gem &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/242" rel="noopener noreferrer" target="_blank"&gt;§ 242 AGBG&lt;/a&gt; nicht eingeschränkt&lt;/p&gt;</t>
+    <t>&lt;p&gt;gem &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/242" rel="noopener noreferrer" target="_blank"&gt;§ 242 AGBG&lt;/a&gt; &lt;strong&gt;nicht &lt;/strong&gt;eingeschränkt&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Rechtsgrundlage für die gerichtliche Erwachsenenvertretung?&lt;/span&gt;&lt;/p&gt;</t>
@@ -151,12 +307,6 @@
     <t>&lt;ul&gt;&lt;li&gt;Fähigkeit Träger von Rechten und Pflichten zu sein&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/16" rel="noopener noreferrer" target="_blank"&gt;§ 16 ABGB&lt;/a&gt;: Lebenslänglich&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was sind Rechtsobjekte?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Gegenstand der Rechte (eines Rechtssubjekts) bzw des Rechtsverkehrs&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was sind Rechtssubjekte?&lt;/p&gt;&lt;p&gt;Welche Arten gibt es?&lt;/p&gt;</t>
   </si>
   <si>
@@ -1067,12 +1217,6 @@
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Einschränkung &lt;/strong&gt;des Anwendungsbereichs einer &lt;strong&gt;überschießend formulierten&lt;/strong&gt; &lt;strong&gt;Norm&lt;/strong&gt;. &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Rechtsfolge &lt;/strong&gt;wird für jene Sachverhalte &lt;strong&gt;ausgeschlossen&lt;/strong&gt;, die vom &lt;strong&gt;Sinn &lt;/strong&gt;und &lt;strong&gt;Zweck &lt;/strong&gt;der Norm &lt;strong&gt;nicht&lt;/strong&gt; &lt;strong&gt;erfasst &lt;/strong&gt;sein sollen.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die natürlichen Rechtsgrundsätze?&lt;/p&gt;&lt;p&gt;Wann werden sie angewendet?&lt;/p&gt;&lt;p&gt;Kommen sie häufig zum Einsatz?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrunldage? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Der Rückgriff auf die &lt;strong&gt;allgemeinen Wertprinzipien&lt;/strong&gt; die der gesamten Rechtsordnung zugrunde liegen.&lt;/li&gt;&lt;li&gt;Nach § 7 ABGB werden sie angewendet, wenn &lt;strong&gt;weder Gesetzes- noch Rechtsanalogie&lt;/strong&gt; zu einer &lt;strong&gt;Lösung &lt;/strong&gt;des Sachverhalts führen&lt;/li&gt;&lt;li&gt;Stellen die&lt;strong&gt; ultima ratio&lt;/strong&gt; (letztmöglicher Weg) dar, daher selten Angewendet.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Wann wird die teleologische Interpretation eingesetzt?&lt;/p&gt;</t>
@@ -1780,7 +1924,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B230"/>
+  <dimension ref="A1:B254"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -3626,6 +3770,198 @@
         <v>459</v>
       </c>
     </row>
+    <row r="231" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A249" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A254" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Add cards for chapter 9
Now 1-15 are done
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
+++ b/flashcards/Memcode - KS Privatrecht I Test 1 (JKU, Austria).xlsx
@@ -11,12 +11,114 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="542">
   <si>
     <t>Question</t>
   </si>
   <si>
     <t>Answer</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Woraus leiten sich Ansprüche einer vertraglichen Vereinbarung ab? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;unmittelbar &lt;/strong&gt;aus dem &lt;strong&gt;objektiven Recht&lt;/strong&gt;: z.B.: Recht des Käufers auf die Kaufsache&lt;/li&gt;&lt;li&gt;&lt;strong&gt;mittelbar &lt;/strong&gt;aus dem&lt;strong&gt; objektiven Recht abgeleitet&lt;/strong&gt;: Es gibt &lt;strong&gt;keine unmittelbare gesetzliche Grundlage&lt;/strong&gt;, aber das &lt;strong&gt;Prinzip der Vertragsfreiheit&lt;/strong&gt; aus dem Schuldrecht regelt die Vereinbarung.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die 3 wesentliche Entstehungsgründe für einen Anspruch? &lt;/p&gt;&lt;p&gt;Was sind die Rechtsgrundlagen und jeweiligen Voraussetzungen? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;strong&gt;das Gesetz&lt;/strong&gt;: Anspruch unmittelbar durch die Rechtsordnung eingeräumt (z.B.: Persönlichkeitsrechte von Geburt an)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;die erlittene&lt;/strong&gt; &lt;strong&gt;Beschädigung&lt;/strong&gt;: Bei Körperverletzung erwirbt der Geschädigte gem §§ 1325ff ABGB einen Anspruch auf Schadenersatz. Benötigt rechtswidriges schuldhaftes Verhalten einer anderen Person&lt;/li&gt;&lt;li&gt;&lt;strong&gt;das&lt;/strong&gt; &lt;strong&gt;Rechtsgeschäft &lt;/strong&gt;(Vertrag): Vertrag und daraus resultierende Rechte und Pflichten&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind dingliche Berechtigungen?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Legaldefinition siehe &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/424" rel="noopener noreferrer" target="_blank"&gt;§ 424 ABGB&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Obligatorische Berechtigungen?&lt;/p&gt;&lt;p&gt;Was ist die Rechtsgrundlage? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Legaldefinition siehe &lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/859" rel="noopener noreferrer" target="_blank"&gt;§ 859 ABGB&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Abgrenzung zwischen Anspruch und Herrschaftsrecht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ein &lt;strong&gt;Herrschaftsrecht&lt;/strong&gt; bezieht sich auf ein &lt;strong&gt;Rechtsobjekt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Ein &lt;strong&gt;Anspruch&lt;/strong&gt; bezieht sich auf ein &lt;strong&gt;Rechtssubjekt &lt;/strong&gt;(das zu einer Leistung verpflichtet ist)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Der &lt;strong&gt;Anspruch &lt;/strong&gt;gibt also nur ein "&lt;strong&gt;Recht&lt;/strong&gt;" auf die zu &lt;strong&gt;leistende Sache&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Arten der Klagen gibt es um Ansprüche durchzustezen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Leistungsklage&lt;/strong&gt;: auf Positives Tun gerichtet&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Unterlassungsklage&lt;/strong&gt;: auf passives Unterlassen gerichtet&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Feststellungsklage&lt;/strong&gt;: Bestehen oder Nichtbestehen eines Rechts wird festgestellt&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie kann ein Anspruch durchgesetzt werden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Durch &lt;strong&gt;Klage&lt;/strong&gt; oder &lt;strong&gt;Exekution &lt;/strong&gt;(Zwangsvollstreckung)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Gestaltungsrechte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Verleihen dem Berechtigten die &lt;strong&gt;Macht &lt;/strong&gt;durch &lt;strong&gt;einseitige&lt;/strong&gt; &lt;strong&gt;Erklärung &lt;/strong&gt;(ohne Mitwirken anderer) eine &lt;strong&gt;Veränderung der Rechtsverhältnisse&lt;/strong&gt; herbeizühren.&lt;/li&gt;&lt;li&gt;z.B.: Kündigung von Miet- oder Dienstvertrag&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Herrschaftsrechte?&lt;/p&gt;&lt;p&gt;Welche Rechte sind den Herrschaftsrechten zugeordnet?&lt;/p&gt;&lt;p&gt;Zu welcher Kategorie der Rechte gehören die Herrschaftsrechte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Erlauben es, auf bestimmte &lt;strong&gt;Rechtsobjekte unmittelbar einzuwirken &lt;/strong&gt;und fremde Einflüsse auszuschließen.&lt;/li&gt;&lt;li&gt;alle &lt;strong&gt;dinglichen Rechte &lt;/strong&gt;und &lt;strong&gt;Immaterialgüterrechte &lt;/strong&gt;sind Herrschaftsrechte&lt;/li&gt;&lt;li&gt;Herrschaftsrechte sind &lt;strong&gt;absolute &lt;/strong&gt;Rechte&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Immaterialgüterrechte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vermögensrechte &lt;/strong&gt;an geistigen Produkten&lt;/li&gt;&lt;li&gt;z.B.: Markenrechte, Patentrechte&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Familienrechte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Sind wie obligatorische Rechte auf das &lt;strong&gt;Verhalten bestimmter Personen&lt;/strong&gt; &lt;strong&gt;bezogen&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;z.B.: Recht des Kindes auf Pflege und erziehung&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind obligatorische Rechte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kein &lt;/strong&gt;unmittelbarer &lt;strong&gt;Sachbezug&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Forderungsrechte &lt;/strong&gt;die auf das &lt;strong&gt;Verhalten bestimmter &lt;/strong&gt;anderer &lt;strong&gt;Rechtssubjekte &lt;/strong&gt;bezogen sind.&lt;/li&gt;&lt;li&gt;z.B.: Recht des Arbeitgebers auf erbringung der Arbeitsleistung durch Arbeitnehmer&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind dingliche Rechte?&lt;/p&gt;&lt;p&gt;Wie werden sie noch genannt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Subjektive &lt;/strong&gt;Rechte, die sich &lt;strong&gt;unmittelbar &lt;/strong&gt;auf &lt;strong&gt;körperliche Sachen &lt;/strong&gt;beziehen, und dem Rechtssubjekt ein &lt;strong&gt;Herrschaftsrecht &lt;/strong&gt;an der Sache verleihen. &lt;/li&gt;&lt;li&gt;z.B.: Eigentumsrecht, Baurecht&lt;/li&gt;&lt;li&gt;Sachenrecht&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind relative Rechte?&lt;/p&gt;&lt;p&gt;Wodurch entstehen sie?&lt;/p&gt;&lt;p&gt;Wie wirken sie? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Wirken nur gegenüber &lt;strong&gt;bestimmten Personen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Meist durch schuldrechtliche Vereinbarungen (z.B.: Vertrag), aber auch ex lege (Schadenersatzansprüche)&lt;/li&gt;&lt;li&gt;Wirken nur zwischen an der Vereinbarung beteiligten (&lt;strong&gt;inter partes&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind absolute Rechte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wirken gegenüber &lt;strong&gt;jedermann &lt;/strong&gt;(z.B.: Stellung des Eigentümers)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist subjektives Recht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Das subjektive Recht ist eine &lt;strong&gt;Rechtsmacht&lt;/strong&gt;, die dem &lt;strong&gt;einzelnen Rechtssubjekt &lt;/strong&gt;zur &lt;strong&gt;Befriedigung seiner Interessen &lt;/strong&gt;von der Rechtsordnung (dem objektiven Recht) verliehen ist und deren &lt;strong&gt;Geltendmachung &lt;/strong&gt;allein vom &lt;strong&gt;Willen&lt;/strong&gt; &lt;strong&gt;des Berechtigten&lt;/strong&gt; abhängt&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist objektives Recht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Gesamtheit aller Normen, die das menschliche Zusammenleben regeln&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was sind die 4 weiteren (neben den 4 Haupteinteilungen) Unterscheidungen von Sachen?&lt;/p&gt;</t>
@@ -1924,7 +2026,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B254"/>
+  <dimension ref="A1:B271"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -3962,6 +4064,142 @@
         <v>507</v>
       </c>
     </row>
+    <row r="255" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A255" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A256" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A258" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A259" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A261" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A262" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="B262" s="2" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A263" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="B263" s="2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A264" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="B264" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="B265" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A266" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="B266" s="2" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A267" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="B267" s="2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A268" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="B268" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A269" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="B269" s="2" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A270" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A271" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>541</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>